<commit_message>
2da Entrega - 05-12-2022
</commit_message>
<xml_diff>
--- a/helps/Historial de Jugadas.xlsx
+++ b/helps/Historial de Jugadas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edinson.Quevedo\Mi unidad (quevedo.edinson@gmail.com)\Proyectos\Randon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Practicando\Java\Randon\JugadaGanadora\helps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72B55A9-FDCB-4210-A1EA-CF115834DE05}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC4690C-E99E-464B-A844-7A4E8110C8EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{A3392D85-3030-46DE-B96E-7922EDC7109E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A3392D85-3030-46DE-B96E-7922EDC7109E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tinka" sheetId="2" r:id="rId1"/>
@@ -20,6 +20,15 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -75,7 +84,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -245,7 +254,7 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -562,26 +571,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE65A1AE-D24F-426E-B6EF-7BC880E7680E}">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B1" s="16">
         <v>44626</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
         <v>9</v>
       </c>
@@ -589,7 +598,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="9" t="s">
         <v>10</v>
       </c>
@@ -597,17 +606,17 @@
         <v>929</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C5" s="17">
         <f>SUM(C3:C4)</f>
         <v>2359</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="6"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="14"/>
       <c r="C7" s="12" t="s">
         <v>1</v>
@@ -626,7 +635,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="15"/>
       <c r="C8" s="18"/>
       <c r="D8" s="11"/>
@@ -635,7 +644,7 @@
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
     </row>
-    <row r="9" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="15"/>
       <c r="C9" s="18"/>
       <c r="D9" s="11"/>
@@ -644,7 +653,7 @@
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
     </row>
-    <row r="10" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="15"/>
       <c r="C10" s="18"/>
       <c r="D10" s="11"/>
@@ -653,7 +662,7 @@
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
     </row>
-    <row r="11" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="15"/>
       <c r="C11" s="18"/>
       <c r="D11" s="11"/>
@@ -662,7 +671,7 @@
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
     </row>
-    <row r="12" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="15"/>
       <c r="C12" s="18"/>
       <c r="D12" s="11"/>
@@ -671,7 +680,7 @@
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
     </row>
-    <row r="13" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="15"/>
       <c r="C13" s="18"/>
       <c r="D13" s="11"/>
@@ -680,7 +689,7 @@
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
     </row>
-    <row r="14" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="15"/>
       <c r="C14" s="18"/>
       <c r="D14" s="11"/>
@@ -689,7 +698,7 @@
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
     </row>
-    <row r="15" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="15"/>
       <c r="C15" s="18"/>
       <c r="D15" s="11"/>
@@ -698,7 +707,7 @@
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
     </row>
-    <row r="16" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="15"/>
       <c r="C16" s="18"/>
       <c r="D16" s="11"/>
@@ -707,7 +716,7 @@
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
     </row>
-    <row r="17" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="15"/>
       <c r="C17" s="18"/>
       <c r="D17" s="11"/>
@@ -716,48 +725,64 @@
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
     </row>
-    <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="15"/>
-      <c r="C18" s="18"/>
+    <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="15">
+        <v>2380</v>
+      </c>
+      <c r="C18" s="18">
+        <v>44699</v>
+      </c>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
       <c r="H18" s="11"/>
     </row>
-    <row r="19" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="15"/>
-      <c r="C19" s="18"/>
+    <row r="19" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="15">
+        <v>2379</v>
+      </c>
+      <c r="C19" s="18">
+        <v>44696</v>
+      </c>
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
     </row>
-    <row r="20" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="15"/>
-      <c r="C20" s="18"/>
+    <row r="20" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="15">
+        <v>2378</v>
+      </c>
+      <c r="C20" s="18">
+        <v>44692</v>
+      </c>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
     </row>
-    <row r="21" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="15"/>
-      <c r="C21" s="18"/>
+    <row r="21" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="15">
+        <v>2377</v>
+      </c>
+      <c r="C21" s="18">
+        <v>44689</v>
+      </c>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
     </row>
-    <row r="22" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="15">
-        <v>2380</v>
+        <v>2376</v>
       </c>
       <c r="C22" s="18">
-        <v>44699</v>
+        <v>44685</v>
       </c>
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
@@ -765,12 +790,12 @@
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
     </row>
-    <row r="23" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="15">
-        <v>2379</v>
+        <v>2375</v>
       </c>
       <c r="C23" s="18">
-        <v>44696</v>
+        <v>44682</v>
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="11"/>
@@ -778,12 +803,12 @@
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
     </row>
-    <row r="24" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="15">
-        <v>2378</v>
+        <v>2374</v>
       </c>
       <c r="C24" s="18">
-        <v>44692</v>
+        <v>44678</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
@@ -791,12 +816,12 @@
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
     </row>
-    <row r="25" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="15">
-        <v>2377</v>
+        <v>2373</v>
       </c>
       <c r="C25" s="18">
-        <v>44689</v>
+        <v>44675</v>
       </c>
       <c r="D25" s="11"/>
       <c r="E25" s="11"/>
@@ -804,12 +829,12 @@
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
     </row>
-    <row r="26" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="15">
-        <v>2376</v>
+        <v>2372</v>
       </c>
       <c r="C26" s="18">
-        <v>44685</v>
+        <v>44671</v>
       </c>
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
@@ -817,12 +842,12 @@
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
     </row>
-    <row r="27" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="15">
-        <v>2375</v>
+        <v>2371</v>
       </c>
       <c r="C27" s="18">
-        <v>44682</v>
+        <v>44668</v>
       </c>
       <c r="D27" s="11"/>
       <c r="E27" s="11"/>
@@ -830,12 +855,12 @@
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
     </row>
-    <row r="28" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="15">
-        <v>2374</v>
+        <v>2370</v>
       </c>
       <c r="C28" s="18">
-        <v>44678</v>
+        <v>44664</v>
       </c>
       <c r="D28" s="11"/>
       <c r="E28" s="11"/>
@@ -843,12 +868,12 @@
       <c r="G28" s="11"/>
       <c r="H28" s="11"/>
     </row>
-    <row r="29" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="15">
-        <v>2373</v>
+        <v>2369</v>
       </c>
       <c r="C29" s="18">
-        <v>44675</v>
+        <v>44661</v>
       </c>
       <c r="D29" s="11"/>
       <c r="E29" s="11"/>
@@ -856,12 +881,12 @@
       <c r="G29" s="11"/>
       <c r="H29" s="11"/>
     </row>
-    <row r="30" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="15">
-        <v>2372</v>
+        <v>2368</v>
       </c>
       <c r="C30" s="18">
-        <v>44671</v>
+        <v>44657</v>
       </c>
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
@@ -869,12 +894,12 @@
       <c r="G30" s="11"/>
       <c r="H30" s="11"/>
     </row>
-    <row r="31" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="15">
-        <v>2371</v>
+        <v>2367</v>
       </c>
       <c r="C31" s="18">
-        <v>44668</v>
+        <v>44654</v>
       </c>
       <c r="D31" s="11"/>
       <c r="E31" s="11"/>
@@ -882,12 +907,12 @@
       <c r="G31" s="11"/>
       <c r="H31" s="11"/>
     </row>
-    <row r="32" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="15">
-        <v>2370</v>
+        <v>2366</v>
       </c>
       <c r="C32" s="18">
-        <v>44664</v>
+        <v>44650</v>
       </c>
       <c r="D32" s="11"/>
       <c r="E32" s="11"/>
@@ -895,12 +920,12 @@
       <c r="G32" s="11"/>
       <c r="H32" s="11"/>
     </row>
-    <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B33" s="15">
-        <v>2369</v>
+        <v>2365</v>
       </c>
       <c r="C33" s="18">
-        <v>44661</v>
+        <v>44647</v>
       </c>
       <c r="D33" s="11"/>
       <c r="E33" s="11"/>
@@ -908,12 +933,12 @@
       <c r="G33" s="11"/>
       <c r="H33" s="11"/>
     </row>
-    <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="15">
-        <v>2368</v>
+        <v>2364</v>
       </c>
       <c r="C34" s="18">
-        <v>44657</v>
+        <v>44643</v>
       </c>
       <c r="D34" s="11"/>
       <c r="E34" s="11"/>
@@ -921,12 +946,12 @@
       <c r="G34" s="11"/>
       <c r="H34" s="11"/>
     </row>
-    <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B35" s="15">
-        <v>2367</v>
+        <v>2363</v>
       </c>
       <c r="C35" s="18">
-        <v>44654</v>
+        <v>44640</v>
       </c>
       <c r="D35" s="11"/>
       <c r="E35" s="11"/>
@@ -934,12 +959,12 @@
       <c r="G35" s="11"/>
       <c r="H35" s="11"/>
     </row>
-    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B36" s="15">
-        <v>2366</v>
+        <v>2362</v>
       </c>
       <c r="C36" s="18">
-        <v>44650</v>
+        <v>44636</v>
       </c>
       <c r="D36" s="11"/>
       <c r="E36" s="11"/>
@@ -947,12 +972,12 @@
       <c r="G36" s="11"/>
       <c r="H36" s="11"/>
     </row>
-    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B37" s="15">
-        <v>2365</v>
+        <v>2361</v>
       </c>
       <c r="C37" s="18">
-        <v>44647</v>
+        <v>44633</v>
       </c>
       <c r="D37" s="11"/>
       <c r="E37" s="11"/>
@@ -960,12 +985,12 @@
       <c r="G37" s="11"/>
       <c r="H37" s="11"/>
     </row>
-    <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B38" s="15">
-        <v>2364</v>
+        <v>2360</v>
       </c>
       <c r="C38" s="18">
-        <v>44643</v>
+        <v>44629</v>
       </c>
       <c r="D38" s="11"/>
       <c r="E38" s="11"/>
@@ -973,12 +998,12 @@
       <c r="G38" s="11"/>
       <c r="H38" s="11"/>
     </row>
-    <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B39" s="15">
-        <v>2363</v>
+        <v>2359</v>
       </c>
       <c r="C39" s="18">
-        <v>44640</v>
+        <v>44626</v>
       </c>
       <c r="D39" s="11"/>
       <c r="E39" s="11"/>
@@ -986,91 +1011,39 @@
       <c r="G39" s="11"/>
       <c r="H39" s="11"/>
     </row>
-    <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="15">
-        <v>2362</v>
+    <row r="40" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>12</v>
       </c>
       <c r="C40" s="18">
-        <v>44636</v>
+        <v>34623</v>
       </c>
       <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
+      <c r="E40" s="11" t="s">
+        <v>7</v>
+      </c>
       <c r="F40" s="11"/>
       <c r="G40" s="11"/>
       <c r="H40" s="11"/>
     </row>
-    <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="15">
-        <v>2361</v>
+    <row r="41" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>12</v>
       </c>
       <c r="C41" s="18">
-        <v>44633</v>
+        <v>38126</v>
       </c>
       <c r="D41" s="11"/>
       <c r="E41" s="11"/>
       <c r="F41" s="11"/>
       <c r="G41" s="11"/>
       <c r="H41" s="11"/>
-    </row>
-    <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="15">
-        <v>2360</v>
-      </c>
-      <c r="C42" s="18">
-        <v>44629</v>
-      </c>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
-    </row>
-    <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="15">
-        <v>2359</v>
-      </c>
-      <c r="C43" s="18">
-        <v>44626</v>
-      </c>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
-    </row>
-    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>11</v>
-      </c>
-      <c r="B44" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C44" s="18">
-        <v>34623</v>
-      </c>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-    </row>
-    <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>10</v>
-      </c>
-      <c r="B45" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C45" s="18">
-        <v>38126</v>
-      </c>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1086,17 +1059,17 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.109375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.140625" style="9"/>
+    <col min="2" max="2" width="15.109375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16">
         <v>41769</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16">
         <v>44593</v>
       </c>
@@ -1107,11 +1080,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="6"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="7"/>
       <c r="C4" s="2" t="s">
         <v>1</v>
@@ -1132,7 +1105,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="8"/>
       <c r="C5" s="10"/>
       <c r="D5" s="5"/>
@@ -1141,7 +1114,7 @@
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="8"/>
       <c r="C6" s="10"/>
       <c r="D6" s="5"/>
@@ -1150,7 +1123,7 @@
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="8"/>
       <c r="C7" s="10"/>
       <c r="D7" s="5"/>
@@ -1159,7 +1132,7 @@
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="8"/>
       <c r="C8" s="10"/>
       <c r="D8" s="5"/>
@@ -1168,7 +1141,7 @@
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="8">
         <v>1256</v>
       </c>
@@ -1181,7 +1154,7 @@
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="8">
         <v>1255</v>
       </c>
@@ -1194,7 +1167,7 @@
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="8">
         <v>1254</v>
       </c>
@@ -1207,7 +1180,7 @@
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="8">
         <v>1253</v>
       </c>
@@ -1220,7 +1193,7 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="8">
         <v>1252</v>
       </c>
@@ -1233,7 +1206,7 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="8">
         <v>1251</v>
       </c>
@@ -1246,7 +1219,7 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="8">
         <v>1250</v>
       </c>
@@ -1259,7 +1232,7 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="8">
         <v>1249</v>
       </c>
@@ -1272,7 +1245,7 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="8">
         <v>1248</v>
       </c>
@@ -1285,7 +1258,7 @@
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="8">
         <v>1247</v>
       </c>
@@ -1298,7 +1271,7 @@
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="8">
         <v>1246</v>
       </c>
@@ -1311,7 +1284,7 @@
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="8">
         <v>1245</v>
       </c>
@@ -1324,7 +1297,7 @@
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="8">
         <v>1244</v>
       </c>
@@ -1337,7 +1310,7 @@
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="8">
         <v>1243</v>
       </c>
@@ -1350,7 +1323,7 @@
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="8">
         <v>1242</v>
       </c>
@@ -1363,7 +1336,7 @@
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="8">
         <v>1241</v>
       </c>
@@ -1376,7 +1349,7 @@
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="8">
         <v>1240</v>
       </c>
@@ -1389,7 +1362,7 @@
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="8">
         <v>1239</v>
       </c>
@@ -1402,7 +1375,7 @@
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="8">
         <v>1238</v>
       </c>
@@ -1415,7 +1388,7 @@
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="8">
         <v>1237</v>
       </c>
@@ -1428,7 +1401,7 @@
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="8">
         <v>1236</v>
       </c>
@@ -1441,7 +1414,7 @@
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
     </row>
-    <row r="30" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="8">
         <v>1235</v>
       </c>
@@ -1454,7 +1427,7 @@
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
     </row>
-    <row r="31" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="8">
         <v>1234</v>
       </c>
@@ -1467,7 +1440,7 @@
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
     </row>
-    <row r="32" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="8">
         <v>1233</v>
       </c>
@@ -1480,7 +1453,7 @@
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
     </row>
-    <row r="33" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B33" s="8">
         <v>1232</v>
       </c>
@@ -1493,7 +1466,7 @@
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
     </row>
-    <row r="34" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="8">
         <v>1231</v>
       </c>
@@ -1506,7 +1479,7 @@
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
     </row>
-    <row r="35" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B35" s="8">
         <v>1230</v>
       </c>
@@ -1519,7 +1492,7 @@
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
     </row>
-    <row r="36" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B36" s="8">
         <v>1229</v>
       </c>
@@ -1532,7 +1505,7 @@
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
     </row>
-    <row r="37" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B37" s="8">
         <v>1228</v>
       </c>
@@ -1545,7 +1518,7 @@
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
     </row>
-    <row r="38" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B38" s="8">
         <v>1227</v>
       </c>
@@ -1558,7 +1531,7 @@
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
     </row>
-    <row r="39" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B39" s="8">
         <v>1226</v>
       </c>
@@ -1571,7 +1544,7 @@
       <c r="G39" s="5"/>
       <c r="H39" s="5"/>
     </row>
-    <row r="40" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B40" s="8">
         <v>1225</v>
       </c>
@@ -1584,7 +1557,7 @@
       <c r="G40" s="5"/>
       <c r="H40" s="5"/>
     </row>
-    <row r="41" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B41" s="8">
         <v>1224</v>
       </c>
@@ -1597,7 +1570,7 @@
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
     </row>
-    <row r="42" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B42" s="8">
         <v>1223</v>
       </c>
@@ -1610,7 +1583,7 @@
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
     </row>
-    <row r="43" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B43" s="8">
         <v>1222</v>
       </c>
@@ -1623,7 +1596,7 @@
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
     </row>
-    <row r="44" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B44" s="8">
         <v>1221</v>
       </c>
@@ -1636,7 +1609,7 @@
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
     </row>
-    <row r="45" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B45" s="8">
         <v>1220</v>
       </c>
@@ -1649,7 +1622,7 @@
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
     </row>
-    <row r="46" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B46" s="8">
         <v>1219</v>
       </c>
@@ -1662,7 +1635,7 @@
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
     </row>
-    <row r="47" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B47" s="8">
         <v>1218</v>
       </c>
@@ -1675,7 +1648,7 @@
       <c r="G47" s="5"/>
       <c r="H47" s="5"/>
     </row>
-    <row r="48" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B48" s="8">
         <v>1217</v>
       </c>
@@ -1688,7 +1661,7 @@
       <c r="G48" s="5"/>
       <c r="H48" s="5"/>
     </row>
-    <row r="49" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B49" s="8">
         <v>1216</v>
       </c>
@@ -1701,7 +1674,7 @@
       <c r="G49" s="5"/>
       <c r="H49" s="5"/>
     </row>
-    <row r="50" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B50" s="8">
         <v>1215</v>
       </c>
@@ -1714,7 +1687,7 @@
       <c r="G50" s="5"/>
       <c r="H50" s="5"/>
     </row>
-    <row r="51" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B51" s="8">
         <v>1214</v>
       </c>
@@ -1727,7 +1700,7 @@
       <c r="G51" s="5"/>
       <c r="H51" s="5"/>
     </row>
-    <row r="52" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B52" s="8">
         <v>1213</v>
       </c>
@@ -1740,7 +1713,7 @@
       <c r="G52" s="5"/>
       <c r="H52" s="5"/>
     </row>
-    <row r="53" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B53" s="8">
         <v>1212</v>
       </c>
@@ -1753,7 +1726,7 @@
       <c r="G53" s="5"/>
       <c r="H53" s="5"/>
     </row>
-    <row r="54" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B54" s="8">
         <v>1211</v>
       </c>

</xml_diff>

<commit_message>
Actualziación Historial de Jugadas
</commit_message>
<xml_diff>
--- a/helps/Historial de Jugadas.xlsx
+++ b/helps/Historial de Jugadas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20393"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Randon\helps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69380E0F-84EE-4D0D-9B7C-672BAB47A834}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B53345-9A24-44E1-B824-57F08EF3C563}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1" xr2:uid="{A3392D85-3030-46DE-B96E-7922EDC7109E}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{A3392D85-3030-46DE-B96E-7922EDC7109E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tinka" sheetId="2" r:id="rId1"/>
@@ -74,7 +74,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,6 +116,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -195,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -231,6 +237,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -547,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE65A1AE-D24F-426E-B6EF-7BC880E7680E}">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,6 +568,7 @@
     <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" customWidth="1"/>
     <col min="8" max="8" width="19.28515625" customWidth="1"/>
+    <col min="9" max="9" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
@@ -702,12 +712,8 @@
       <c r="H17" s="7"/>
     </row>
     <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="11">
-        <v>2380</v>
-      </c>
-      <c r="C18" s="14">
-        <v>44699</v>
-      </c>
+      <c r="B18" s="11"/>
+      <c r="C18" s="14"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -715,12 +721,8 @@
       <c r="H18" s="7"/>
     </row>
     <row r="19" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="11">
-        <v>2379</v>
-      </c>
-      <c r="C19" s="14">
-        <v>44696</v>
-      </c>
+      <c r="B19" s="11"/>
+      <c r="C19" s="14"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -728,12 +730,8 @@
       <c r="H19" s="7"/>
     </row>
     <row r="20" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="11">
-        <v>2378</v>
-      </c>
-      <c r="C20" s="14">
-        <v>44692</v>
-      </c>
+      <c r="B20" s="11"/>
+      <c r="C20" s="14"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -741,12 +739,8 @@
       <c r="H20" s="7"/>
     </row>
     <row r="21" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="11">
-        <v>2377</v>
-      </c>
-      <c r="C21" s="14">
-        <v>44689</v>
-      </c>
+      <c r="B21" s="11"/>
+      <c r="C21" s="14"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -754,12 +748,8 @@
       <c r="H21" s="7"/>
     </row>
     <row r="22" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="11">
-        <v>2376</v>
-      </c>
-      <c r="C22" s="14">
-        <v>44685</v>
-      </c>
+      <c r="B22" s="11"/>
+      <c r="C22" s="14"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
@@ -767,12 +757,8 @@
       <c r="H22" s="7"/>
     </row>
     <row r="23" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="11">
-        <v>2375</v>
-      </c>
-      <c r="C23" s="14">
-        <v>44682</v>
-      </c>
+      <c r="B23" s="11"/>
+      <c r="C23" s="14"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
@@ -780,12 +766,8 @@
       <c r="H23" s="7"/>
     </row>
     <row r="24" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="11">
-        <v>2374</v>
-      </c>
-      <c r="C24" s="14">
-        <v>44678</v>
-      </c>
+      <c r="B24" s="11"/>
+      <c r="C24" s="14"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
@@ -793,12 +775,8 @@
       <c r="H24" s="7"/>
     </row>
     <row r="25" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="11">
-        <v>2373</v>
-      </c>
-      <c r="C25" s="14">
-        <v>44675</v>
-      </c>
+      <c r="B25" s="11"/>
+      <c r="C25" s="14"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
@@ -806,12 +784,8 @@
       <c r="H25" s="7"/>
     </row>
     <row r="26" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="11">
-        <v>2372</v>
-      </c>
-      <c r="C26" s="14">
-        <v>44671</v>
-      </c>
+      <c r="B26" s="11"/>
+      <c r="C26" s="14"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
@@ -819,12 +793,8 @@
       <c r="H26" s="7"/>
     </row>
     <row r="27" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="11">
-        <v>2371</v>
-      </c>
-      <c r="C27" s="14">
-        <v>44668</v>
-      </c>
+      <c r="B27" s="11"/>
+      <c r="C27" s="14"/>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
@@ -832,12 +802,8 @@
       <c r="H27" s="7"/>
     </row>
     <row r="28" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="11">
-        <v>2370</v>
-      </c>
-      <c r="C28" s="14">
-        <v>44664</v>
-      </c>
+      <c r="B28" s="11"/>
+      <c r="C28" s="14"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
@@ -845,12 +811,8 @@
       <c r="H28" s="7"/>
     </row>
     <row r="29" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="11">
-        <v>2369</v>
-      </c>
-      <c r="C29" s="14">
-        <v>44661</v>
-      </c>
+      <c r="B29" s="11"/>
+      <c r="C29" s="14"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
@@ -858,12 +820,8 @@
       <c r="H29" s="7"/>
     </row>
     <row r="30" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="11">
-        <v>2368</v>
-      </c>
-      <c r="C30" s="14">
-        <v>44657</v>
-      </c>
+      <c r="B30" s="11"/>
+      <c r="C30" s="14"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
@@ -871,12 +829,8 @@
       <c r="H30" s="7"/>
     </row>
     <row r="31" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="11">
-        <v>2367</v>
-      </c>
-      <c r="C31" s="14">
-        <v>44654</v>
-      </c>
+      <c r="B31" s="11"/>
+      <c r="C31" s="14"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
@@ -884,24 +838,21 @@
       <c r="H31" s="7"/>
     </row>
     <row r="32" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="11">
-        <v>2366</v>
-      </c>
-      <c r="C32" s="14">
-        <v>44650</v>
-      </c>
+      <c r="B32" s="11"/>
+      <c r="C32" s="14"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
     </row>
-    <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="11">
-        <v>2365</v>
-      </c>
-      <c r="C33" s="14">
-        <v>44647</v>
+        <f>B34+23</f>
+        <v>2403</v>
+      </c>
+      <c r="C33" s="15">
+        <v>44927</v>
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
@@ -909,12 +860,12 @@
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
     </row>
-    <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="11">
-        <v>2364</v>
+        <v>2380</v>
       </c>
       <c r="C34" s="14">
-        <v>44643</v>
+        <v>44699</v>
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
@@ -922,12 +873,12 @@
       <c r="G34" s="7"/>
       <c r="H34" s="7"/>
     </row>
-    <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="11">
-        <v>2363</v>
+        <v>2379</v>
       </c>
       <c r="C35" s="14">
-        <v>44640</v>
+        <v>44696</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
@@ -935,12 +886,12 @@
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
     </row>
-    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="11">
-        <v>2362</v>
+        <v>2378</v>
       </c>
       <c r="C36" s="14">
-        <v>44636</v>
+        <v>44692</v>
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
@@ -948,12 +899,12 @@
       <c r="G36" s="7"/>
       <c r="H36" s="7"/>
     </row>
-    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="11">
-        <v>2361</v>
+        <v>2377</v>
       </c>
       <c r="C37" s="14">
-        <v>44633</v>
+        <v>44689</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
@@ -961,12 +912,12 @@
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
     </row>
-    <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="11">
-        <v>2360</v>
+        <v>2376</v>
       </c>
       <c r="C38" s="14">
-        <v>44629</v>
+        <v>44685</v>
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
@@ -974,12 +925,12 @@
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
     </row>
-    <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="11">
-        <v>2359</v>
+        <v>2375</v>
       </c>
       <c r="C39" s="14">
-        <v>44626</v>
+        <v>44682</v>
       </c>
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
@@ -987,39 +938,247 @@
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
     </row>
-    <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>11</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>12</v>
+    <row r="40" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="11">
+        <v>2374</v>
       </c>
       <c r="C40" s="14">
-        <v>34623</v>
+        <v>44678</v>
       </c>
       <c r="D40" s="7"/>
-      <c r="E40" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="E40" s="7"/>
       <c r="F40" s="7"/>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
     </row>
-    <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>10</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>12</v>
+    <row r="41" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="11">
+        <v>2373</v>
       </c>
       <c r="C41" s="14">
-        <v>38126</v>
+        <v>44675</v>
       </c>
       <c r="D41" s="7"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
       <c r="H41" s="7"/>
+    </row>
+    <row r="42" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="11">
+        <v>2372</v>
+      </c>
+      <c r="C42" s="14">
+        <v>44671</v>
+      </c>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+    </row>
+    <row r="43" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="11">
+        <v>2371</v>
+      </c>
+      <c r="C43" s="14">
+        <v>44668</v>
+      </c>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+    </row>
+    <row r="44" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="11">
+        <v>2370</v>
+      </c>
+      <c r="C44" s="14">
+        <v>44664</v>
+      </c>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+    </row>
+    <row r="45" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="11">
+        <v>2369</v>
+      </c>
+      <c r="C45" s="14">
+        <v>44661</v>
+      </c>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+    </row>
+    <row r="46" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="11">
+        <v>2368</v>
+      </c>
+      <c r="C46" s="14">
+        <v>44657</v>
+      </c>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+    </row>
+    <row r="47" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="11">
+        <v>2367</v>
+      </c>
+      <c r="C47" s="14">
+        <v>44654</v>
+      </c>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+    </row>
+    <row r="48" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="11">
+        <v>2366</v>
+      </c>
+      <c r="C48" s="14">
+        <v>44650</v>
+      </c>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
+    </row>
+    <row r="49" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="11">
+        <v>2365</v>
+      </c>
+      <c r="C49" s="14">
+        <v>44647</v>
+      </c>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
+    </row>
+    <row r="50" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="11">
+        <v>2364</v>
+      </c>
+      <c r="C50" s="14">
+        <v>44643</v>
+      </c>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
+    </row>
+    <row r="51" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="11">
+        <v>2363</v>
+      </c>
+      <c r="C51" s="14">
+        <v>44640</v>
+      </c>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="7"/>
+    </row>
+    <row r="52" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="11">
+        <v>2362</v>
+      </c>
+      <c r="C52" s="14">
+        <v>44636</v>
+      </c>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="7"/>
+    </row>
+    <row r="53" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="11">
+        <v>2361</v>
+      </c>
+      <c r="C53" s="14">
+        <v>44633</v>
+      </c>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="7"/>
+    </row>
+    <row r="54" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="11">
+        <v>2360</v>
+      </c>
+      <c r="C54" s="14">
+        <v>44629</v>
+      </c>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
+    </row>
+    <row r="55" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="11">
+        <v>2359</v>
+      </c>
+      <c r="C55" s="14">
+        <v>44626</v>
+      </c>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
+    </row>
+    <row r="56" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>11</v>
+      </c>
+      <c r="B56" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C56" s="14">
+        <v>34623</v>
+      </c>
+      <c r="D56" s="7"/>
+      <c r="E56" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="7"/>
+    </row>
+    <row r="57" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>10</v>
+      </c>
+      <c r="B57" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C57" s="14">
+        <v>38126</v>
+      </c>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1029,10 +1188,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15FEB743-8F41-4809-BA70-E7C1EBE37B84}">
-  <dimension ref="A1:H150"/>
+  <dimension ref="A1:H159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1180,8 +1339,12 @@
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="4"/>
-      <c r="C16" s="14"/>
+      <c r="B16" s="4">
+        <v>1354</v>
+      </c>
+      <c r="C16" s="14">
+        <v>44926</v>
+      </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -1190,10 +1353,10 @@
     </row>
     <row r="17" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="4">
-        <v>1344</v>
+        <v>1353</v>
       </c>
       <c r="C17" s="14">
-        <v>44903</v>
+        <v>44924</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -1203,10 +1366,10 @@
     </row>
     <row r="18" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="4">
-        <v>1343</v>
+        <v>1352</v>
       </c>
       <c r="C18" s="14">
-        <v>44901</v>
+        <v>44922</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
@@ -1216,10 +1379,10 @@
     </row>
     <row r="19" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="4">
-        <v>1342</v>
+        <v>1351</v>
       </c>
       <c r="C19" s="14">
-        <v>44898</v>
+        <v>44919</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
@@ -1229,10 +1392,10 @@
     </row>
     <row r="20" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="4">
-        <v>1341</v>
+        <v>1350</v>
       </c>
       <c r="C20" s="14">
-        <v>44896</v>
+        <v>44917</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
@@ -1242,10 +1405,10 @@
     </row>
     <row r="21" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="4">
-        <v>1340</v>
+        <v>1349</v>
       </c>
       <c r="C21" s="14">
-        <v>44894</v>
+        <v>44915</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
@@ -1255,10 +1418,10 @@
     </row>
     <row r="22" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="4">
-        <v>1339</v>
+        <v>1348</v>
       </c>
       <c r="C22" s="14">
-        <v>44891</v>
+        <v>44912</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
@@ -1268,12 +1431,12 @@
     </row>
     <row r="23" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="4">
-        <v>1338</v>
+        <v>1347</v>
       </c>
       <c r="C23" s="14">
-        <v>44889</v>
-      </c>
-      <c r="D23" s="14"/>
+        <v>44910</v>
+      </c>
+      <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
@@ -1281,10 +1444,10 @@
     </row>
     <row r="24" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="4">
-        <v>1337</v>
+        <v>1346</v>
       </c>
       <c r="C24" s="14">
-        <v>44887</v>
+        <v>44908</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
@@ -1294,10 +1457,10 @@
     </row>
     <row r="25" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="4">
-        <v>1336</v>
+        <v>1345</v>
       </c>
       <c r="C25" s="14">
-        <v>44884</v>
+        <v>44905</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
@@ -1307,10 +1470,10 @@
     </row>
     <row r="26" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="4">
-        <v>1335</v>
+        <v>1344</v>
       </c>
       <c r="C26" s="14">
-        <v>44882</v>
+        <v>44903</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
@@ -1320,10 +1483,10 @@
     </row>
     <row r="27" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="4">
-        <v>1334</v>
+        <v>1343</v>
       </c>
       <c r="C27" s="14">
-        <v>44880</v>
+        <v>44901</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
@@ -1333,10 +1496,10 @@
     </row>
     <row r="28" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="4">
-        <v>1333</v>
+        <v>1342</v>
       </c>
       <c r="C28" s="14">
-        <v>44877</v>
+        <v>44898</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
@@ -1346,10 +1509,10 @@
     </row>
     <row r="29" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="4">
-        <v>1332</v>
+        <v>1341</v>
       </c>
       <c r="C29" s="14">
-        <v>44875</v>
+        <v>44896</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -1359,10 +1522,10 @@
     </row>
     <row r="30" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="4">
-        <v>1331</v>
+        <v>1340</v>
       </c>
       <c r="C30" s="14">
-        <v>44873</v>
+        <v>44894</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
@@ -1372,10 +1535,10 @@
     </row>
     <row r="31" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="4">
-        <v>1330</v>
+        <v>1339</v>
       </c>
       <c r="C31" s="14">
-        <v>44870</v>
+        <v>44891</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -1385,12 +1548,12 @@
     </row>
     <row r="32" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="4">
-        <v>1329</v>
+        <v>1338</v>
       </c>
       <c r="C32" s="14">
-        <v>44868</v>
-      </c>
-      <c r="D32" s="4"/>
+        <v>44889</v>
+      </c>
+      <c r="D32" s="14"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
@@ -1398,10 +1561,10 @@
     </row>
     <row r="33" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="4">
-        <v>1328</v>
+        <v>1337</v>
       </c>
       <c r="C33" s="14">
-        <v>44866</v>
+        <v>44887</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
@@ -1411,10 +1574,10 @@
     </row>
     <row r="34" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="4">
-        <v>1327</v>
+        <v>1336</v>
       </c>
       <c r="C34" s="14">
-        <v>44863</v>
+        <v>44884</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
@@ -1424,10 +1587,10 @@
     </row>
     <row r="35" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="4">
-        <v>1326</v>
+        <v>1335</v>
       </c>
       <c r="C35" s="14">
-        <v>44861</v>
+        <v>44882</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -1437,10 +1600,10 @@
     </row>
     <row r="36" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="4">
-        <v>1325</v>
+        <v>1334</v>
       </c>
       <c r="C36" s="14">
-        <v>44859</v>
+        <v>44880</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -1450,10 +1613,10 @@
     </row>
     <row r="37" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="4">
-        <v>1324</v>
+        <v>1333</v>
       </c>
       <c r="C37" s="14">
-        <v>44856</v>
+        <v>44877</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -1463,10 +1626,10 @@
     </row>
     <row r="38" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="4">
-        <v>1323</v>
+        <v>1332</v>
       </c>
       <c r="C38" s="14">
-        <v>44854</v>
+        <v>44875</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
@@ -1476,10 +1639,10 @@
     </row>
     <row r="39" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="4">
-        <v>1322</v>
+        <v>1331</v>
       </c>
       <c r="C39" s="14">
-        <v>44852</v>
+        <v>44873</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
@@ -1489,10 +1652,10 @@
     </row>
     <row r="40" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="4">
-        <v>1321</v>
+        <v>1330</v>
       </c>
       <c r="C40" s="14">
-        <v>44849</v>
+        <v>44870</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
@@ -1502,10 +1665,10 @@
     </row>
     <row r="41" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="4">
-        <v>1320</v>
+        <v>1329</v>
       </c>
       <c r="C41" s="14">
-        <v>44847</v>
+        <v>44868</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
@@ -1515,10 +1678,10 @@
     </row>
     <row r="42" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="4">
-        <v>1319</v>
+        <v>1328</v>
       </c>
       <c r="C42" s="14">
-        <v>44845</v>
+        <v>44866</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
@@ -1528,10 +1691,10 @@
     </row>
     <row r="43" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="4">
-        <v>1318</v>
+        <v>1327</v>
       </c>
       <c r="C43" s="14">
-        <v>44842</v>
+        <v>44863</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
@@ -1541,10 +1704,10 @@
     </row>
     <row r="44" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="4">
-        <v>1317</v>
+        <v>1326</v>
       </c>
       <c r="C44" s="14">
-        <v>44840</v>
+        <v>44861</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -1554,10 +1717,10 @@
     </row>
     <row r="45" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="4">
-        <v>1316</v>
+        <v>1325</v>
       </c>
       <c r="C45" s="14">
-        <v>44838</v>
+        <v>44859</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
@@ -1567,10 +1730,10 @@
     </row>
     <row r="46" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="4">
-        <v>1315</v>
+        <v>1324</v>
       </c>
       <c r="C46" s="14">
-        <v>44835</v>
+        <v>44856</v>
       </c>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
@@ -1580,10 +1743,10 @@
     </row>
     <row r="47" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="4">
-        <v>1314</v>
+        <v>1323</v>
       </c>
       <c r="C47" s="14">
-        <v>44833</v>
+        <v>44854</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
@@ -1593,10 +1756,10 @@
     </row>
     <row r="48" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="4">
-        <v>1313</v>
+        <v>1322</v>
       </c>
       <c r="C48" s="14">
-        <v>44831</v>
+        <v>44852</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
@@ -1606,10 +1769,10 @@
     </row>
     <row r="49" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="4">
-        <v>1312</v>
+        <v>1321</v>
       </c>
       <c r="C49" s="14">
-        <v>44828</v>
+        <v>44849</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
@@ -1619,10 +1782,10 @@
     </row>
     <row r="50" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="4">
-        <v>1311</v>
+        <v>1320</v>
       </c>
       <c r="C50" s="14">
-        <v>44826</v>
+        <v>44847</v>
       </c>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
@@ -1632,10 +1795,10 @@
     </row>
     <row r="51" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="4">
-        <v>1310</v>
+        <v>1319</v>
       </c>
       <c r="C51" s="14">
-        <v>44824</v>
+        <v>44845</v>
       </c>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
@@ -1645,10 +1808,10 @@
     </row>
     <row r="52" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="4">
-        <v>1309</v>
+        <v>1318</v>
       </c>
       <c r="C52" s="14">
-        <v>44821</v>
+        <v>44842</v>
       </c>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
@@ -1658,10 +1821,10 @@
     </row>
     <row r="53" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="4">
-        <v>1308</v>
+        <v>1317</v>
       </c>
       <c r="C53" s="14">
-        <v>44819</v>
+        <v>44840</v>
       </c>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
@@ -1671,10 +1834,10 @@
     </row>
     <row r="54" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="4">
-        <v>1307</v>
+        <v>1316</v>
       </c>
       <c r="C54" s="14">
-        <v>44817</v>
+        <v>44838</v>
       </c>
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
@@ -1684,10 +1847,10 @@
     </row>
     <row r="55" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="4">
-        <v>1306</v>
+        <v>1315</v>
       </c>
       <c r="C55" s="14">
-        <v>44814</v>
+        <v>44835</v>
       </c>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
@@ -1697,10 +1860,10 @@
     </row>
     <row r="56" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="4">
-        <v>1305</v>
+        <v>1314</v>
       </c>
       <c r="C56" s="14">
-        <v>44812</v>
+        <v>44833</v>
       </c>
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
@@ -1710,10 +1873,10 @@
     </row>
     <row r="57" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="4">
-        <v>1304</v>
+        <v>1313</v>
       </c>
       <c r="C57" s="14">
-        <v>44810</v>
+        <v>44831</v>
       </c>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
@@ -1723,10 +1886,10 @@
     </row>
     <row r="58" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="4">
-        <v>1303</v>
+        <v>1312</v>
       </c>
       <c r="C58" s="14">
-        <v>44807</v>
+        <v>44828</v>
       </c>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
@@ -1736,10 +1899,10 @@
     </row>
     <row r="59" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="4">
-        <v>1302</v>
+        <v>1311</v>
       </c>
       <c r="C59" s="14">
-        <v>44805</v>
+        <v>44826</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
@@ -1749,10 +1912,10 @@
     </row>
     <row r="60" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B60" s="4">
-        <v>1301</v>
+        <v>1310</v>
       </c>
       <c r="C60" s="14">
-        <v>44803</v>
+        <v>44824</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
@@ -1762,10 +1925,10 @@
     </row>
     <row r="61" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B61" s="4">
-        <v>1300</v>
+        <v>1309</v>
       </c>
       <c r="C61" s="14">
-        <v>44800</v>
+        <v>44821</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
@@ -1775,10 +1938,10 @@
     </row>
     <row r="62" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B62" s="4">
-        <v>1299</v>
+        <v>1308</v>
       </c>
       <c r="C62" s="14">
-        <v>44798</v>
+        <v>44819</v>
       </c>
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
@@ -1788,10 +1951,10 @@
     </row>
     <row r="63" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="4">
-        <v>1298</v>
+        <v>1307</v>
       </c>
       <c r="C63" s="14">
-        <v>44796</v>
+        <v>44817</v>
       </c>
       <c r="D63" s="4"/>
       <c r="E63" s="4"/>
@@ -1801,10 +1964,10 @@
     </row>
     <row r="64" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B64" s="4">
-        <v>1297</v>
+        <v>1306</v>
       </c>
       <c r="C64" s="14">
-        <v>44793</v>
+        <v>44814</v>
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="4"/>
@@ -1814,10 +1977,10 @@
     </row>
     <row r="65" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B65" s="4">
-        <v>1296</v>
+        <v>1305</v>
       </c>
       <c r="C65" s="14">
-        <v>44791</v>
+        <v>44812</v>
       </c>
       <c r="D65" s="4"/>
       <c r="E65" s="4"/>
@@ -1827,10 +1990,10 @@
     </row>
     <row r="66" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B66" s="4">
-        <v>1295</v>
+        <v>1304</v>
       </c>
       <c r="C66" s="14">
-        <v>44789</v>
+        <v>44810</v>
       </c>
       <c r="D66" s="4"/>
       <c r="E66" s="4"/>
@@ -1840,10 +2003,10 @@
     </row>
     <row r="67" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B67" s="4">
-        <v>1294</v>
+        <v>1303</v>
       </c>
       <c r="C67" s="14">
-        <v>44786</v>
+        <v>44807</v>
       </c>
       <c r="D67" s="4"/>
       <c r="E67" s="4"/>
@@ -1853,10 +2016,10 @@
     </row>
     <row r="68" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="4">
-        <v>1293</v>
+        <v>1302</v>
       </c>
       <c r="C68" s="14">
-        <v>44784</v>
+        <v>44805</v>
       </c>
       <c r="D68" s="4"/>
       <c r="E68" s="4"/>
@@ -1866,10 +2029,10 @@
     </row>
     <row r="69" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B69" s="4">
-        <v>1292</v>
+        <v>1301</v>
       </c>
       <c r="C69" s="14">
-        <v>44782</v>
+        <v>44803</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69" s="4"/>
@@ -1879,10 +2042,10 @@
     </row>
     <row r="70" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B70" s="4">
-        <v>1291</v>
+        <v>1300</v>
       </c>
       <c r="C70" s="14">
-        <v>44779</v>
+        <v>44800</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="4"/>
@@ -1892,10 +2055,10 @@
     </row>
     <row r="71" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B71" s="4">
-        <v>1290</v>
+        <v>1299</v>
       </c>
       <c r="C71" s="14">
-        <v>44777</v>
+        <v>44798</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" s="4"/>
@@ -1905,10 +2068,10 @@
     </row>
     <row r="72" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B72" s="4">
-        <v>1289</v>
+        <v>1298</v>
       </c>
       <c r="C72" s="14">
-        <v>44775</v>
+        <v>44796</v>
       </c>
       <c r="D72" s="4"/>
       <c r="E72" s="4"/>
@@ -1918,10 +2081,10 @@
     </row>
     <row r="73" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B73" s="4">
-        <v>1288</v>
+        <v>1297</v>
       </c>
       <c r="C73" s="14">
-        <v>44772</v>
+        <v>44793</v>
       </c>
       <c r="D73" s="4"/>
       <c r="E73" s="4"/>
@@ -1931,10 +2094,10 @@
     </row>
     <row r="74" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B74" s="4">
-        <v>1287</v>
+        <v>1296</v>
       </c>
       <c r="C74" s="14">
-        <v>44770</v>
+        <v>44791</v>
       </c>
       <c r="D74" s="4"/>
       <c r="E74" s="4"/>
@@ -1944,10 +2107,10 @@
     </row>
     <row r="75" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B75" s="4">
-        <v>1286</v>
+        <v>1295</v>
       </c>
       <c r="C75" s="14">
-        <v>44768</v>
+        <v>44789</v>
       </c>
       <c r="D75" s="4"/>
       <c r="E75" s="4"/>
@@ -1957,10 +2120,10 @@
     </row>
     <row r="76" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B76" s="4">
-        <v>1285</v>
+        <v>1294</v>
       </c>
       <c r="C76" s="14">
-        <v>44765</v>
+        <v>44786</v>
       </c>
       <c r="D76" s="4"/>
       <c r="E76" s="4"/>
@@ -1970,10 +2133,10 @@
     </row>
     <row r="77" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B77" s="4">
-        <v>1284</v>
+        <v>1293</v>
       </c>
       <c r="C77" s="14">
-        <v>44763</v>
+        <v>44784</v>
       </c>
       <c r="D77" s="4"/>
       <c r="E77" s="4"/>
@@ -1983,10 +2146,10 @@
     </row>
     <row r="78" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="4">
-        <v>1283</v>
+        <v>1292</v>
       </c>
       <c r="C78" s="14">
-        <v>44761</v>
+        <v>44782</v>
       </c>
       <c r="D78" s="4"/>
       <c r="E78" s="4"/>
@@ -1996,10 +2159,10 @@
     </row>
     <row r="79" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B79" s="4">
-        <v>1282</v>
+        <v>1291</v>
       </c>
       <c r="C79" s="14">
-        <v>44758</v>
+        <v>44779</v>
       </c>
       <c r="D79" s="4"/>
       <c r="E79" s="4"/>
@@ -2009,10 +2172,10 @@
     </row>
     <row r="80" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B80" s="4">
-        <v>1281</v>
+        <v>1290</v>
       </c>
       <c r="C80" s="14">
-        <v>44756</v>
+        <v>44777</v>
       </c>
       <c r="D80" s="4"/>
       <c r="E80" s="4"/>
@@ -2022,10 +2185,10 @@
     </row>
     <row r="81" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B81" s="4">
-        <v>1280</v>
+        <v>1289</v>
       </c>
       <c r="C81" s="14">
-        <v>44754</v>
+        <v>44775</v>
       </c>
       <c r="D81" s="4"/>
       <c r="E81" s="4"/>
@@ -2035,10 +2198,10 @@
     </row>
     <row r="82" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B82" s="4">
-        <v>1279</v>
+        <v>1288</v>
       </c>
       <c r="C82" s="14">
-        <v>44751</v>
+        <v>44772</v>
       </c>
       <c r="D82" s="4"/>
       <c r="E82" s="4"/>
@@ -2048,10 +2211,10 @@
     </row>
     <row r="83" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B83" s="4">
-        <v>1278</v>
+        <v>1287</v>
       </c>
       <c r="C83" s="14">
-        <v>44749</v>
+        <v>44770</v>
       </c>
       <c r="D83" s="4"/>
       <c r="E83" s="4"/>
@@ -2061,10 +2224,10 @@
     </row>
     <row r="84" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B84" s="4">
-        <v>1277</v>
+        <v>1286</v>
       </c>
       <c r="C84" s="14">
-        <v>44747</v>
+        <v>44768</v>
       </c>
       <c r="D84" s="4"/>
       <c r="E84" s="4"/>
@@ -2074,10 +2237,10 @@
     </row>
     <row r="85" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B85" s="4">
-        <v>1276</v>
+        <v>1285</v>
       </c>
       <c r="C85" s="14">
-        <v>44744</v>
+        <v>44765</v>
       </c>
       <c r="D85" s="4"/>
       <c r="E85" s="4"/>
@@ -2087,10 +2250,10 @@
     </row>
     <row r="86" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B86" s="4">
-        <v>1275</v>
+        <v>1284</v>
       </c>
       <c r="C86" s="14">
-        <v>44742</v>
+        <v>44763</v>
       </c>
       <c r="D86" s="4"/>
       <c r="E86" s="4"/>
@@ -2100,10 +2263,10 @@
     </row>
     <row r="87" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B87" s="4">
-        <v>1274</v>
+        <v>1283</v>
       </c>
       <c r="C87" s="14">
-        <v>44740</v>
+        <v>44761</v>
       </c>
       <c r="D87" s="4"/>
       <c r="E87" s="4"/>
@@ -2113,10 +2276,10 @@
     </row>
     <row r="88" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B88" s="4">
-        <v>1273</v>
+        <v>1282</v>
       </c>
       <c r="C88" s="14">
-        <v>44737</v>
+        <v>44758</v>
       </c>
       <c r="D88" s="4"/>
       <c r="E88" s="4"/>
@@ -2126,10 +2289,10 @@
     </row>
     <row r="89" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B89" s="4">
-        <v>1272</v>
+        <v>1281</v>
       </c>
       <c r="C89" s="14">
-        <v>44735</v>
+        <v>44756</v>
       </c>
       <c r="D89" s="4"/>
       <c r="E89" s="4"/>
@@ -2139,10 +2302,10 @@
     </row>
     <row r="90" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B90" s="4">
-        <v>1271</v>
+        <v>1280</v>
       </c>
       <c r="C90" s="14">
-        <v>44733</v>
+        <v>44754</v>
       </c>
       <c r="D90" s="4"/>
       <c r="E90" s="4"/>
@@ -2152,10 +2315,10 @@
     </row>
     <row r="91" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B91" s="4">
-        <v>1270</v>
+        <v>1279</v>
       </c>
       <c r="C91" s="14">
-        <v>44730</v>
+        <v>44751</v>
       </c>
       <c r="D91" s="4"/>
       <c r="E91" s="4"/>
@@ -2165,10 +2328,10 @@
     </row>
     <row r="92" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B92" s="4">
-        <v>1269</v>
+        <v>1278</v>
       </c>
       <c r="C92" s="14">
-        <v>44728</v>
+        <v>44749</v>
       </c>
       <c r="D92" s="4"/>
       <c r="E92" s="4"/>
@@ -2178,10 +2341,10 @@
     </row>
     <row r="93" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B93" s="4">
-        <v>1268</v>
+        <v>1277</v>
       </c>
       <c r="C93" s="14">
-        <v>44726</v>
+        <v>44747</v>
       </c>
       <c r="D93" s="4"/>
       <c r="E93" s="4"/>
@@ -2191,10 +2354,10 @@
     </row>
     <row r="94" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B94" s="4">
-        <v>1267</v>
+        <v>1276</v>
       </c>
       <c r="C94" s="14">
-        <v>44723</v>
+        <v>44744</v>
       </c>
       <c r="D94" s="4"/>
       <c r="E94" s="4"/>
@@ -2204,10 +2367,10 @@
     </row>
     <row r="95" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B95" s="4">
-        <v>1266</v>
+        <v>1275</v>
       </c>
       <c r="C95" s="14">
-        <v>44721</v>
+        <v>44742</v>
       </c>
       <c r="D95" s="4"/>
       <c r="E95" s="4"/>
@@ -2217,10 +2380,10 @@
     </row>
     <row r="96" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B96" s="4">
-        <v>1265</v>
+        <v>1274</v>
       </c>
       <c r="C96" s="14">
-        <v>44719</v>
+        <v>44740</v>
       </c>
       <c r="D96" s="4"/>
       <c r="E96" s="4"/>
@@ -2230,10 +2393,10 @@
     </row>
     <row r="97" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B97" s="4">
-        <v>1264</v>
+        <v>1273</v>
       </c>
       <c r="C97" s="14">
-        <v>44716</v>
+        <v>44737</v>
       </c>
       <c r="D97" s="4"/>
       <c r="E97" s="4"/>
@@ -2243,10 +2406,10 @@
     </row>
     <row r="98" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B98" s="4">
-        <v>1263</v>
+        <v>1272</v>
       </c>
       <c r="C98" s="14">
-        <v>44714</v>
+        <v>44735</v>
       </c>
       <c r="D98" s="4"/>
       <c r="E98" s="4"/>
@@ -2256,10 +2419,10 @@
     </row>
     <row r="99" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B99" s="4">
-        <v>1262</v>
+        <v>1271</v>
       </c>
       <c r="C99" s="14">
-        <v>44712</v>
+        <v>44733</v>
       </c>
       <c r="D99" s="4"/>
       <c r="E99" s="4"/>
@@ -2269,10 +2432,10 @@
     </row>
     <row r="100" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B100" s="4">
-        <v>1261</v>
+        <v>1270</v>
       </c>
       <c r="C100" s="14">
-        <v>44709</v>
+        <v>44730</v>
       </c>
       <c r="D100" s="4"/>
       <c r="E100" s="4"/>
@@ -2282,10 +2445,10 @@
     </row>
     <row r="101" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B101" s="4">
-        <v>1260</v>
+        <v>1269</v>
       </c>
       <c r="C101" s="14">
-        <v>44707</v>
+        <v>44728</v>
       </c>
       <c r="D101" s="4"/>
       <c r="E101" s="4"/>
@@ -2295,10 +2458,10 @@
     </row>
     <row r="102" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B102" s="4">
-        <v>1259</v>
+        <v>1268</v>
       </c>
       <c r="C102" s="14">
-        <v>44705</v>
+        <v>44726</v>
       </c>
       <c r="D102" s="4"/>
       <c r="E102" s="4"/>
@@ -2308,10 +2471,10 @@
     </row>
     <row r="103" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B103" s="4">
-        <v>1258</v>
+        <v>1267</v>
       </c>
       <c r="C103" s="14">
-        <v>44702</v>
+        <v>44723</v>
       </c>
       <c r="D103" s="4"/>
       <c r="E103" s="4"/>
@@ -2321,10 +2484,10 @@
     </row>
     <row r="104" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B104" s="4">
-        <v>1257</v>
+        <v>1266</v>
       </c>
       <c r="C104" s="14">
-        <v>44700</v>
+        <v>44721</v>
       </c>
       <c r="D104" s="4"/>
       <c r="E104" s="4"/>
@@ -2334,10 +2497,10 @@
     </row>
     <row r="105" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B105" s="4">
-        <v>1256</v>
+        <v>1265</v>
       </c>
       <c r="C105" s="14">
-        <v>44698</v>
+        <v>44719</v>
       </c>
       <c r="D105" s="4"/>
       <c r="E105" s="4"/>
@@ -2347,10 +2510,10 @@
     </row>
     <row r="106" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B106" s="4">
-        <v>1255</v>
+        <v>1264</v>
       </c>
       <c r="C106" s="14">
-        <v>44695</v>
+        <v>44716</v>
       </c>
       <c r="D106" s="4"/>
       <c r="E106" s="4"/>
@@ -2360,10 +2523,10 @@
     </row>
     <row r="107" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B107" s="4">
-        <v>1254</v>
+        <v>1263</v>
       </c>
       <c r="C107" s="14">
-        <v>44693</v>
+        <v>44714</v>
       </c>
       <c r="D107" s="4"/>
       <c r="E107" s="4"/>
@@ -2373,10 +2536,10 @@
     </row>
     <row r="108" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B108" s="4">
-        <v>1253</v>
+        <v>1262</v>
       </c>
       <c r="C108" s="14">
-        <v>44691</v>
+        <v>44712</v>
       </c>
       <c r="D108" s="4"/>
       <c r="E108" s="4"/>
@@ -2386,10 +2549,10 @@
     </row>
     <row r="109" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B109" s="4">
-        <v>1252</v>
+        <v>1261</v>
       </c>
       <c r="C109" s="14">
-        <v>44688</v>
+        <v>44709</v>
       </c>
       <c r="D109" s="4"/>
       <c r="E109" s="4"/>
@@ -2399,10 +2562,10 @@
     </row>
     <row r="110" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B110" s="4">
-        <v>1251</v>
+        <v>1260</v>
       </c>
       <c r="C110" s="14">
-        <v>44686</v>
+        <v>44707</v>
       </c>
       <c r="D110" s="4"/>
       <c r="E110" s="4"/>
@@ -2412,10 +2575,10 @@
     </row>
     <row r="111" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B111" s="4">
-        <v>1250</v>
+        <v>1259</v>
       </c>
       <c r="C111" s="14">
-        <v>44684</v>
+        <v>44705</v>
       </c>
       <c r="D111" s="4"/>
       <c r="E111" s="4"/>
@@ -2425,10 +2588,10 @@
     </row>
     <row r="112" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B112" s="4">
-        <v>1249</v>
+        <v>1258</v>
       </c>
       <c r="C112" s="14">
-        <v>44681</v>
+        <v>44702</v>
       </c>
       <c r="D112" s="4"/>
       <c r="E112" s="4"/>
@@ -2438,10 +2601,10 @@
     </row>
     <row r="113" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B113" s="4">
-        <v>1248</v>
+        <v>1257</v>
       </c>
       <c r="C113" s="14">
-        <v>44679</v>
+        <v>44700</v>
       </c>
       <c r="D113" s="4"/>
       <c r="E113" s="4"/>
@@ -2451,10 +2614,10 @@
     </row>
     <row r="114" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B114" s="4">
-        <v>1247</v>
+        <v>1256</v>
       </c>
       <c r="C114" s="14">
-        <v>44677</v>
+        <v>44698</v>
       </c>
       <c r="D114" s="4"/>
       <c r="E114" s="4"/>
@@ -2464,10 +2627,10 @@
     </row>
     <row r="115" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B115" s="4">
-        <v>1246</v>
+        <v>1255</v>
       </c>
       <c r="C115" s="14">
-        <v>44674</v>
+        <v>44695</v>
       </c>
       <c r="D115" s="4"/>
       <c r="E115" s="4"/>
@@ -2477,10 +2640,10 @@
     </row>
     <row r="116" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B116" s="4">
-        <v>1245</v>
+        <v>1254</v>
       </c>
       <c r="C116" s="14">
-        <v>44672</v>
+        <v>44693</v>
       </c>
       <c r="D116" s="4"/>
       <c r="E116" s="4"/>
@@ -2490,10 +2653,10 @@
     </row>
     <row r="117" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B117" s="4">
-        <v>1244</v>
+        <v>1253</v>
       </c>
       <c r="C117" s="14">
-        <v>44670</v>
+        <v>44691</v>
       </c>
       <c r="D117" s="4"/>
       <c r="E117" s="4"/>
@@ -2503,10 +2666,10 @@
     </row>
     <row r="118" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B118" s="4">
-        <v>1243</v>
+        <v>1252</v>
       </c>
       <c r="C118" s="14">
-        <v>44667</v>
+        <v>44688</v>
       </c>
       <c r="D118" s="4"/>
       <c r="E118" s="4"/>
@@ -2516,10 +2679,10 @@
     </row>
     <row r="119" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B119" s="4">
-        <v>1242</v>
+        <v>1251</v>
       </c>
       <c r="C119" s="14">
-        <v>44665</v>
+        <v>44686</v>
       </c>
       <c r="D119" s="4"/>
       <c r="E119" s="4"/>
@@ -2529,10 +2692,10 @@
     </row>
     <row r="120" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B120" s="4">
-        <v>1241</v>
+        <v>1250</v>
       </c>
       <c r="C120" s="14">
-        <v>44663</v>
+        <v>44684</v>
       </c>
       <c r="D120" s="4"/>
       <c r="E120" s="4"/>
@@ -2542,10 +2705,10 @@
     </row>
     <row r="121" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B121" s="4">
-        <v>1240</v>
+        <v>1249</v>
       </c>
       <c r="C121" s="14">
-        <v>44660</v>
+        <v>44681</v>
       </c>
       <c r="D121" s="4"/>
       <c r="E121" s="4"/>
@@ -2555,10 +2718,10 @@
     </row>
     <row r="122" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B122" s="4">
-        <v>1239</v>
+        <v>1248</v>
       </c>
       <c r="C122" s="14">
-        <v>44658</v>
+        <v>44679</v>
       </c>
       <c r="D122" s="4"/>
       <c r="E122" s="4"/>
@@ -2568,10 +2731,10 @@
     </row>
     <row r="123" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B123" s="4">
-        <v>1238</v>
+        <v>1247</v>
       </c>
       <c r="C123" s="14">
-        <v>44656</v>
+        <v>44677</v>
       </c>
       <c r="D123" s="4"/>
       <c r="E123" s="4"/>
@@ -2581,10 +2744,10 @@
     </row>
     <row r="124" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B124" s="4">
-        <v>1237</v>
+        <v>1246</v>
       </c>
       <c r="C124" s="14">
-        <v>44653</v>
+        <v>44674</v>
       </c>
       <c r="D124" s="4"/>
       <c r="E124" s="4"/>
@@ -2594,10 +2757,10 @@
     </row>
     <row r="125" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B125" s="4">
-        <v>1236</v>
+        <v>1245</v>
       </c>
       <c r="C125" s="14">
-        <v>44651</v>
+        <v>44672</v>
       </c>
       <c r="D125" s="4"/>
       <c r="E125" s="4"/>
@@ -2607,10 +2770,10 @@
     </row>
     <row r="126" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B126" s="4">
-        <v>1235</v>
+        <v>1244</v>
       </c>
       <c r="C126" s="14">
-        <v>44649</v>
+        <v>44670</v>
       </c>
       <c r="D126" s="4"/>
       <c r="E126" s="4"/>
@@ -2620,10 +2783,10 @@
     </row>
     <row r="127" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B127" s="4">
-        <v>1234</v>
+        <v>1243</v>
       </c>
       <c r="C127" s="14">
-        <v>44646</v>
+        <v>44667</v>
       </c>
       <c r="D127" s="4"/>
       <c r="E127" s="4"/>
@@ -2633,10 +2796,10 @@
     </row>
     <row r="128" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B128" s="4">
-        <v>1233</v>
+        <v>1242</v>
       </c>
       <c r="C128" s="14">
-        <v>44644</v>
+        <v>44665</v>
       </c>
       <c r="D128" s="4"/>
       <c r="E128" s="4"/>
@@ -2646,10 +2809,10 @@
     </row>
     <row r="129" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B129" s="4">
-        <v>1232</v>
+        <v>1241</v>
       </c>
       <c r="C129" s="14">
-        <v>44642</v>
+        <v>44663</v>
       </c>
       <c r="D129" s="4"/>
       <c r="E129" s="4"/>
@@ -2659,10 +2822,10 @@
     </row>
     <row r="130" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B130" s="4">
-        <v>1231</v>
+        <v>1240</v>
       </c>
       <c r="C130" s="14">
-        <v>44639</v>
+        <v>44660</v>
       </c>
       <c r="D130" s="4"/>
       <c r="E130" s="4"/>
@@ -2672,10 +2835,10 @@
     </row>
     <row r="131" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B131" s="4">
-        <v>1230</v>
+        <v>1239</v>
       </c>
       <c r="C131" s="14">
-        <v>44637</v>
+        <v>44658</v>
       </c>
       <c r="D131" s="4"/>
       <c r="E131" s="4"/>
@@ -2685,10 +2848,10 @@
     </row>
     <row r="132" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B132" s="4">
-        <v>1229</v>
+        <v>1238</v>
       </c>
       <c r="C132" s="14">
-        <v>44635</v>
+        <v>44656</v>
       </c>
       <c r="D132" s="4"/>
       <c r="E132" s="4"/>
@@ -2698,10 +2861,10 @@
     </row>
     <row r="133" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B133" s="4">
-        <v>1228</v>
-      </c>
-      <c r="C133">
-        <v>44632</v>
+        <v>1237</v>
+      </c>
+      <c r="C133" s="14">
+        <v>44653</v>
       </c>
       <c r="D133" s="4"/>
       <c r="E133" s="4"/>
@@ -2711,10 +2874,10 @@
     </row>
     <row r="134" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B134" s="4">
-        <v>1227</v>
-      </c>
-      <c r="C134">
-        <v>44630</v>
+        <v>1236</v>
+      </c>
+      <c r="C134" s="14">
+        <v>44651</v>
       </c>
       <c r="D134" s="4"/>
       <c r="E134" s="4"/>
@@ -2724,10 +2887,10 @@
     </row>
     <row r="135" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B135" s="4">
-        <v>1226</v>
-      </c>
-      <c r="C135">
-        <v>44628</v>
+        <v>1235</v>
+      </c>
+      <c r="C135" s="14">
+        <v>44649</v>
       </c>
       <c r="D135" s="4"/>
       <c r="E135" s="4"/>
@@ -2737,10 +2900,10 @@
     </row>
     <row r="136" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B136" s="4">
-        <v>1225</v>
-      </c>
-      <c r="C136">
-        <v>44625</v>
+        <v>1234</v>
+      </c>
+      <c r="C136" s="14">
+        <v>44646</v>
       </c>
       <c r="D136" s="4"/>
       <c r="E136" s="4"/>
@@ -2750,10 +2913,10 @@
     </row>
     <row r="137" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B137" s="4">
-        <v>1224</v>
-      </c>
-      <c r="C137">
-        <v>44623</v>
+        <v>1233</v>
+      </c>
+      <c r="C137" s="14">
+        <v>44644</v>
       </c>
       <c r="D137" s="4"/>
       <c r="E137" s="4"/>
@@ -2763,10 +2926,10 @@
     </row>
     <row r="138" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B138" s="4">
-        <v>1223</v>
-      </c>
-      <c r="C138">
-        <v>44621</v>
+        <v>1232</v>
+      </c>
+      <c r="C138" s="14">
+        <v>44642</v>
       </c>
       <c r="D138" s="4"/>
       <c r="E138" s="4"/>
@@ -2776,10 +2939,10 @@
     </row>
     <row r="139" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B139" s="4">
-        <v>1222</v>
-      </c>
-      <c r="C139">
-        <v>44618</v>
+        <v>1231</v>
+      </c>
+      <c r="C139" s="14">
+        <v>44639</v>
       </c>
       <c r="D139" s="4"/>
       <c r="E139" s="4"/>
@@ -2789,10 +2952,10 @@
     </row>
     <row r="140" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B140" s="4">
-        <v>1221</v>
-      </c>
-      <c r="C140">
-        <v>44616</v>
+        <v>1230</v>
+      </c>
+      <c r="C140" s="14">
+        <v>44637</v>
       </c>
       <c r="D140" s="4"/>
       <c r="E140" s="4"/>
@@ -2802,10 +2965,10 @@
     </row>
     <row r="141" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B141" s="4">
-        <v>1220</v>
-      </c>
-      <c r="C141">
-        <v>44614</v>
+        <v>1229</v>
+      </c>
+      <c r="C141" s="14">
+        <v>44635</v>
       </c>
       <c r="D141" s="4"/>
       <c r="E141" s="4"/>
@@ -2815,10 +2978,10 @@
     </row>
     <row r="142" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B142" s="4">
-        <v>1219</v>
+        <v>1228</v>
       </c>
       <c r="C142">
-        <v>44611</v>
+        <v>44632</v>
       </c>
       <c r="D142" s="4"/>
       <c r="E142" s="4"/>
@@ -2828,10 +2991,10 @@
     </row>
     <row r="143" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B143" s="4">
-        <v>1218</v>
+        <v>1227</v>
       </c>
       <c r="C143">
-        <v>44609</v>
+        <v>44630</v>
       </c>
       <c r="D143" s="4"/>
       <c r="E143" s="4"/>
@@ -2841,10 +3004,10 @@
     </row>
     <row r="144" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B144" s="4">
-        <v>1217</v>
+        <v>1226</v>
       </c>
       <c r="C144">
-        <v>44607</v>
+        <v>44628</v>
       </c>
       <c r="D144" s="4"/>
       <c r="E144" s="4"/>
@@ -2854,10 +3017,10 @@
     </row>
     <row r="145" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B145" s="4">
-        <v>1216</v>
+        <v>1225</v>
       </c>
       <c r="C145">
-        <v>44604</v>
+        <v>44625</v>
       </c>
       <c r="D145" s="4"/>
       <c r="E145" s="4"/>
@@ -2867,10 +3030,10 @@
     </row>
     <row r="146" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B146" s="4">
-        <v>1215</v>
+        <v>1224</v>
       </c>
       <c r="C146">
-        <v>44602</v>
+        <v>44623</v>
       </c>
       <c r="D146" s="4"/>
       <c r="E146" s="4"/>
@@ -2880,10 +3043,10 @@
     </row>
     <row r="147" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B147" s="4">
-        <v>1214</v>
+        <v>1223</v>
       </c>
       <c r="C147">
-        <v>44600</v>
+        <v>44621</v>
       </c>
       <c r="D147" s="4"/>
       <c r="E147" s="4"/>
@@ -2893,10 +3056,10 @@
     </row>
     <row r="148" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B148" s="4">
-        <v>1213</v>
+        <v>1222</v>
       </c>
       <c r="C148">
-        <v>44597</v>
+        <v>44618</v>
       </c>
       <c r="D148" s="4"/>
       <c r="E148" s="4"/>
@@ -2906,10 +3069,10 @@
     </row>
     <row r="149" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B149" s="4">
-        <v>1212</v>
+        <v>1221</v>
       </c>
       <c r="C149">
-        <v>44595</v>
+        <v>44616</v>
       </c>
       <c r="D149" s="4"/>
       <c r="E149" s="4"/>
@@ -2919,10 +3082,10 @@
     </row>
     <row r="150" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B150" s="4">
-        <v>1211</v>
+        <v>1220</v>
       </c>
       <c r="C150">
-        <v>44593</v>
+        <v>44614</v>
       </c>
       <c r="D150" s="4"/>
       <c r="E150" s="4"/>
@@ -2930,6 +3093,123 @@
       <c r="G150" s="4"/>
       <c r="H150" s="4"/>
     </row>
+    <row r="151" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B151" s="4">
+        <v>1219</v>
+      </c>
+      <c r="C151">
+        <v>44611</v>
+      </c>
+      <c r="D151" s="4"/>
+      <c r="E151" s="4"/>
+      <c r="F151" s="4"/>
+      <c r="G151" s="4"/>
+      <c r="H151" s="4"/>
+    </row>
+    <row r="152" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B152" s="4">
+        <v>1218</v>
+      </c>
+      <c r="C152">
+        <v>44609</v>
+      </c>
+      <c r="D152" s="4"/>
+      <c r="E152" s="4"/>
+      <c r="F152" s="4"/>
+      <c r="G152" s="4"/>
+      <c r="H152" s="4"/>
+    </row>
+    <row r="153" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B153" s="4">
+        <v>1217</v>
+      </c>
+      <c r="C153">
+        <v>44607</v>
+      </c>
+      <c r="D153" s="4"/>
+      <c r="E153" s="4"/>
+      <c r="F153" s="4"/>
+      <c r="G153" s="4"/>
+      <c r="H153" s="4"/>
+    </row>
+    <row r="154" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B154" s="4">
+        <v>1216</v>
+      </c>
+      <c r="C154">
+        <v>44604</v>
+      </c>
+      <c r="D154" s="4"/>
+      <c r="E154" s="4"/>
+      <c r="F154" s="4"/>
+      <c r="G154" s="4"/>
+      <c r="H154" s="4"/>
+    </row>
+    <row r="155" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B155" s="4">
+        <v>1215</v>
+      </c>
+      <c r="C155">
+        <v>44602</v>
+      </c>
+      <c r="D155" s="4"/>
+      <c r="E155" s="4"/>
+      <c r="F155" s="4"/>
+      <c r="G155" s="4"/>
+      <c r="H155" s="4"/>
+    </row>
+    <row r="156" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B156" s="4">
+        <v>1214</v>
+      </c>
+      <c r="C156">
+        <v>44600</v>
+      </c>
+      <c r="D156" s="4"/>
+      <c r="E156" s="4"/>
+      <c r="F156" s="4"/>
+      <c r="G156" s="4"/>
+      <c r="H156" s="4"/>
+    </row>
+    <row r="157" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B157" s="4">
+        <v>1213</v>
+      </c>
+      <c r="C157">
+        <v>44597</v>
+      </c>
+      <c r="D157" s="4"/>
+      <c r="E157" s="4"/>
+      <c r="F157" s="4"/>
+      <c r="G157" s="4"/>
+      <c r="H157" s="4"/>
+    </row>
+    <row r="158" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B158" s="4">
+        <v>1212</v>
+      </c>
+      <c r="C158">
+        <v>44595</v>
+      </c>
+      <c r="D158" s="4"/>
+      <c r="E158" s="4"/>
+      <c r="F158" s="4"/>
+      <c r="G158" s="4"/>
+      <c r="H158" s="4"/>
+    </row>
+    <row r="159" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B159" s="4">
+        <v>1211</v>
+      </c>
+      <c r="C159">
+        <v>44593</v>
+      </c>
+      <c r="D159" s="4"/>
+      <c r="E159" s="4"/>
+      <c r="F159" s="4"/>
+      <c r="G159" s="4"/>
+      <c r="H159" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualziación Historial de Jugadas 09-01-2023
</commit_message>
<xml_diff>
--- a/helps/Historial de Jugadas.xlsx
+++ b/helps/Historial de Jugadas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Randon\helps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B53345-9A24-44E1-B824-57F08EF3C563}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE077B30-A10A-47D4-8366-920A36D74161}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{A3392D85-3030-46DE-B96E-7922EDC7109E}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1" xr2:uid="{A3392D85-3030-46DE-B96E-7922EDC7109E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tinka" sheetId="2" r:id="rId1"/>
@@ -558,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE65A1AE-D24F-426E-B6EF-7BC880E7680E}">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1190,8 +1190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15FEB743-8F41-4809-BA70-E7C1EBE37B84}">
   <dimension ref="A1:H159"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1303,8 +1303,12 @@
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="4"/>
-      <c r="C12" s="14"/>
+      <c r="B12" s="4">
+        <v>1358</v>
+      </c>
+      <c r="C12" s="14">
+        <v>44936</v>
+      </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -1312,8 +1316,12 @@
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="4"/>
-      <c r="C13" s="14"/>
+      <c r="B13" s="4">
+        <v>1357</v>
+      </c>
+      <c r="C13" s="14">
+        <v>44933</v>
+      </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -1321,8 +1329,12 @@
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="4"/>
-      <c r="C14" s="14"/>
+      <c r="B14" s="4">
+        <v>1356</v>
+      </c>
+      <c r="C14" s="14">
+        <v>44931</v>
+      </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -1330,8 +1342,12 @@
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="4"/>
-      <c r="C15" s="14"/>
+      <c r="B15" s="4">
+        <v>1355</v>
+      </c>
+      <c r="C15" s="14">
+        <v>44929</v>
+      </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>

</xml_diff>

<commit_message>
Actulización del excel CC - 19-01-2023
</commit_message>
<xml_diff>
--- a/helps/Historial de Jugadas.xlsx
+++ b/helps/Historial de Jugadas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20393"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Randon\helps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE077B30-A10A-47D4-8366-920A36D74161}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D98CB6-5A1C-47C5-806F-C533E79A6E24}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1" xr2:uid="{A3392D85-3030-46DE-B96E-7922EDC7109E}"/>
   </bookViews>
@@ -1190,8 +1190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15FEB743-8F41-4809-BA70-E7C1EBE37B84}">
   <dimension ref="A1:H159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1267,8 +1267,12 @@
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="4"/>
-      <c r="C8" s="14"/>
+      <c r="B8" s="4">
+        <v>1362</v>
+      </c>
+      <c r="C8" s="14">
+        <v>44945</v>
+      </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -1276,8 +1280,12 @@
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="4"/>
-      <c r="C9" s="14"/>
+      <c r="B9" s="4">
+        <v>1361</v>
+      </c>
+      <c r="C9" s="14">
+        <v>44943</v>
+      </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -1285,8 +1293,12 @@
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="4"/>
-      <c r="C10" s="14"/>
+      <c r="B10" s="4">
+        <v>1360</v>
+      </c>
+      <c r="C10" s="14">
+        <v>44940</v>
+      </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -1294,8 +1306,12 @@
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="4"/>
-      <c r="C11" s="14"/>
+      <c r="B11" s="4">
+        <v>1359</v>
+      </c>
+      <c r="C11" s="14">
+        <v>44938</v>
+      </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>

</xml_diff>

<commit_message>
Actualización del excel CC - 21-01-2023
</commit_message>
<xml_diff>
--- a/helps/Historial de Jugadas.xlsx
+++ b/helps/Historial de Jugadas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Randon\helps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D98CB6-5A1C-47C5-806F-C533E79A6E24}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CBCA313-6DB4-462A-A16E-06319543457E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1" xr2:uid="{A3392D85-3030-46DE-B96E-7922EDC7109E}"/>
   </bookViews>
@@ -1191,7 +1191,7 @@
   <dimension ref="A1:H159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1258,8 +1258,12 @@
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="4"/>
-      <c r="C7" s="14"/>
+      <c r="B7" s="4">
+        <v>1363</v>
+      </c>
+      <c r="C7" s="14">
+        <v>44947</v>
+      </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>

</xml_diff>

<commit_message>
Actualización del excel CC - 25-01-2023
</commit_message>
<xml_diff>
--- a/helps/Historial de Jugadas.xlsx
+++ b/helps/Historial de Jugadas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Randon\helps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CBCA313-6DB4-462A-A16E-06319543457E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6616974-60E6-411F-B56D-6FA97D03F58F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1" xr2:uid="{A3392D85-3030-46DE-B96E-7922EDC7109E}"/>
   </bookViews>
@@ -1188,10 +1188,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15FEB743-8F41-4809-BA70-E7C1EBE37B84}">
-  <dimension ref="A1:H159"/>
+  <dimension ref="A1:H161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1259,10 +1259,10 @@
     </row>
     <row r="7" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
-        <v>1363</v>
+        <v>1365</v>
       </c>
       <c r="C7" s="14">
-        <v>44947</v>
+        <v>44952</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
@@ -1272,10 +1272,10 @@
     </row>
     <row r="8" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
-        <v>1362</v>
+        <v>1364</v>
       </c>
       <c r="C8" s="14">
-        <v>44945</v>
+        <v>44950</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -1285,10 +1285,10 @@
     </row>
     <row r="9" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
-        <v>1361</v>
+        <v>1363</v>
       </c>
       <c r="C9" s="14">
-        <v>44943</v>
+        <v>44947</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -1298,10 +1298,10 @@
     </row>
     <row r="10" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
-        <v>1360</v>
+        <v>1362</v>
       </c>
       <c r="C10" s="14">
-        <v>44940</v>
+        <v>44945</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -1311,10 +1311,10 @@
     </row>
     <row r="11" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4">
-        <v>1359</v>
+        <v>1361</v>
       </c>
       <c r="C11" s="14">
-        <v>44938</v>
+        <v>44943</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -1324,10 +1324,10 @@
     </row>
     <row r="12" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
-        <v>1358</v>
+        <v>1360</v>
       </c>
       <c r="C12" s="14">
-        <v>44936</v>
+        <v>44940</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
@@ -1337,10 +1337,10 @@
     </row>
     <row r="13" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="4">
-        <v>1357</v>
+        <v>1359</v>
       </c>
       <c r="C13" s="14">
-        <v>44933</v>
+        <v>44938</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -1350,10 +1350,10 @@
     </row>
     <row r="14" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
-        <v>1356</v>
+        <v>1358</v>
       </c>
       <c r="C14" s="14">
-        <v>44931</v>
+        <v>44936</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
@@ -1363,10 +1363,10 @@
     </row>
     <row r="15" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="4">
-        <v>1355</v>
+        <v>1357</v>
       </c>
       <c r="C15" s="14">
-        <v>44929</v>
+        <v>44933</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -1376,10 +1376,10 @@
     </row>
     <row r="16" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="4">
-        <v>1354</v>
+        <v>1356</v>
       </c>
       <c r="C16" s="14">
-        <v>44926</v>
+        <v>44931</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
@@ -1389,10 +1389,10 @@
     </row>
     <row r="17" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="4">
-        <v>1353</v>
+        <v>1355</v>
       </c>
       <c r="C17" s="14">
-        <v>44924</v>
+        <v>44929</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -1402,10 +1402,10 @@
     </row>
     <row r="18" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="4">
-        <v>1352</v>
+        <v>1354</v>
       </c>
       <c r="C18" s="14">
-        <v>44922</v>
+        <v>44926</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
@@ -1415,10 +1415,10 @@
     </row>
     <row r="19" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="4">
-        <v>1351</v>
+        <v>1353</v>
       </c>
       <c r="C19" s="14">
-        <v>44919</v>
+        <v>44924</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
@@ -1428,10 +1428,10 @@
     </row>
     <row r="20" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="4">
-        <v>1350</v>
+        <v>1352</v>
       </c>
       <c r="C20" s="14">
-        <v>44917</v>
+        <v>44922</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
@@ -1441,10 +1441,10 @@
     </row>
     <row r="21" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="4">
-        <v>1349</v>
+        <v>1351</v>
       </c>
       <c r="C21" s="14">
-        <v>44915</v>
+        <v>44919</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
@@ -1454,10 +1454,10 @@
     </row>
     <row r="22" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="4">
-        <v>1348</v>
+        <v>1350</v>
       </c>
       <c r="C22" s="14">
-        <v>44912</v>
+        <v>44917</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
@@ -1467,10 +1467,10 @@
     </row>
     <row r="23" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="4">
-        <v>1347</v>
+        <v>1349</v>
       </c>
       <c r="C23" s="14">
-        <v>44910</v>
+        <v>44915</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
@@ -1480,10 +1480,10 @@
     </row>
     <row r="24" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="4">
-        <v>1346</v>
+        <v>1348</v>
       </c>
       <c r="C24" s="14">
-        <v>44908</v>
+        <v>44912</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
@@ -1493,10 +1493,10 @@
     </row>
     <row r="25" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="4">
-        <v>1345</v>
+        <v>1347</v>
       </c>
       <c r="C25" s="14">
-        <v>44905</v>
+        <v>44910</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
@@ -1506,10 +1506,10 @@
     </row>
     <row r="26" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="4">
-        <v>1344</v>
+        <v>1346</v>
       </c>
       <c r="C26" s="14">
-        <v>44903</v>
+        <v>44908</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
@@ -1519,10 +1519,10 @@
     </row>
     <row r="27" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="4">
-        <v>1343</v>
+        <v>1345</v>
       </c>
       <c r="C27" s="14">
-        <v>44901</v>
+        <v>44905</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
@@ -1532,10 +1532,10 @@
     </row>
     <row r="28" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="4">
-        <v>1342</v>
+        <v>1344</v>
       </c>
       <c r="C28" s="14">
-        <v>44898</v>
+        <v>44903</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
@@ -1545,10 +1545,10 @@
     </row>
     <row r="29" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="4">
-        <v>1341</v>
+        <v>1343</v>
       </c>
       <c r="C29" s="14">
-        <v>44896</v>
+        <v>44901</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -1558,10 +1558,10 @@
     </row>
     <row r="30" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="4">
-        <v>1340</v>
+        <v>1342</v>
       </c>
       <c r="C30" s="14">
-        <v>44894</v>
+        <v>44898</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
@@ -1571,10 +1571,10 @@
     </row>
     <row r="31" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="4">
-        <v>1339</v>
+        <v>1341</v>
       </c>
       <c r="C31" s="14">
-        <v>44891</v>
+        <v>44896</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -1584,12 +1584,12 @@
     </row>
     <row r="32" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="4">
-        <v>1338</v>
+        <v>1340</v>
       </c>
       <c r="C32" s="14">
-        <v>44889</v>
-      </c>
-      <c r="D32" s="14"/>
+        <v>44894</v>
+      </c>
+      <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
@@ -1597,10 +1597,10 @@
     </row>
     <row r="33" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="4">
-        <v>1337</v>
+        <v>1339</v>
       </c>
       <c r="C33" s="14">
-        <v>44887</v>
+        <v>44891</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
@@ -1610,12 +1610,12 @@
     </row>
     <row r="34" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="4">
-        <v>1336</v>
+        <v>1338</v>
       </c>
       <c r="C34" s="14">
-        <v>44884</v>
-      </c>
-      <c r="D34" s="4"/>
+        <v>44889</v>
+      </c>
+      <c r="D34" s="14"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
@@ -1623,10 +1623,10 @@
     </row>
     <row r="35" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="4">
-        <v>1335</v>
+        <v>1337</v>
       </c>
       <c r="C35" s="14">
-        <v>44882</v>
+        <v>44887</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -1636,10 +1636,10 @@
     </row>
     <row r="36" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="4">
-        <v>1334</v>
+        <v>1336</v>
       </c>
       <c r="C36" s="14">
-        <v>44880</v>
+        <v>44884</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -1649,10 +1649,10 @@
     </row>
     <row r="37" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="4">
-        <v>1333</v>
+        <v>1335</v>
       </c>
       <c r="C37" s="14">
-        <v>44877</v>
+        <v>44882</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -1662,10 +1662,10 @@
     </row>
     <row r="38" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="4">
-        <v>1332</v>
+        <v>1334</v>
       </c>
       <c r="C38" s="14">
-        <v>44875</v>
+        <v>44880</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
@@ -1675,10 +1675,10 @@
     </row>
     <row r="39" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="4">
-        <v>1331</v>
+        <v>1333</v>
       </c>
       <c r="C39" s="14">
-        <v>44873</v>
+        <v>44877</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
@@ -1688,10 +1688,10 @@
     </row>
     <row r="40" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="4">
-        <v>1330</v>
+        <v>1332</v>
       </c>
       <c r="C40" s="14">
-        <v>44870</v>
+        <v>44875</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
@@ -1701,10 +1701,10 @@
     </row>
     <row r="41" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="4">
-        <v>1329</v>
+        <v>1331</v>
       </c>
       <c r="C41" s="14">
-        <v>44868</v>
+        <v>44873</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
@@ -1714,10 +1714,10 @@
     </row>
     <row r="42" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="4">
-        <v>1328</v>
+        <v>1330</v>
       </c>
       <c r="C42" s="14">
-        <v>44866</v>
+        <v>44870</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
@@ -1727,10 +1727,10 @@
     </row>
     <row r="43" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="4">
-        <v>1327</v>
+        <v>1329</v>
       </c>
       <c r="C43" s="14">
-        <v>44863</v>
+        <v>44868</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
@@ -1740,10 +1740,10 @@
     </row>
     <row r="44" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="4">
-        <v>1326</v>
+        <v>1328</v>
       </c>
       <c r="C44" s="14">
-        <v>44861</v>
+        <v>44866</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -1753,10 +1753,10 @@
     </row>
     <row r="45" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="4">
-        <v>1325</v>
+        <v>1327</v>
       </c>
       <c r="C45" s="14">
-        <v>44859</v>
+        <v>44863</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
@@ -1766,10 +1766,10 @@
     </row>
     <row r="46" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="4">
-        <v>1324</v>
+        <v>1326</v>
       </c>
       <c r="C46" s="14">
-        <v>44856</v>
+        <v>44861</v>
       </c>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
@@ -1779,10 +1779,10 @@
     </row>
     <row r="47" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="4">
-        <v>1323</v>
+        <v>1325</v>
       </c>
       <c r="C47" s="14">
-        <v>44854</v>
+        <v>44859</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
@@ -1792,10 +1792,10 @@
     </row>
     <row r="48" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="4">
-        <v>1322</v>
+        <v>1324</v>
       </c>
       <c r="C48" s="14">
-        <v>44852</v>
+        <v>44856</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
@@ -1805,10 +1805,10 @@
     </row>
     <row r="49" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="4">
-        <v>1321</v>
+        <v>1323</v>
       </c>
       <c r="C49" s="14">
-        <v>44849</v>
+        <v>44854</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
@@ -1818,10 +1818,10 @@
     </row>
     <row r="50" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="4">
-        <v>1320</v>
+        <v>1322</v>
       </c>
       <c r="C50" s="14">
-        <v>44847</v>
+        <v>44852</v>
       </c>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
@@ -1831,10 +1831,10 @@
     </row>
     <row r="51" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="4">
-        <v>1319</v>
+        <v>1321</v>
       </c>
       <c r="C51" s="14">
-        <v>44845</v>
+        <v>44849</v>
       </c>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
@@ -1844,10 +1844,10 @@
     </row>
     <row r="52" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="4">
-        <v>1318</v>
+        <v>1320</v>
       </c>
       <c r="C52" s="14">
-        <v>44842</v>
+        <v>44847</v>
       </c>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
@@ -1857,10 +1857,10 @@
     </row>
     <row r="53" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="4">
-        <v>1317</v>
+        <v>1319</v>
       </c>
       <c r="C53" s="14">
-        <v>44840</v>
+        <v>44845</v>
       </c>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
@@ -1870,10 +1870,10 @@
     </row>
     <row r="54" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="4">
-        <v>1316</v>
+        <v>1318</v>
       </c>
       <c r="C54" s="14">
-        <v>44838</v>
+        <v>44842</v>
       </c>
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
@@ -1883,10 +1883,10 @@
     </row>
     <row r="55" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="4">
-        <v>1315</v>
+        <v>1317</v>
       </c>
       <c r="C55" s="14">
-        <v>44835</v>
+        <v>44840</v>
       </c>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
@@ -1896,10 +1896,10 @@
     </row>
     <row r="56" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="4">
-        <v>1314</v>
+        <v>1316</v>
       </c>
       <c r="C56" s="14">
-        <v>44833</v>
+        <v>44838</v>
       </c>
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
@@ -1909,10 +1909,10 @@
     </row>
     <row r="57" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="4">
-        <v>1313</v>
+        <v>1315</v>
       </c>
       <c r="C57" s="14">
-        <v>44831</v>
+        <v>44835</v>
       </c>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
@@ -1922,10 +1922,10 @@
     </row>
     <row r="58" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="4">
-        <v>1312</v>
+        <v>1314</v>
       </c>
       <c r="C58" s="14">
-        <v>44828</v>
+        <v>44833</v>
       </c>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
@@ -1935,10 +1935,10 @@
     </row>
     <row r="59" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="4">
-        <v>1311</v>
+        <v>1313</v>
       </c>
       <c r="C59" s="14">
-        <v>44826</v>
+        <v>44831</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
@@ -1948,10 +1948,10 @@
     </row>
     <row r="60" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B60" s="4">
-        <v>1310</v>
+        <v>1312</v>
       </c>
       <c r="C60" s="14">
-        <v>44824</v>
+        <v>44828</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
@@ -1961,10 +1961,10 @@
     </row>
     <row r="61" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B61" s="4">
-        <v>1309</v>
+        <v>1311</v>
       </c>
       <c r="C61" s="14">
-        <v>44821</v>
+        <v>44826</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
@@ -1974,10 +1974,10 @@
     </row>
     <row r="62" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B62" s="4">
-        <v>1308</v>
+        <v>1310</v>
       </c>
       <c r="C62" s="14">
-        <v>44819</v>
+        <v>44824</v>
       </c>
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
@@ -1987,10 +1987,10 @@
     </row>
     <row r="63" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="4">
-        <v>1307</v>
+        <v>1309</v>
       </c>
       <c r="C63" s="14">
-        <v>44817</v>
+        <v>44821</v>
       </c>
       <c r="D63" s="4"/>
       <c r="E63" s="4"/>
@@ -2000,10 +2000,10 @@
     </row>
     <row r="64" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B64" s="4">
-        <v>1306</v>
+        <v>1308</v>
       </c>
       <c r="C64" s="14">
-        <v>44814</v>
+        <v>44819</v>
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="4"/>
@@ -2013,10 +2013,10 @@
     </row>
     <row r="65" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B65" s="4">
-        <v>1305</v>
+        <v>1307</v>
       </c>
       <c r="C65" s="14">
-        <v>44812</v>
+        <v>44817</v>
       </c>
       <c r="D65" s="4"/>
       <c r="E65" s="4"/>
@@ -2026,10 +2026,10 @@
     </row>
     <row r="66" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B66" s="4">
-        <v>1304</v>
+        <v>1306</v>
       </c>
       <c r="C66" s="14">
-        <v>44810</v>
+        <v>44814</v>
       </c>
       <c r="D66" s="4"/>
       <c r="E66" s="4"/>
@@ -2039,10 +2039,10 @@
     </row>
     <row r="67" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B67" s="4">
-        <v>1303</v>
+        <v>1305</v>
       </c>
       <c r="C67" s="14">
-        <v>44807</v>
+        <v>44812</v>
       </c>
       <c r="D67" s="4"/>
       <c r="E67" s="4"/>
@@ -2052,10 +2052,10 @@
     </row>
     <row r="68" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="4">
-        <v>1302</v>
+        <v>1304</v>
       </c>
       <c r="C68" s="14">
-        <v>44805</v>
+        <v>44810</v>
       </c>
       <c r="D68" s="4"/>
       <c r="E68" s="4"/>
@@ -2065,10 +2065,10 @@
     </row>
     <row r="69" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B69" s="4">
-        <v>1301</v>
+        <v>1303</v>
       </c>
       <c r="C69" s="14">
-        <v>44803</v>
+        <v>44807</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69" s="4"/>
@@ -2078,10 +2078,10 @@
     </row>
     <row r="70" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B70" s="4">
-        <v>1300</v>
+        <v>1302</v>
       </c>
       <c r="C70" s="14">
-        <v>44800</v>
+        <v>44805</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="4"/>
@@ -2091,10 +2091,10 @@
     </row>
     <row r="71" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B71" s="4">
-        <v>1299</v>
+        <v>1301</v>
       </c>
       <c r="C71" s="14">
-        <v>44798</v>
+        <v>44803</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" s="4"/>
@@ -2104,10 +2104,10 @@
     </row>
     <row r="72" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B72" s="4">
-        <v>1298</v>
+        <v>1300</v>
       </c>
       <c r="C72" s="14">
-        <v>44796</v>
+        <v>44800</v>
       </c>
       <c r="D72" s="4"/>
       <c r="E72" s="4"/>
@@ -2117,10 +2117,10 @@
     </row>
     <row r="73" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B73" s="4">
-        <v>1297</v>
+        <v>1299</v>
       </c>
       <c r="C73" s="14">
-        <v>44793</v>
+        <v>44798</v>
       </c>
       <c r="D73" s="4"/>
       <c r="E73" s="4"/>
@@ -2130,10 +2130,10 @@
     </row>
     <row r="74" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B74" s="4">
-        <v>1296</v>
+        <v>1298</v>
       </c>
       <c r="C74" s="14">
-        <v>44791</v>
+        <v>44796</v>
       </c>
       <c r="D74" s="4"/>
       <c r="E74" s="4"/>
@@ -2143,10 +2143,10 @@
     </row>
     <row r="75" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B75" s="4">
-        <v>1295</v>
+        <v>1297</v>
       </c>
       <c r="C75" s="14">
-        <v>44789</v>
+        <v>44793</v>
       </c>
       <c r="D75" s="4"/>
       <c r="E75" s="4"/>
@@ -2156,10 +2156,10 @@
     </row>
     <row r="76" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B76" s="4">
-        <v>1294</v>
+        <v>1296</v>
       </c>
       <c r="C76" s="14">
-        <v>44786</v>
+        <v>44791</v>
       </c>
       <c r="D76" s="4"/>
       <c r="E76" s="4"/>
@@ -2169,10 +2169,10 @@
     </row>
     <row r="77" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B77" s="4">
-        <v>1293</v>
+        <v>1295</v>
       </c>
       <c r="C77" s="14">
-        <v>44784</v>
+        <v>44789</v>
       </c>
       <c r="D77" s="4"/>
       <c r="E77" s="4"/>
@@ -2182,10 +2182,10 @@
     </row>
     <row r="78" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="4">
-        <v>1292</v>
+        <v>1294</v>
       </c>
       <c r="C78" s="14">
-        <v>44782</v>
+        <v>44786</v>
       </c>
       <c r="D78" s="4"/>
       <c r="E78" s="4"/>
@@ -2195,10 +2195,10 @@
     </row>
     <row r="79" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B79" s="4">
-        <v>1291</v>
+        <v>1293</v>
       </c>
       <c r="C79" s="14">
-        <v>44779</v>
+        <v>44784</v>
       </c>
       <c r="D79" s="4"/>
       <c r="E79" s="4"/>
@@ -2208,10 +2208,10 @@
     </row>
     <row r="80" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B80" s="4">
-        <v>1290</v>
+        <v>1292</v>
       </c>
       <c r="C80" s="14">
-        <v>44777</v>
+        <v>44782</v>
       </c>
       <c r="D80" s="4"/>
       <c r="E80" s="4"/>
@@ -2221,10 +2221,10 @@
     </row>
     <row r="81" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B81" s="4">
-        <v>1289</v>
+        <v>1291</v>
       </c>
       <c r="C81" s="14">
-        <v>44775</v>
+        <v>44779</v>
       </c>
       <c r="D81" s="4"/>
       <c r="E81" s="4"/>
@@ -2234,10 +2234,10 @@
     </row>
     <row r="82" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B82" s="4">
-        <v>1288</v>
+        <v>1290</v>
       </c>
       <c r="C82" s="14">
-        <v>44772</v>
+        <v>44777</v>
       </c>
       <c r="D82" s="4"/>
       <c r="E82" s="4"/>
@@ -2247,10 +2247,10 @@
     </row>
     <row r="83" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B83" s="4">
-        <v>1287</v>
+        <v>1289</v>
       </c>
       <c r="C83" s="14">
-        <v>44770</v>
+        <v>44775</v>
       </c>
       <c r="D83" s="4"/>
       <c r="E83" s="4"/>
@@ -2260,10 +2260,10 @@
     </row>
     <row r="84" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B84" s="4">
-        <v>1286</v>
+        <v>1288</v>
       </c>
       <c r="C84" s="14">
-        <v>44768</v>
+        <v>44772</v>
       </c>
       <c r="D84" s="4"/>
       <c r="E84" s="4"/>
@@ -2273,10 +2273,10 @@
     </row>
     <row r="85" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B85" s="4">
-        <v>1285</v>
+        <v>1287</v>
       </c>
       <c r="C85" s="14">
-        <v>44765</v>
+        <v>44770</v>
       </c>
       <c r="D85" s="4"/>
       <c r="E85" s="4"/>
@@ -2286,10 +2286,10 @@
     </row>
     <row r="86" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B86" s="4">
-        <v>1284</v>
+        <v>1286</v>
       </c>
       <c r="C86" s="14">
-        <v>44763</v>
+        <v>44768</v>
       </c>
       <c r="D86" s="4"/>
       <c r="E86" s="4"/>
@@ -2299,10 +2299,10 @@
     </row>
     <row r="87" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B87" s="4">
-        <v>1283</v>
+        <v>1285</v>
       </c>
       <c r="C87" s="14">
-        <v>44761</v>
+        <v>44765</v>
       </c>
       <c r="D87" s="4"/>
       <c r="E87" s="4"/>
@@ -2312,10 +2312,10 @@
     </row>
     <row r="88" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B88" s="4">
-        <v>1282</v>
+        <v>1284</v>
       </c>
       <c r="C88" s="14">
-        <v>44758</v>
+        <v>44763</v>
       </c>
       <c r="D88" s="4"/>
       <c r="E88" s="4"/>
@@ -2325,10 +2325,10 @@
     </row>
     <row r="89" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B89" s="4">
-        <v>1281</v>
+        <v>1283</v>
       </c>
       <c r="C89" s="14">
-        <v>44756</v>
+        <v>44761</v>
       </c>
       <c r="D89" s="4"/>
       <c r="E89" s="4"/>
@@ -2338,10 +2338,10 @@
     </row>
     <row r="90" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B90" s="4">
-        <v>1280</v>
+        <v>1282</v>
       </c>
       <c r="C90" s="14">
-        <v>44754</v>
+        <v>44758</v>
       </c>
       <c r="D90" s="4"/>
       <c r="E90" s="4"/>
@@ -2351,10 +2351,10 @@
     </row>
     <row r="91" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B91" s="4">
-        <v>1279</v>
+        <v>1281</v>
       </c>
       <c r="C91" s="14">
-        <v>44751</v>
+        <v>44756</v>
       </c>
       <c r="D91" s="4"/>
       <c r="E91" s="4"/>
@@ -2364,10 +2364,10 @@
     </row>
     <row r="92" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B92" s="4">
-        <v>1278</v>
+        <v>1280</v>
       </c>
       <c r="C92" s="14">
-        <v>44749</v>
+        <v>44754</v>
       </c>
       <c r="D92" s="4"/>
       <c r="E92" s="4"/>
@@ -2377,10 +2377,10 @@
     </row>
     <row r="93" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B93" s="4">
-        <v>1277</v>
+        <v>1279</v>
       </c>
       <c r="C93" s="14">
-        <v>44747</v>
+        <v>44751</v>
       </c>
       <c r="D93" s="4"/>
       <c r="E93" s="4"/>
@@ -2390,10 +2390,10 @@
     </row>
     <row r="94" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B94" s="4">
-        <v>1276</v>
+        <v>1278</v>
       </c>
       <c r="C94" s="14">
-        <v>44744</v>
+        <v>44749</v>
       </c>
       <c r="D94" s="4"/>
       <c r="E94" s="4"/>
@@ -2403,10 +2403,10 @@
     </row>
     <row r="95" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B95" s="4">
-        <v>1275</v>
+        <v>1277</v>
       </c>
       <c r="C95" s="14">
-        <v>44742</v>
+        <v>44747</v>
       </c>
       <c r="D95" s="4"/>
       <c r="E95" s="4"/>
@@ -2416,10 +2416,10 @@
     </row>
     <row r="96" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B96" s="4">
-        <v>1274</v>
+        <v>1276</v>
       </c>
       <c r="C96" s="14">
-        <v>44740</v>
+        <v>44744</v>
       </c>
       <c r="D96" s="4"/>
       <c r="E96" s="4"/>
@@ -2429,10 +2429,10 @@
     </row>
     <row r="97" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B97" s="4">
-        <v>1273</v>
+        <v>1275</v>
       </c>
       <c r="C97" s="14">
-        <v>44737</v>
+        <v>44742</v>
       </c>
       <c r="D97" s="4"/>
       <c r="E97" s="4"/>
@@ -2442,10 +2442,10 @@
     </row>
     <row r="98" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B98" s="4">
-        <v>1272</v>
+        <v>1274</v>
       </c>
       <c r="C98" s="14">
-        <v>44735</v>
+        <v>44740</v>
       </c>
       <c r="D98" s="4"/>
       <c r="E98" s="4"/>
@@ -2455,10 +2455,10 @@
     </row>
     <row r="99" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B99" s="4">
-        <v>1271</v>
+        <v>1273</v>
       </c>
       <c r="C99" s="14">
-        <v>44733</v>
+        <v>44737</v>
       </c>
       <c r="D99" s="4"/>
       <c r="E99" s="4"/>
@@ -2468,10 +2468,10 @@
     </row>
     <row r="100" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B100" s="4">
-        <v>1270</v>
+        <v>1272</v>
       </c>
       <c r="C100" s="14">
-        <v>44730</v>
+        <v>44735</v>
       </c>
       <c r="D100" s="4"/>
       <c r="E100" s="4"/>
@@ -2481,10 +2481,10 @@
     </row>
     <row r="101" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B101" s="4">
-        <v>1269</v>
+        <v>1271</v>
       </c>
       <c r="C101" s="14">
-        <v>44728</v>
+        <v>44733</v>
       </c>
       <c r="D101" s="4"/>
       <c r="E101" s="4"/>
@@ -2494,10 +2494,10 @@
     </row>
     <row r="102" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B102" s="4">
-        <v>1268</v>
+        <v>1270</v>
       </c>
       <c r="C102" s="14">
-        <v>44726</v>
+        <v>44730</v>
       </c>
       <c r="D102" s="4"/>
       <c r="E102" s="4"/>
@@ -2507,10 +2507,10 @@
     </row>
     <row r="103" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B103" s="4">
-        <v>1267</v>
+        <v>1269</v>
       </c>
       <c r="C103" s="14">
-        <v>44723</v>
+        <v>44728</v>
       </c>
       <c r="D103" s="4"/>
       <c r="E103" s="4"/>
@@ -2520,10 +2520,10 @@
     </row>
     <row r="104" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B104" s="4">
-        <v>1266</v>
+        <v>1268</v>
       </c>
       <c r="C104" s="14">
-        <v>44721</v>
+        <v>44726</v>
       </c>
       <c r="D104" s="4"/>
       <c r="E104" s="4"/>
@@ -2533,10 +2533,10 @@
     </row>
     <row r="105" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B105" s="4">
-        <v>1265</v>
+        <v>1267</v>
       </c>
       <c r="C105" s="14">
-        <v>44719</v>
+        <v>44723</v>
       </c>
       <c r="D105" s="4"/>
       <c r="E105" s="4"/>
@@ -2546,10 +2546,10 @@
     </row>
     <row r="106" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B106" s="4">
-        <v>1264</v>
+        <v>1266</v>
       </c>
       <c r="C106" s="14">
-        <v>44716</v>
+        <v>44721</v>
       </c>
       <c r="D106" s="4"/>
       <c r="E106" s="4"/>
@@ -2559,10 +2559,10 @@
     </row>
     <row r="107" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B107" s="4">
-        <v>1263</v>
+        <v>1265</v>
       </c>
       <c r="C107" s="14">
-        <v>44714</v>
+        <v>44719</v>
       </c>
       <c r="D107" s="4"/>
       <c r="E107" s="4"/>
@@ -2572,10 +2572,10 @@
     </row>
     <row r="108" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B108" s="4">
-        <v>1262</v>
+        <v>1264</v>
       </c>
       <c r="C108" s="14">
-        <v>44712</v>
+        <v>44716</v>
       </c>
       <c r="D108" s="4"/>
       <c r="E108" s="4"/>
@@ -2585,10 +2585,10 @@
     </row>
     <row r="109" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B109" s="4">
-        <v>1261</v>
+        <v>1263</v>
       </c>
       <c r="C109" s="14">
-        <v>44709</v>
+        <v>44714</v>
       </c>
       <c r="D109" s="4"/>
       <c r="E109" s="4"/>
@@ -2598,10 +2598,10 @@
     </row>
     <row r="110" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B110" s="4">
-        <v>1260</v>
+        <v>1262</v>
       </c>
       <c r="C110" s="14">
-        <v>44707</v>
+        <v>44712</v>
       </c>
       <c r="D110" s="4"/>
       <c r="E110" s="4"/>
@@ -2611,10 +2611,10 @@
     </row>
     <row r="111" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B111" s="4">
-        <v>1259</v>
+        <v>1261</v>
       </c>
       <c r="C111" s="14">
-        <v>44705</v>
+        <v>44709</v>
       </c>
       <c r="D111" s="4"/>
       <c r="E111" s="4"/>
@@ -2624,10 +2624,10 @@
     </row>
     <row r="112" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B112" s="4">
-        <v>1258</v>
+        <v>1260</v>
       </c>
       <c r="C112" s="14">
-        <v>44702</v>
+        <v>44707</v>
       </c>
       <c r="D112" s="4"/>
       <c r="E112" s="4"/>
@@ -2637,10 +2637,10 @@
     </row>
     <row r="113" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B113" s="4">
-        <v>1257</v>
+        <v>1259</v>
       </c>
       <c r="C113" s="14">
-        <v>44700</v>
+        <v>44705</v>
       </c>
       <c r="D113" s="4"/>
       <c r="E113" s="4"/>
@@ -2650,10 +2650,10 @@
     </row>
     <row r="114" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B114" s="4">
-        <v>1256</v>
+        <v>1258</v>
       </c>
       <c r="C114" s="14">
-        <v>44698</v>
+        <v>44702</v>
       </c>
       <c r="D114" s="4"/>
       <c r="E114" s="4"/>
@@ -2663,10 +2663,10 @@
     </row>
     <row r="115" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B115" s="4">
-        <v>1255</v>
+        <v>1257</v>
       </c>
       <c r="C115" s="14">
-        <v>44695</v>
+        <v>44700</v>
       </c>
       <c r="D115" s="4"/>
       <c r="E115" s="4"/>
@@ -2676,10 +2676,10 @@
     </row>
     <row r="116" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B116" s="4">
-        <v>1254</v>
+        <v>1256</v>
       </c>
       <c r="C116" s="14">
-        <v>44693</v>
+        <v>44698</v>
       </c>
       <c r="D116" s="4"/>
       <c r="E116" s="4"/>
@@ -2689,10 +2689,10 @@
     </row>
     <row r="117" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B117" s="4">
-        <v>1253</v>
+        <v>1255</v>
       </c>
       <c r="C117" s="14">
-        <v>44691</v>
+        <v>44695</v>
       </c>
       <c r="D117" s="4"/>
       <c r="E117" s="4"/>
@@ -2702,10 +2702,10 @@
     </row>
     <row r="118" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B118" s="4">
-        <v>1252</v>
+        <v>1254</v>
       </c>
       <c r="C118" s="14">
-        <v>44688</v>
+        <v>44693</v>
       </c>
       <c r="D118" s="4"/>
       <c r="E118" s="4"/>
@@ -2715,10 +2715,10 @@
     </row>
     <row r="119" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B119" s="4">
-        <v>1251</v>
+        <v>1253</v>
       </c>
       <c r="C119" s="14">
-        <v>44686</v>
+        <v>44691</v>
       </c>
       <c r="D119" s="4"/>
       <c r="E119" s="4"/>
@@ -2728,10 +2728,10 @@
     </row>
     <row r="120" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B120" s="4">
-        <v>1250</v>
+        <v>1252</v>
       </c>
       <c r="C120" s="14">
-        <v>44684</v>
+        <v>44688</v>
       </c>
       <c r="D120" s="4"/>
       <c r="E120" s="4"/>
@@ -2741,10 +2741,10 @@
     </row>
     <row r="121" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B121" s="4">
-        <v>1249</v>
+        <v>1251</v>
       </c>
       <c r="C121" s="14">
-        <v>44681</v>
+        <v>44686</v>
       </c>
       <c r="D121" s="4"/>
       <c r="E121" s="4"/>
@@ -2754,10 +2754,10 @@
     </row>
     <row r="122" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B122" s="4">
-        <v>1248</v>
+        <v>1250</v>
       </c>
       <c r="C122" s="14">
-        <v>44679</v>
+        <v>44684</v>
       </c>
       <c r="D122" s="4"/>
       <c r="E122" s="4"/>
@@ -2767,10 +2767,10 @@
     </row>
     <row r="123" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B123" s="4">
-        <v>1247</v>
+        <v>1249</v>
       </c>
       <c r="C123" s="14">
-        <v>44677</v>
+        <v>44681</v>
       </c>
       <c r="D123" s="4"/>
       <c r="E123" s="4"/>
@@ -2780,10 +2780,10 @@
     </row>
     <row r="124" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B124" s="4">
-        <v>1246</v>
+        <v>1248</v>
       </c>
       <c r="C124" s="14">
-        <v>44674</v>
+        <v>44679</v>
       </c>
       <c r="D124" s="4"/>
       <c r="E124" s="4"/>
@@ -2793,10 +2793,10 @@
     </row>
     <row r="125" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B125" s="4">
-        <v>1245</v>
+        <v>1247</v>
       </c>
       <c r="C125" s="14">
-        <v>44672</v>
+        <v>44677</v>
       </c>
       <c r="D125" s="4"/>
       <c r="E125" s="4"/>
@@ -2806,10 +2806,10 @@
     </row>
     <row r="126" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B126" s="4">
-        <v>1244</v>
+        <v>1246</v>
       </c>
       <c r="C126" s="14">
-        <v>44670</v>
+        <v>44674</v>
       </c>
       <c r="D126" s="4"/>
       <c r="E126" s="4"/>
@@ -2819,10 +2819,10 @@
     </row>
     <row r="127" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B127" s="4">
-        <v>1243</v>
+        <v>1245</v>
       </c>
       <c r="C127" s="14">
-        <v>44667</v>
+        <v>44672</v>
       </c>
       <c r="D127" s="4"/>
       <c r="E127" s="4"/>
@@ -2832,10 +2832,10 @@
     </row>
     <row r="128" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B128" s="4">
-        <v>1242</v>
+        <v>1244</v>
       </c>
       <c r="C128" s="14">
-        <v>44665</v>
+        <v>44670</v>
       </c>
       <c r="D128" s="4"/>
       <c r="E128" s="4"/>
@@ -2845,10 +2845,10 @@
     </row>
     <row r="129" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B129" s="4">
-        <v>1241</v>
+        <v>1243</v>
       </c>
       <c r="C129" s="14">
-        <v>44663</v>
+        <v>44667</v>
       </c>
       <c r="D129" s="4"/>
       <c r="E129" s="4"/>
@@ -2858,10 +2858,10 @@
     </row>
     <row r="130" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B130" s="4">
-        <v>1240</v>
+        <v>1242</v>
       </c>
       <c r="C130" s="14">
-        <v>44660</v>
+        <v>44665</v>
       </c>
       <c r="D130" s="4"/>
       <c r="E130" s="4"/>
@@ -2871,10 +2871,10 @@
     </row>
     <row r="131" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B131" s="4">
-        <v>1239</v>
+        <v>1241</v>
       </c>
       <c r="C131" s="14">
-        <v>44658</v>
+        <v>44663</v>
       </c>
       <c r="D131" s="4"/>
       <c r="E131" s="4"/>
@@ -2884,10 +2884,10 @@
     </row>
     <row r="132" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B132" s="4">
-        <v>1238</v>
+        <v>1240</v>
       </c>
       <c r="C132" s="14">
-        <v>44656</v>
+        <v>44660</v>
       </c>
       <c r="D132" s="4"/>
       <c r="E132" s="4"/>
@@ -2897,10 +2897,10 @@
     </row>
     <row r="133" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B133" s="4">
-        <v>1237</v>
+        <v>1239</v>
       </c>
       <c r="C133" s="14">
-        <v>44653</v>
+        <v>44658</v>
       </c>
       <c r="D133" s="4"/>
       <c r="E133" s="4"/>
@@ -2910,10 +2910,10 @@
     </row>
     <row r="134" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B134" s="4">
-        <v>1236</v>
+        <v>1238</v>
       </c>
       <c r="C134" s="14">
-        <v>44651</v>
+        <v>44656</v>
       </c>
       <c r="D134" s="4"/>
       <c r="E134" s="4"/>
@@ -2923,10 +2923,10 @@
     </row>
     <row r="135" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B135" s="4">
-        <v>1235</v>
+        <v>1237</v>
       </c>
       <c r="C135" s="14">
-        <v>44649</v>
+        <v>44653</v>
       </c>
       <c r="D135" s="4"/>
       <c r="E135" s="4"/>
@@ -2936,10 +2936,10 @@
     </row>
     <row r="136" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B136" s="4">
-        <v>1234</v>
+        <v>1236</v>
       </c>
       <c r="C136" s="14">
-        <v>44646</v>
+        <v>44651</v>
       </c>
       <c r="D136" s="4"/>
       <c r="E136" s="4"/>
@@ -2949,10 +2949,10 @@
     </row>
     <row r="137" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B137" s="4">
-        <v>1233</v>
+        <v>1235</v>
       </c>
       <c r="C137" s="14">
-        <v>44644</v>
+        <v>44649</v>
       </c>
       <c r="D137" s="4"/>
       <c r="E137" s="4"/>
@@ -2962,10 +2962,10 @@
     </row>
     <row r="138" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B138" s="4">
-        <v>1232</v>
+        <v>1234</v>
       </c>
       <c r="C138" s="14">
-        <v>44642</v>
+        <v>44646</v>
       </c>
       <c r="D138" s="4"/>
       <c r="E138" s="4"/>
@@ -2975,10 +2975,10 @@
     </row>
     <row r="139" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B139" s="4">
-        <v>1231</v>
+        <v>1233</v>
       </c>
       <c r="C139" s="14">
-        <v>44639</v>
+        <v>44644</v>
       </c>
       <c r="D139" s="4"/>
       <c r="E139" s="4"/>
@@ -2988,10 +2988,10 @@
     </row>
     <row r="140" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B140" s="4">
-        <v>1230</v>
+        <v>1232</v>
       </c>
       <c r="C140" s="14">
-        <v>44637</v>
+        <v>44642</v>
       </c>
       <c r="D140" s="4"/>
       <c r="E140" s="4"/>
@@ -3001,10 +3001,10 @@
     </row>
     <row r="141" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B141" s="4">
-        <v>1229</v>
+        <v>1231</v>
       </c>
       <c r="C141" s="14">
-        <v>44635</v>
+        <v>44639</v>
       </c>
       <c r="D141" s="4"/>
       <c r="E141" s="4"/>
@@ -3014,10 +3014,10 @@
     </row>
     <row r="142" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B142" s="4">
-        <v>1228</v>
-      </c>
-      <c r="C142">
-        <v>44632</v>
+        <v>1230</v>
+      </c>
+      <c r="C142" s="14">
+        <v>44637</v>
       </c>
       <c r="D142" s="4"/>
       <c r="E142" s="4"/>
@@ -3027,10 +3027,10 @@
     </row>
     <row r="143" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B143" s="4">
-        <v>1227</v>
-      </c>
-      <c r="C143">
-        <v>44630</v>
+        <v>1229</v>
+      </c>
+      <c r="C143" s="14">
+        <v>44635</v>
       </c>
       <c r="D143" s="4"/>
       <c r="E143" s="4"/>
@@ -3040,10 +3040,10 @@
     </row>
     <row r="144" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B144" s="4">
-        <v>1226</v>
+        <v>1228</v>
       </c>
       <c r="C144">
-        <v>44628</v>
+        <v>44632</v>
       </c>
       <c r="D144" s="4"/>
       <c r="E144" s="4"/>
@@ -3053,10 +3053,10 @@
     </row>
     <row r="145" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B145" s="4">
-        <v>1225</v>
+        <v>1227</v>
       </c>
       <c r="C145">
-        <v>44625</v>
+        <v>44630</v>
       </c>
       <c r="D145" s="4"/>
       <c r="E145" s="4"/>
@@ -3066,10 +3066,10 @@
     </row>
     <row r="146" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B146" s="4">
-        <v>1224</v>
+        <v>1226</v>
       </c>
       <c r="C146">
-        <v>44623</v>
+        <v>44628</v>
       </c>
       <c r="D146" s="4"/>
       <c r="E146" s="4"/>
@@ -3079,10 +3079,10 @@
     </row>
     <row r="147" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B147" s="4">
-        <v>1223</v>
+        <v>1225</v>
       </c>
       <c r="C147">
-        <v>44621</v>
+        <v>44625</v>
       </c>
       <c r="D147" s="4"/>
       <c r="E147" s="4"/>
@@ -3092,10 +3092,10 @@
     </row>
     <row r="148" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B148" s="4">
-        <v>1222</v>
+        <v>1224</v>
       </c>
       <c r="C148">
-        <v>44618</v>
+        <v>44623</v>
       </c>
       <c r="D148" s="4"/>
       <c r="E148" s="4"/>
@@ -3105,10 +3105,10 @@
     </row>
     <row r="149" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B149" s="4">
-        <v>1221</v>
+        <v>1223</v>
       </c>
       <c r="C149">
-        <v>44616</v>
+        <v>44621</v>
       </c>
       <c r="D149" s="4"/>
       <c r="E149" s="4"/>
@@ -3118,10 +3118,10 @@
     </row>
     <row r="150" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B150" s="4">
-        <v>1220</v>
+        <v>1222</v>
       </c>
       <c r="C150">
-        <v>44614</v>
+        <v>44618</v>
       </c>
       <c r="D150" s="4"/>
       <c r="E150" s="4"/>
@@ -3131,10 +3131,10 @@
     </row>
     <row r="151" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B151" s="4">
-        <v>1219</v>
+        <v>1221</v>
       </c>
       <c r="C151">
-        <v>44611</v>
+        <v>44616</v>
       </c>
       <c r="D151" s="4"/>
       <c r="E151" s="4"/>
@@ -3144,10 +3144,10 @@
     </row>
     <row r="152" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B152" s="4">
-        <v>1218</v>
+        <v>1220</v>
       </c>
       <c r="C152">
-        <v>44609</v>
+        <v>44614</v>
       </c>
       <c r="D152" s="4"/>
       <c r="E152" s="4"/>
@@ -3157,10 +3157,10 @@
     </row>
     <row r="153" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B153" s="4">
-        <v>1217</v>
+        <v>1219</v>
       </c>
       <c r="C153">
-        <v>44607</v>
+        <v>44611</v>
       </c>
       <c r="D153" s="4"/>
       <c r="E153" s="4"/>
@@ -3170,10 +3170,10 @@
     </row>
     <row r="154" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B154" s="4">
-        <v>1216</v>
+        <v>1218</v>
       </c>
       <c r="C154">
-        <v>44604</v>
+        <v>44609</v>
       </c>
       <c r="D154" s="4"/>
       <c r="E154" s="4"/>
@@ -3183,10 +3183,10 @@
     </row>
     <row r="155" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B155" s="4">
-        <v>1215</v>
+        <v>1217</v>
       </c>
       <c r="C155">
-        <v>44602</v>
+        <v>44607</v>
       </c>
       <c r="D155" s="4"/>
       <c r="E155" s="4"/>
@@ -3196,10 +3196,10 @@
     </row>
     <row r="156" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B156" s="4">
-        <v>1214</v>
+        <v>1216</v>
       </c>
       <c r="C156">
-        <v>44600</v>
+        <v>44604</v>
       </c>
       <c r="D156" s="4"/>
       <c r="E156" s="4"/>
@@ -3209,10 +3209,10 @@
     </row>
     <row r="157" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B157" s="4">
-        <v>1213</v>
+        <v>1215</v>
       </c>
       <c r="C157">
-        <v>44597</v>
+        <v>44602</v>
       </c>
       <c r="D157" s="4"/>
       <c r="E157" s="4"/>
@@ -3222,10 +3222,10 @@
     </row>
     <row r="158" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B158" s="4">
-        <v>1212</v>
+        <v>1214</v>
       </c>
       <c r="C158">
-        <v>44595</v>
+        <v>44600</v>
       </c>
       <c r="D158" s="4"/>
       <c r="E158" s="4"/>
@@ -3235,10 +3235,10 @@
     </row>
     <row r="159" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B159" s="4">
-        <v>1211</v>
+        <v>1213</v>
       </c>
       <c r="C159">
-        <v>44593</v>
+        <v>44597</v>
       </c>
       <c r="D159" s="4"/>
       <c r="E159" s="4"/>
@@ -3246,6 +3246,32 @@
       <c r="G159" s="4"/>
       <c r="H159" s="4"/>
     </row>
+    <row r="160" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B160" s="4">
+        <v>1212</v>
+      </c>
+      <c r="C160">
+        <v>44595</v>
+      </c>
+      <c r="D160" s="4"/>
+      <c r="E160" s="4"/>
+      <c r="F160" s="4"/>
+      <c r="G160" s="4"/>
+      <c r="H160" s="4"/>
+    </row>
+    <row r="161" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B161" s="4">
+        <v>1211</v>
+      </c>
+      <c r="C161">
+        <v>44593</v>
+      </c>
+      <c r="D161" s="4"/>
+      <c r="E161" s="4"/>
+      <c r="F161" s="4"/>
+      <c r="G161" s="4"/>
+      <c r="H161" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
se actualizo excel cc 10-02-2023
</commit_message>
<xml_diff>
--- a/helps/Historial de Jugadas.xlsx
+++ b/helps/Historial de Jugadas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Randon\helps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6616974-60E6-411F-B56D-6FA97D03F58F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39AB2B68-6A2C-492B-B198-256F89624B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1" xr2:uid="{A3392D85-3030-46DE-B96E-7922EDC7109E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{A3392D85-3030-46DE-B96E-7922EDC7109E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tinka" sheetId="2" r:id="rId1"/>
@@ -20,6 +20,15 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -201,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -215,10 +224,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -226,12 +231,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -564,7 +563,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" customWidth="1"/>
     <col min="8" max="8" width="19.28515625" customWidth="1"/>
@@ -572,12 +571,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="12">
+      <c r="B1" s="8">
         <v>44626</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3">
@@ -585,7 +584,7 @@
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
+      <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4">
@@ -593,592 +592,592 @@
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C5" s="13">
+      <c r="C5" s="9">
         <f>SUM(C3:C4)</f>
         <v>2359</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="5"/>
+      <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="10"/>
-      <c r="C7" s="8" t="s">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8" t="s">
+      <c r="F7" s="6"/>
+      <c r="G7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="11"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
     </row>
     <row r="9" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="11"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
     </row>
     <row r="10" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="11"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
     </row>
     <row r="11" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="11"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
     </row>
     <row r="12" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="11"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
     </row>
     <row r="13" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="11"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
     </row>
     <row r="14" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="11"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
     </row>
     <row r="15" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="11"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
     </row>
     <row r="16" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="11"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
     </row>
     <row r="17" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="11"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
     </row>
     <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="11"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
     </row>
     <row r="19" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="11"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
     </row>
     <row r="20" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="11"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
     </row>
     <row r="21" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="11"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
     </row>
     <row r="22" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="11"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
     </row>
     <row r="23" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="11"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
     </row>
     <row r="24" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="11"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
     </row>
     <row r="25" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="11"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
     </row>
     <row r="26" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="11"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
     </row>
     <row r="27" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="11"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
     </row>
     <row r="28" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="11"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
     </row>
     <row r="29" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="11"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
     </row>
     <row r="30" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="11"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
     </row>
     <row r="31" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="11"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
     </row>
     <row r="32" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="11"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
     </row>
     <row r="33" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="11">
+      <c r="B33" s="5">
         <f>B34+23</f>
         <v>2403</v>
       </c>
-      <c r="C33" s="15">
+      <c r="C33" s="11">
         <v>44927</v>
       </c>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
     </row>
     <row r="34" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="11">
+      <c r="B34" s="5">
         <v>2380</v>
       </c>
-      <c r="C34" s="14">
+      <c r="C34" s="10">
         <v>44699</v>
       </c>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
     </row>
     <row r="35" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="11">
+      <c r="B35" s="5">
         <v>2379</v>
       </c>
-      <c r="C35" s="14">
+      <c r="C35" s="10">
         <v>44696</v>
       </c>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
     </row>
     <row r="36" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="11">
+      <c r="B36" s="5">
         <v>2378</v>
       </c>
-      <c r="C36" s="14">
+      <c r="C36" s="10">
         <v>44692</v>
       </c>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
     </row>
     <row r="37" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="11">
+      <c r="B37" s="5">
         <v>2377</v>
       </c>
-      <c r="C37" s="14">
+      <c r="C37" s="10">
         <v>44689</v>
       </c>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
     </row>
     <row r="38" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="11">
+      <c r="B38" s="5">
         <v>2376</v>
       </c>
-      <c r="C38" s="14">
+      <c r="C38" s="10">
         <v>44685</v>
       </c>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
     </row>
     <row r="39" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="11">
+      <c r="B39" s="5">
         <v>2375</v>
       </c>
-      <c r="C39" s="14">
+      <c r="C39" s="10">
         <v>44682</v>
       </c>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
     </row>
     <row r="40" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="11">
+      <c r="B40" s="5">
         <v>2374</v>
       </c>
-      <c r="C40" s="14">
+      <c r="C40" s="10">
         <v>44678</v>
       </c>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
     </row>
     <row r="41" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="11">
+      <c r="B41" s="5">
         <v>2373</v>
       </c>
-      <c r="C41" s="14">
+      <c r="C41" s="10">
         <v>44675</v>
       </c>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
     </row>
     <row r="42" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="11">
+      <c r="B42" s="5">
         <v>2372</v>
       </c>
-      <c r="C42" s="14">
+      <c r="C42" s="10">
         <v>44671</v>
       </c>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
     </row>
     <row r="43" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="11">
+      <c r="B43" s="5">
         <v>2371</v>
       </c>
-      <c r="C43" s="14">
+      <c r="C43" s="10">
         <v>44668</v>
       </c>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
     </row>
     <row r="44" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="11">
+      <c r="B44" s="5">
         <v>2370</v>
       </c>
-      <c r="C44" s="14">
+      <c r="C44" s="10">
         <v>44664</v>
       </c>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="7"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
     </row>
     <row r="45" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="11">
+      <c r="B45" s="5">
         <v>2369</v>
       </c>
-      <c r="C45" s="14">
+      <c r="C45" s="10">
         <v>44661</v>
       </c>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="7"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
     </row>
     <row r="46" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="11">
+      <c r="B46" s="5">
         <v>2368</v>
       </c>
-      <c r="C46" s="14">
+      <c r="C46" s="10">
         <v>44657</v>
       </c>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="7"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
     </row>
     <row r="47" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="11">
+      <c r="B47" s="5">
         <v>2367</v>
       </c>
-      <c r="C47" s="14">
+      <c r="C47" s="10">
         <v>44654</v>
       </c>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
     </row>
     <row r="48" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="11">
+      <c r="B48" s="5">
         <v>2366</v>
       </c>
-      <c r="C48" s="14">
+      <c r="C48" s="10">
         <v>44650</v>
       </c>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7"/>
-      <c r="G48" s="7"/>
-      <c r="H48" s="7"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
     </row>
     <row r="49" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="11">
+      <c r="B49" s="5">
         <v>2365</v>
       </c>
-      <c r="C49" s="14">
+      <c r="C49" s="10">
         <v>44647</v>
       </c>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="7"/>
-      <c r="G49" s="7"/>
-      <c r="H49" s="7"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
     </row>
     <row r="50" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="11">
+      <c r="B50" s="5">
         <v>2364</v>
       </c>
-      <c r="C50" s="14">
+      <c r="C50" s="10">
         <v>44643</v>
       </c>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
-      <c r="G50" s="7"/>
-      <c r="H50" s="7"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
     </row>
     <row r="51" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="11">
+      <c r="B51" s="5">
         <v>2363</v>
       </c>
-      <c r="C51" s="14">
+      <c r="C51" s="10">
         <v>44640</v>
       </c>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
-      <c r="F51" s="7"/>
-      <c r="G51" s="7"/>
-      <c r="H51" s="7"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
     </row>
     <row r="52" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="11">
+      <c r="B52" s="5">
         <v>2362</v>
       </c>
-      <c r="C52" s="14">
+      <c r="C52" s="10">
         <v>44636</v>
       </c>
-      <c r="D52" s="7"/>
-      <c r="E52" s="7"/>
-      <c r="F52" s="7"/>
-      <c r="G52" s="7"/>
-      <c r="H52" s="7"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
     </row>
     <row r="53" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="11">
+      <c r="B53" s="5">
         <v>2361</v>
       </c>
-      <c r="C53" s="14">
+      <c r="C53" s="10">
         <v>44633</v>
       </c>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="7"/>
-      <c r="G53" s="7"/>
-      <c r="H53" s="7"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
     </row>
     <row r="54" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="11">
+      <c r="B54" s="5">
         <v>2360</v>
       </c>
-      <c r="C54" s="14">
+      <c r="C54" s="10">
         <v>44629</v>
       </c>
-      <c r="D54" s="7"/>
-      <c r="E54" s="7"/>
-      <c r="F54" s="7"/>
-      <c r="G54" s="7"/>
-      <c r="H54" s="7"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
     </row>
     <row r="55" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="11">
+      <c r="B55" s="5">
         <v>2359</v>
       </c>
-      <c r="C55" s="14">
+      <c r="C55" s="10">
         <v>44626</v>
       </c>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="7"/>
-      <c r="G55" s="7"/>
-      <c r="H55" s="7"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="5"/>
     </row>
     <row r="56" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>11</v>
       </c>
-      <c r="B56" s="11" t="s">
+      <c r="B56" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C56" s="14">
+      <c r="C56" s="10">
         <v>34623</v>
       </c>
-      <c r="D56" s="7"/>
-      <c r="E56" s="7" t="s">
+      <c r="D56" s="5"/>
+      <c r="E56" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F56" s="7"/>
-      <c r="G56" s="7"/>
-      <c r="H56" s="7"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
     </row>
     <row r="57" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>10</v>
       </c>
-      <c r="B57" s="11" t="s">
+      <c r="B57" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C57" s="14">
+      <c r="C57" s="10">
         <v>38126</v>
       </c>
-      <c r="D57" s="7"/>
-      <c r="E57" s="7"/>
-      <c r="F57" s="7"/>
-      <c r="G57" s="7"/>
-      <c r="H57" s="7"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1188,10 +1187,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15FEB743-8F41-4809-BA70-E7C1EBE37B84}">
-  <dimension ref="A1:H161"/>
+  <dimension ref="A1:H174"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1200,12 +1199,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12">
+      <c r="A1" s="8">
         <v>41769</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
+      <c r="A2" s="8">
         <v>44593</v>
       </c>
       <c r="B2">
@@ -1241,7 +1240,7 @@
     </row>
     <row r="5" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4"/>
-      <c r="C5" s="14"/>
+      <c r="C5" s="10"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -1250,7 +1249,7 @@
     </row>
     <row r="6" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4"/>
-      <c r="C6" s="14"/>
+      <c r="C6" s="10"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -1258,12 +1257,8 @@
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="4">
-        <v>1365</v>
-      </c>
-      <c r="C7" s="14">
-        <v>44952</v>
-      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="10"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -1271,12 +1266,8 @@
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="4">
-        <v>1364</v>
-      </c>
-      <c r="C8" s="14">
-        <v>44950</v>
-      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="10"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -1284,12 +1275,8 @@
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="4">
-        <v>1363</v>
-      </c>
-      <c r="C9" s="14">
-        <v>44947</v>
-      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="10"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -1297,12 +1284,8 @@
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="4">
-        <v>1362</v>
-      </c>
-      <c r="C10" s="14">
-        <v>44945</v>
-      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="10"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -1310,12 +1293,8 @@
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="4">
-        <v>1361</v>
-      </c>
-      <c r="C11" s="14">
-        <v>44943</v>
-      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="10"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -1324,10 +1303,10 @@
     </row>
     <row r="12" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
-        <v>1360</v>
-      </c>
-      <c r="C12" s="14">
-        <v>44940</v>
+        <v>1373</v>
+      </c>
+      <c r="C12" s="10">
+        <v>44971</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
@@ -1337,10 +1316,10 @@
     </row>
     <row r="13" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="4">
-        <v>1359</v>
-      </c>
-      <c r="C13" s="14">
-        <v>44938</v>
+        <v>1372</v>
+      </c>
+      <c r="C13" s="10">
+        <v>44968</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -1350,10 +1329,10 @@
     </row>
     <row r="14" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
-        <v>1358</v>
-      </c>
-      <c r="C14" s="14">
-        <v>44936</v>
+        <v>1371</v>
+      </c>
+      <c r="C14" s="10">
+        <v>44966</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
@@ -1363,10 +1342,10 @@
     </row>
     <row r="15" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="4">
-        <v>1357</v>
-      </c>
-      <c r="C15" s="14">
-        <v>44933</v>
+        <v>1370</v>
+      </c>
+      <c r="C15" s="10">
+        <v>44964</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -1376,10 +1355,10 @@
     </row>
     <row r="16" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="4">
-        <v>1356</v>
-      </c>
-      <c r="C16" s="14">
-        <v>44931</v>
+        <v>1369</v>
+      </c>
+      <c r="C16" s="10">
+        <v>44961</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
@@ -1389,10 +1368,10 @@
     </row>
     <row r="17" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="4">
-        <v>1355</v>
-      </c>
-      <c r="C17" s="14">
-        <v>44929</v>
+        <v>1368</v>
+      </c>
+      <c r="C17" s="10">
+        <v>44959</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -1402,10 +1381,10 @@
     </row>
     <row r="18" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="4">
-        <v>1354</v>
-      </c>
-      <c r="C18" s="14">
-        <v>44926</v>
+        <v>1367</v>
+      </c>
+      <c r="C18" s="10">
+        <v>44957</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
@@ -1415,10 +1394,10 @@
     </row>
     <row r="19" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="4">
-        <v>1353</v>
-      </c>
-      <c r="C19" s="14">
-        <v>44924</v>
+        <v>1366</v>
+      </c>
+      <c r="C19" s="10">
+        <v>44954</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
@@ -1428,10 +1407,10 @@
     </row>
     <row r="20" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="4">
-        <v>1352</v>
-      </c>
-      <c r="C20" s="14">
-        <v>44922</v>
+        <v>1365</v>
+      </c>
+      <c r="C20" s="10">
+        <v>44952</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
@@ -1441,10 +1420,10 @@
     </row>
     <row r="21" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="4">
-        <v>1351</v>
-      </c>
-      <c r="C21" s="14">
-        <v>44919</v>
+        <v>1364</v>
+      </c>
+      <c r="C21" s="10">
+        <v>44950</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
@@ -1454,10 +1433,10 @@
     </row>
     <row r="22" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="4">
-        <v>1350</v>
-      </c>
-      <c r="C22" s="14">
-        <v>44917</v>
+        <v>1363</v>
+      </c>
+      <c r="C22" s="10">
+        <v>44947</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
@@ -1467,10 +1446,10 @@
     </row>
     <row r="23" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="4">
-        <v>1349</v>
-      </c>
-      <c r="C23" s="14">
-        <v>44915</v>
+        <v>1362</v>
+      </c>
+      <c r="C23" s="10">
+        <v>44945</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
@@ -1480,10 +1459,10 @@
     </row>
     <row r="24" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="4">
-        <v>1348</v>
-      </c>
-      <c r="C24" s="14">
-        <v>44912</v>
+        <v>1361</v>
+      </c>
+      <c r="C24" s="10">
+        <v>44943</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
@@ -1493,10 +1472,10 @@
     </row>
     <row r="25" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="4">
-        <v>1347</v>
-      </c>
-      <c r="C25" s="14">
-        <v>44910</v>
+        <v>1360</v>
+      </c>
+      <c r="C25" s="10">
+        <v>44940</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
@@ -1506,10 +1485,10 @@
     </row>
     <row r="26" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="4">
-        <v>1346</v>
-      </c>
-      <c r="C26" s="14">
-        <v>44908</v>
+        <v>1359</v>
+      </c>
+      <c r="C26" s="10">
+        <v>44938</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
@@ -1519,10 +1498,10 @@
     </row>
     <row r="27" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="4">
-        <v>1345</v>
-      </c>
-      <c r="C27" s="14">
-        <v>44905</v>
+        <v>1358</v>
+      </c>
+      <c r="C27" s="10">
+        <v>44936</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
@@ -1532,10 +1511,10 @@
     </row>
     <row r="28" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="4">
-        <v>1344</v>
-      </c>
-      <c r="C28" s="14">
-        <v>44903</v>
+        <v>1357</v>
+      </c>
+      <c r="C28" s="10">
+        <v>44933</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
@@ -1545,10 +1524,10 @@
     </row>
     <row r="29" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="4">
-        <v>1343</v>
-      </c>
-      <c r="C29" s="14">
-        <v>44901</v>
+        <v>1356</v>
+      </c>
+      <c r="C29" s="10">
+        <v>44931</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -1558,10 +1537,10 @@
     </row>
     <row r="30" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="4">
-        <v>1342</v>
-      </c>
-      <c r="C30" s="14">
-        <v>44898</v>
+        <v>1355</v>
+      </c>
+      <c r="C30" s="10">
+        <v>44929</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
@@ -1571,10 +1550,10 @@
     </row>
     <row r="31" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="4">
-        <v>1341</v>
-      </c>
-      <c r="C31" s="14">
-        <v>44896</v>
+        <v>1354</v>
+      </c>
+      <c r="C31" s="10">
+        <v>44926</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -1584,10 +1563,10 @@
     </row>
     <row r="32" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="4">
-        <v>1340</v>
-      </c>
-      <c r="C32" s="14">
-        <v>44894</v>
+        <v>1353</v>
+      </c>
+      <c r="C32" s="10">
+        <v>44924</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -1597,10 +1576,10 @@
     </row>
     <row r="33" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="4">
-        <v>1339</v>
-      </c>
-      <c r="C33" s="14">
-        <v>44891</v>
+        <v>1352</v>
+      </c>
+      <c r="C33" s="10">
+        <v>44922</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
@@ -1610,12 +1589,12 @@
     </row>
     <row r="34" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="4">
-        <v>1338</v>
-      </c>
-      <c r="C34" s="14">
-        <v>44889</v>
-      </c>
-      <c r="D34" s="14"/>
+        <v>1351</v>
+      </c>
+      <c r="C34" s="10">
+        <v>44919</v>
+      </c>
+      <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
@@ -1623,10 +1602,10 @@
     </row>
     <row r="35" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="4">
-        <v>1337</v>
-      </c>
-      <c r="C35" s="14">
-        <v>44887</v>
+        <v>1350</v>
+      </c>
+      <c r="C35" s="10">
+        <v>44917</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -1636,10 +1615,10 @@
     </row>
     <row r="36" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="4">
-        <v>1336</v>
-      </c>
-      <c r="C36" s="14">
-        <v>44884</v>
+        <v>1349</v>
+      </c>
+      <c r="C36" s="10">
+        <v>44915</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -1649,10 +1628,10 @@
     </row>
     <row r="37" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="4">
-        <v>1335</v>
-      </c>
-      <c r="C37" s="14">
-        <v>44882</v>
+        <v>1348</v>
+      </c>
+      <c r="C37" s="10">
+        <v>44912</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -1662,10 +1641,10 @@
     </row>
     <row r="38" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="4">
-        <v>1334</v>
-      </c>
-      <c r="C38" s="14">
-        <v>44880</v>
+        <v>1347</v>
+      </c>
+      <c r="C38" s="10">
+        <v>44910</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
@@ -1675,10 +1654,10 @@
     </row>
     <row r="39" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="4">
-        <v>1333</v>
-      </c>
-      <c r="C39" s="14">
-        <v>44877</v>
+        <v>1346</v>
+      </c>
+      <c r="C39" s="10">
+        <v>44908</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
@@ -1688,10 +1667,10 @@
     </row>
     <row r="40" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="4">
-        <v>1332</v>
-      </c>
-      <c r="C40" s="14">
-        <v>44875</v>
+        <v>1345</v>
+      </c>
+      <c r="C40" s="10">
+        <v>44905</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
@@ -1701,10 +1680,10 @@
     </row>
     <row r="41" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="4">
-        <v>1331</v>
-      </c>
-      <c r="C41" s="14">
-        <v>44873</v>
+        <v>1344</v>
+      </c>
+      <c r="C41" s="10">
+        <v>44903</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
@@ -1714,10 +1693,10 @@
     </row>
     <row r="42" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="4">
-        <v>1330</v>
-      </c>
-      <c r="C42" s="14">
-        <v>44870</v>
+        <v>1343</v>
+      </c>
+      <c r="C42" s="10">
+        <v>44901</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
@@ -1727,10 +1706,10 @@
     </row>
     <row r="43" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="4">
-        <v>1329</v>
-      </c>
-      <c r="C43" s="14">
-        <v>44868</v>
+        <v>1342</v>
+      </c>
+      <c r="C43" s="10">
+        <v>44898</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
@@ -1740,10 +1719,10 @@
     </row>
     <row r="44" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="4">
-        <v>1328</v>
-      </c>
-      <c r="C44" s="14">
-        <v>44866</v>
+        <v>1341</v>
+      </c>
+      <c r="C44" s="10">
+        <v>44896</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -1753,10 +1732,10 @@
     </row>
     <row r="45" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="4">
-        <v>1327</v>
-      </c>
-      <c r="C45" s="14">
-        <v>44863</v>
+        <v>1340</v>
+      </c>
+      <c r="C45" s="10">
+        <v>44894</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
@@ -1766,10 +1745,10 @@
     </row>
     <row r="46" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="4">
-        <v>1326</v>
-      </c>
-      <c r="C46" s="14">
-        <v>44861</v>
+        <v>1339</v>
+      </c>
+      <c r="C46" s="10">
+        <v>44891</v>
       </c>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
@@ -1779,12 +1758,12 @@
     </row>
     <row r="47" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="4">
-        <v>1325</v>
-      </c>
-      <c r="C47" s="14">
-        <v>44859</v>
-      </c>
-      <c r="D47" s="4"/>
+        <v>1338</v>
+      </c>
+      <c r="C47" s="10">
+        <v>44889</v>
+      </c>
+      <c r="D47" s="10"/>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
@@ -1792,10 +1771,10 @@
     </row>
     <row r="48" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="4">
-        <v>1324</v>
-      </c>
-      <c r="C48" s="14">
-        <v>44856</v>
+        <v>1337</v>
+      </c>
+      <c r="C48" s="10">
+        <v>44887</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
@@ -1805,10 +1784,10 @@
     </row>
     <row r="49" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="4">
-        <v>1323</v>
-      </c>
-      <c r="C49" s="14">
-        <v>44854</v>
+        <v>1336</v>
+      </c>
+      <c r="C49" s="10">
+        <v>44884</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
@@ -1818,10 +1797,10 @@
     </row>
     <row r="50" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="4">
-        <v>1322</v>
-      </c>
-      <c r="C50" s="14">
-        <v>44852</v>
+        <v>1335</v>
+      </c>
+      <c r="C50" s="10">
+        <v>44882</v>
       </c>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
@@ -1831,10 +1810,10 @@
     </row>
     <row r="51" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="4">
-        <v>1321</v>
-      </c>
-      <c r="C51" s="14">
-        <v>44849</v>
+        <v>1334</v>
+      </c>
+      <c r="C51" s="10">
+        <v>44880</v>
       </c>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
@@ -1844,10 +1823,10 @@
     </row>
     <row r="52" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="4">
-        <v>1320</v>
-      </c>
-      <c r="C52" s="14">
-        <v>44847</v>
+        <v>1333</v>
+      </c>
+      <c r="C52" s="10">
+        <v>44877</v>
       </c>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
@@ -1857,10 +1836,10 @@
     </row>
     <row r="53" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="4">
-        <v>1319</v>
-      </c>
-      <c r="C53" s="14">
-        <v>44845</v>
+        <v>1332</v>
+      </c>
+      <c r="C53" s="10">
+        <v>44875</v>
       </c>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
@@ -1870,10 +1849,10 @@
     </row>
     <row r="54" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="4">
-        <v>1318</v>
-      </c>
-      <c r="C54" s="14">
-        <v>44842</v>
+        <v>1331</v>
+      </c>
+      <c r="C54" s="10">
+        <v>44873</v>
       </c>
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
@@ -1883,10 +1862,10 @@
     </row>
     <row r="55" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="4">
-        <v>1317</v>
-      </c>
-      <c r="C55" s="14">
-        <v>44840</v>
+        <v>1330</v>
+      </c>
+      <c r="C55" s="10">
+        <v>44870</v>
       </c>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
@@ -1896,10 +1875,10 @@
     </row>
     <row r="56" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="4">
-        <v>1316</v>
-      </c>
-      <c r="C56" s="14">
-        <v>44838</v>
+        <v>1329</v>
+      </c>
+      <c r="C56" s="10">
+        <v>44868</v>
       </c>
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
@@ -1909,10 +1888,10 @@
     </row>
     <row r="57" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="4">
-        <v>1315</v>
-      </c>
-      <c r="C57" s="14">
-        <v>44835</v>
+        <v>1328</v>
+      </c>
+      <c r="C57" s="10">
+        <v>44866</v>
       </c>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
@@ -1922,10 +1901,10 @@
     </row>
     <row r="58" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="4">
-        <v>1314</v>
-      </c>
-      <c r="C58" s="14">
-        <v>44833</v>
+        <v>1327</v>
+      </c>
+      <c r="C58" s="10">
+        <v>44863</v>
       </c>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
@@ -1935,10 +1914,10 @@
     </row>
     <row r="59" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="4">
-        <v>1313</v>
-      </c>
-      <c r="C59" s="14">
-        <v>44831</v>
+        <v>1326</v>
+      </c>
+      <c r="C59" s="10">
+        <v>44861</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
@@ -1948,10 +1927,10 @@
     </row>
     <row r="60" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B60" s="4">
-        <v>1312</v>
-      </c>
-      <c r="C60" s="14">
-        <v>44828</v>
+        <v>1325</v>
+      </c>
+      <c r="C60" s="10">
+        <v>44859</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
@@ -1961,10 +1940,10 @@
     </row>
     <row r="61" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B61" s="4">
-        <v>1311</v>
-      </c>
-      <c r="C61" s="14">
-        <v>44826</v>
+        <v>1324</v>
+      </c>
+      <c r="C61" s="10">
+        <v>44856</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
@@ -1974,10 +1953,10 @@
     </row>
     <row r="62" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B62" s="4">
-        <v>1310</v>
-      </c>
-      <c r="C62" s="14">
-        <v>44824</v>
+        <v>1323</v>
+      </c>
+      <c r="C62" s="10">
+        <v>44854</v>
       </c>
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
@@ -1987,10 +1966,10 @@
     </row>
     <row r="63" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="4">
-        <v>1309</v>
-      </c>
-      <c r="C63" s="14">
-        <v>44821</v>
+        <v>1322</v>
+      </c>
+      <c r="C63" s="10">
+        <v>44852</v>
       </c>
       <c r="D63" s="4"/>
       <c r="E63" s="4"/>
@@ -2000,10 +1979,10 @@
     </row>
     <row r="64" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B64" s="4">
-        <v>1308</v>
-      </c>
-      <c r="C64" s="14">
-        <v>44819</v>
+        <v>1321</v>
+      </c>
+      <c r="C64" s="10">
+        <v>44849</v>
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="4"/>
@@ -2013,10 +1992,10 @@
     </row>
     <row r="65" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B65" s="4">
-        <v>1307</v>
-      </c>
-      <c r="C65" s="14">
-        <v>44817</v>
+        <v>1320</v>
+      </c>
+      <c r="C65" s="10">
+        <v>44847</v>
       </c>
       <c r="D65" s="4"/>
       <c r="E65" s="4"/>
@@ -2026,10 +2005,10 @@
     </row>
     <row r="66" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B66" s="4">
-        <v>1306</v>
-      </c>
-      <c r="C66" s="14">
-        <v>44814</v>
+        <v>1319</v>
+      </c>
+      <c r="C66" s="10">
+        <v>44845</v>
       </c>
       <c r="D66" s="4"/>
       <c r="E66" s="4"/>
@@ -2039,10 +2018,10 @@
     </row>
     <row r="67" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B67" s="4">
-        <v>1305</v>
-      </c>
-      <c r="C67" s="14">
-        <v>44812</v>
+        <v>1318</v>
+      </c>
+      <c r="C67" s="10">
+        <v>44842</v>
       </c>
       <c r="D67" s="4"/>
       <c r="E67" s="4"/>
@@ -2052,10 +2031,10 @@
     </row>
     <row r="68" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="4">
-        <v>1304</v>
-      </c>
-      <c r="C68" s="14">
-        <v>44810</v>
+        <v>1317</v>
+      </c>
+      <c r="C68" s="10">
+        <v>44840</v>
       </c>
       <c r="D68" s="4"/>
       <c r="E68" s="4"/>
@@ -2065,10 +2044,10 @@
     </row>
     <row r="69" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B69" s="4">
-        <v>1303</v>
-      </c>
-      <c r="C69" s="14">
-        <v>44807</v>
+        <v>1316</v>
+      </c>
+      <c r="C69" s="10">
+        <v>44838</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69" s="4"/>
@@ -2078,10 +2057,10 @@
     </row>
     <row r="70" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B70" s="4">
-        <v>1302</v>
-      </c>
-      <c r="C70" s="14">
-        <v>44805</v>
+        <v>1315</v>
+      </c>
+      <c r="C70" s="10">
+        <v>44835</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="4"/>
@@ -2091,10 +2070,10 @@
     </row>
     <row r="71" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B71" s="4">
-        <v>1301</v>
-      </c>
-      <c r="C71" s="14">
-        <v>44803</v>
+        <v>1314</v>
+      </c>
+      <c r="C71" s="10">
+        <v>44833</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" s="4"/>
@@ -2104,10 +2083,10 @@
     </row>
     <row r="72" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B72" s="4">
-        <v>1300</v>
-      </c>
-      <c r="C72" s="14">
-        <v>44800</v>
+        <v>1313</v>
+      </c>
+      <c r="C72" s="10">
+        <v>44831</v>
       </c>
       <c r="D72" s="4"/>
       <c r="E72" s="4"/>
@@ -2117,10 +2096,10 @@
     </row>
     <row r="73" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B73" s="4">
-        <v>1299</v>
-      </c>
-      <c r="C73" s="14">
-        <v>44798</v>
+        <v>1312</v>
+      </c>
+      <c r="C73" s="10">
+        <v>44828</v>
       </c>
       <c r="D73" s="4"/>
       <c r="E73" s="4"/>
@@ -2130,10 +2109,10 @@
     </row>
     <row r="74" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B74" s="4">
-        <v>1298</v>
-      </c>
-      <c r="C74" s="14">
-        <v>44796</v>
+        <v>1311</v>
+      </c>
+      <c r="C74" s="10">
+        <v>44826</v>
       </c>
       <c r="D74" s="4"/>
       <c r="E74" s="4"/>
@@ -2143,10 +2122,10 @@
     </row>
     <row r="75" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B75" s="4">
-        <v>1297</v>
-      </c>
-      <c r="C75" s="14">
-        <v>44793</v>
+        <v>1310</v>
+      </c>
+      <c r="C75" s="10">
+        <v>44824</v>
       </c>
       <c r="D75" s="4"/>
       <c r="E75" s="4"/>
@@ -2156,10 +2135,10 @@
     </row>
     <row r="76" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B76" s="4">
-        <v>1296</v>
-      </c>
-      <c r="C76" s="14">
-        <v>44791</v>
+        <v>1309</v>
+      </c>
+      <c r="C76" s="10">
+        <v>44821</v>
       </c>
       <c r="D76" s="4"/>
       <c r="E76" s="4"/>
@@ -2169,10 +2148,10 @@
     </row>
     <row r="77" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B77" s="4">
-        <v>1295</v>
-      </c>
-      <c r="C77" s="14">
-        <v>44789</v>
+        <v>1308</v>
+      </c>
+      <c r="C77" s="10">
+        <v>44819</v>
       </c>
       <c r="D77" s="4"/>
       <c r="E77" s="4"/>
@@ -2182,10 +2161,10 @@
     </row>
     <row r="78" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="4">
-        <v>1294</v>
-      </c>
-      <c r="C78" s="14">
-        <v>44786</v>
+        <v>1307</v>
+      </c>
+      <c r="C78" s="10">
+        <v>44817</v>
       </c>
       <c r="D78" s="4"/>
       <c r="E78" s="4"/>
@@ -2195,10 +2174,10 @@
     </row>
     <row r="79" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B79" s="4">
-        <v>1293</v>
-      </c>
-      <c r="C79" s="14">
-        <v>44784</v>
+        <v>1306</v>
+      </c>
+      <c r="C79" s="10">
+        <v>44814</v>
       </c>
       <c r="D79" s="4"/>
       <c r="E79" s="4"/>
@@ -2208,10 +2187,10 @@
     </row>
     <row r="80" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B80" s="4">
-        <v>1292</v>
-      </c>
-      <c r="C80" s="14">
-        <v>44782</v>
+        <v>1305</v>
+      </c>
+      <c r="C80" s="10">
+        <v>44812</v>
       </c>
       <c r="D80" s="4"/>
       <c r="E80" s="4"/>
@@ -2221,10 +2200,10 @@
     </row>
     <row r="81" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B81" s="4">
-        <v>1291</v>
-      </c>
-      <c r="C81" s="14">
-        <v>44779</v>
+        <v>1304</v>
+      </c>
+      <c r="C81" s="10">
+        <v>44810</v>
       </c>
       <c r="D81" s="4"/>
       <c r="E81" s="4"/>
@@ -2234,10 +2213,10 @@
     </row>
     <row r="82" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B82" s="4">
-        <v>1290</v>
-      </c>
-      <c r="C82" s="14">
-        <v>44777</v>
+        <v>1303</v>
+      </c>
+      <c r="C82" s="10">
+        <v>44807</v>
       </c>
       <c r="D82" s="4"/>
       <c r="E82" s="4"/>
@@ -2247,10 +2226,10 @@
     </row>
     <row r="83" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B83" s="4">
-        <v>1289</v>
-      </c>
-      <c r="C83" s="14">
-        <v>44775</v>
+        <v>1302</v>
+      </c>
+      <c r="C83" s="10">
+        <v>44805</v>
       </c>
       <c r="D83" s="4"/>
       <c r="E83" s="4"/>
@@ -2260,10 +2239,10 @@
     </row>
     <row r="84" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B84" s="4">
-        <v>1288</v>
-      </c>
-      <c r="C84" s="14">
-        <v>44772</v>
+        <v>1301</v>
+      </c>
+      <c r="C84" s="10">
+        <v>44803</v>
       </c>
       <c r="D84" s="4"/>
       <c r="E84" s="4"/>
@@ -2273,10 +2252,10 @@
     </row>
     <row r="85" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B85" s="4">
-        <v>1287</v>
-      </c>
-      <c r="C85" s="14">
-        <v>44770</v>
+        <v>1300</v>
+      </c>
+      <c r="C85" s="10">
+        <v>44800</v>
       </c>
       <c r="D85" s="4"/>
       <c r="E85" s="4"/>
@@ -2286,10 +2265,10 @@
     </row>
     <row r="86" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B86" s="4">
-        <v>1286</v>
-      </c>
-      <c r="C86" s="14">
-        <v>44768</v>
+        <v>1299</v>
+      </c>
+      <c r="C86" s="10">
+        <v>44798</v>
       </c>
       <c r="D86" s="4"/>
       <c r="E86" s="4"/>
@@ -2299,10 +2278,10 @@
     </row>
     <row r="87" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B87" s="4">
-        <v>1285</v>
-      </c>
-      <c r="C87" s="14">
-        <v>44765</v>
+        <v>1298</v>
+      </c>
+      <c r="C87" s="10">
+        <v>44796</v>
       </c>
       <c r="D87" s="4"/>
       <c r="E87" s="4"/>
@@ -2312,10 +2291,10 @@
     </row>
     <row r="88" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B88" s="4">
-        <v>1284</v>
-      </c>
-      <c r="C88" s="14">
-        <v>44763</v>
+        <v>1297</v>
+      </c>
+      <c r="C88" s="10">
+        <v>44793</v>
       </c>
       <c r="D88" s="4"/>
       <c r="E88" s="4"/>
@@ -2325,10 +2304,10 @@
     </row>
     <row r="89" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B89" s="4">
-        <v>1283</v>
-      </c>
-      <c r="C89" s="14">
-        <v>44761</v>
+        <v>1296</v>
+      </c>
+      <c r="C89" s="10">
+        <v>44791</v>
       </c>
       <c r="D89" s="4"/>
       <c r="E89" s="4"/>
@@ -2338,10 +2317,10 @@
     </row>
     <row r="90" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B90" s="4">
-        <v>1282</v>
-      </c>
-      <c r="C90" s="14">
-        <v>44758</v>
+        <v>1295</v>
+      </c>
+      <c r="C90" s="10">
+        <v>44789</v>
       </c>
       <c r="D90" s="4"/>
       <c r="E90" s="4"/>
@@ -2351,10 +2330,10 @@
     </row>
     <row r="91" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B91" s="4">
-        <v>1281</v>
-      </c>
-      <c r="C91" s="14">
-        <v>44756</v>
+        <v>1294</v>
+      </c>
+      <c r="C91" s="10">
+        <v>44786</v>
       </c>
       <c r="D91" s="4"/>
       <c r="E91" s="4"/>
@@ -2364,10 +2343,10 @@
     </row>
     <row r="92" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B92" s="4">
-        <v>1280</v>
-      </c>
-      <c r="C92" s="14">
-        <v>44754</v>
+        <v>1293</v>
+      </c>
+      <c r="C92" s="10">
+        <v>44784</v>
       </c>
       <c r="D92" s="4"/>
       <c r="E92" s="4"/>
@@ -2377,10 +2356,10 @@
     </row>
     <row r="93" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B93" s="4">
-        <v>1279</v>
-      </c>
-      <c r="C93" s="14">
-        <v>44751</v>
+        <v>1292</v>
+      </c>
+      <c r="C93" s="10">
+        <v>44782</v>
       </c>
       <c r="D93" s="4"/>
       <c r="E93" s="4"/>
@@ -2390,10 +2369,10 @@
     </row>
     <row r="94" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B94" s="4">
-        <v>1278</v>
-      </c>
-      <c r="C94" s="14">
-        <v>44749</v>
+        <v>1291</v>
+      </c>
+      <c r="C94" s="10">
+        <v>44779</v>
       </c>
       <c r="D94" s="4"/>
       <c r="E94" s="4"/>
@@ -2403,10 +2382,10 @@
     </row>
     <row r="95" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B95" s="4">
-        <v>1277</v>
-      </c>
-      <c r="C95" s="14">
-        <v>44747</v>
+        <v>1290</v>
+      </c>
+      <c r="C95" s="10">
+        <v>44777</v>
       </c>
       <c r="D95" s="4"/>
       <c r="E95" s="4"/>
@@ -2416,10 +2395,10 @@
     </row>
     <row r="96" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B96" s="4">
-        <v>1276</v>
-      </c>
-      <c r="C96" s="14">
-        <v>44744</v>
+        <v>1289</v>
+      </c>
+      <c r="C96" s="10">
+        <v>44775</v>
       </c>
       <c r="D96" s="4"/>
       <c r="E96" s="4"/>
@@ -2429,10 +2408,10 @@
     </row>
     <row r="97" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B97" s="4">
-        <v>1275</v>
-      </c>
-      <c r="C97" s="14">
-        <v>44742</v>
+        <v>1288</v>
+      </c>
+      <c r="C97" s="10">
+        <v>44772</v>
       </c>
       <c r="D97" s="4"/>
       <c r="E97" s="4"/>
@@ -2442,10 +2421,10 @@
     </row>
     <row r="98" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B98" s="4">
-        <v>1274</v>
-      </c>
-      <c r="C98" s="14">
-        <v>44740</v>
+        <v>1287</v>
+      </c>
+      <c r="C98" s="10">
+        <v>44770</v>
       </c>
       <c r="D98" s="4"/>
       <c r="E98" s="4"/>
@@ -2455,10 +2434,10 @@
     </row>
     <row r="99" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B99" s="4">
-        <v>1273</v>
-      </c>
-      <c r="C99" s="14">
-        <v>44737</v>
+        <v>1286</v>
+      </c>
+      <c r="C99" s="10">
+        <v>44768</v>
       </c>
       <c r="D99" s="4"/>
       <c r="E99" s="4"/>
@@ -2468,10 +2447,10 @@
     </row>
     <row r="100" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B100" s="4">
-        <v>1272</v>
-      </c>
-      <c r="C100" s="14">
-        <v>44735</v>
+        <v>1285</v>
+      </c>
+      <c r="C100" s="10">
+        <v>44765</v>
       </c>
       <c r="D100" s="4"/>
       <c r="E100" s="4"/>
@@ -2481,10 +2460,10 @@
     </row>
     <row r="101" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B101" s="4">
-        <v>1271</v>
-      </c>
-      <c r="C101" s="14">
-        <v>44733</v>
+        <v>1284</v>
+      </c>
+      <c r="C101" s="10">
+        <v>44763</v>
       </c>
       <c r="D101" s="4"/>
       <c r="E101" s="4"/>
@@ -2494,10 +2473,10 @@
     </row>
     <row r="102" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B102" s="4">
-        <v>1270</v>
-      </c>
-      <c r="C102" s="14">
-        <v>44730</v>
+        <v>1283</v>
+      </c>
+      <c r="C102" s="10">
+        <v>44761</v>
       </c>
       <c r="D102" s="4"/>
       <c r="E102" s="4"/>
@@ -2507,10 +2486,10 @@
     </row>
     <row r="103" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B103" s="4">
-        <v>1269</v>
-      </c>
-      <c r="C103" s="14">
-        <v>44728</v>
+        <v>1282</v>
+      </c>
+      <c r="C103" s="10">
+        <v>44758</v>
       </c>
       <c r="D103" s="4"/>
       <c r="E103" s="4"/>
@@ -2520,10 +2499,10 @@
     </row>
     <row r="104" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B104" s="4">
-        <v>1268</v>
-      </c>
-      <c r="C104" s="14">
-        <v>44726</v>
+        <v>1281</v>
+      </c>
+      <c r="C104" s="10">
+        <v>44756</v>
       </c>
       <c r="D104" s="4"/>
       <c r="E104" s="4"/>
@@ -2533,10 +2512,10 @@
     </row>
     <row r="105" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B105" s="4">
-        <v>1267</v>
-      </c>
-      <c r="C105" s="14">
-        <v>44723</v>
+        <v>1280</v>
+      </c>
+      <c r="C105" s="10">
+        <v>44754</v>
       </c>
       <c r="D105" s="4"/>
       <c r="E105" s="4"/>
@@ -2546,10 +2525,10 @@
     </row>
     <row r="106" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B106" s="4">
-        <v>1266</v>
-      </c>
-      <c r="C106" s="14">
-        <v>44721</v>
+        <v>1279</v>
+      </c>
+      <c r="C106" s="10">
+        <v>44751</v>
       </c>
       <c r="D106" s="4"/>
       <c r="E106" s="4"/>
@@ -2559,10 +2538,10 @@
     </row>
     <row r="107" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B107" s="4">
-        <v>1265</v>
-      </c>
-      <c r="C107" s="14">
-        <v>44719</v>
+        <v>1278</v>
+      </c>
+      <c r="C107" s="10">
+        <v>44749</v>
       </c>
       <c r="D107" s="4"/>
       <c r="E107" s="4"/>
@@ -2572,10 +2551,10 @@
     </row>
     <row r="108" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B108" s="4">
-        <v>1264</v>
-      </c>
-      <c r="C108" s="14">
-        <v>44716</v>
+        <v>1277</v>
+      </c>
+      <c r="C108" s="10">
+        <v>44747</v>
       </c>
       <c r="D108" s="4"/>
       <c r="E108" s="4"/>
@@ -2585,10 +2564,10 @@
     </row>
     <row r="109" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B109" s="4">
-        <v>1263</v>
-      </c>
-      <c r="C109" s="14">
-        <v>44714</v>
+        <v>1276</v>
+      </c>
+      <c r="C109" s="10">
+        <v>44744</v>
       </c>
       <c r="D109" s="4"/>
       <c r="E109" s="4"/>
@@ -2598,10 +2577,10 @@
     </row>
     <row r="110" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B110" s="4">
-        <v>1262</v>
-      </c>
-      <c r="C110" s="14">
-        <v>44712</v>
+        <v>1275</v>
+      </c>
+      <c r="C110" s="10">
+        <v>44742</v>
       </c>
       <c r="D110" s="4"/>
       <c r="E110" s="4"/>
@@ -2611,10 +2590,10 @@
     </row>
     <row r="111" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B111" s="4">
-        <v>1261</v>
-      </c>
-      <c r="C111" s="14">
-        <v>44709</v>
+        <v>1274</v>
+      </c>
+      <c r="C111" s="10">
+        <v>44740</v>
       </c>
       <c r="D111" s="4"/>
       <c r="E111" s="4"/>
@@ -2624,10 +2603,10 @@
     </row>
     <row r="112" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B112" s="4">
-        <v>1260</v>
-      </c>
-      <c r="C112" s="14">
-        <v>44707</v>
+        <v>1273</v>
+      </c>
+      <c r="C112" s="10">
+        <v>44737</v>
       </c>
       <c r="D112" s="4"/>
       <c r="E112" s="4"/>
@@ -2637,10 +2616,10 @@
     </row>
     <row r="113" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B113" s="4">
-        <v>1259</v>
-      </c>
-      <c r="C113" s="14">
-        <v>44705</v>
+        <v>1272</v>
+      </c>
+      <c r="C113" s="10">
+        <v>44735</v>
       </c>
       <c r="D113" s="4"/>
       <c r="E113" s="4"/>
@@ -2650,10 +2629,10 @@
     </row>
     <row r="114" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B114" s="4">
-        <v>1258</v>
-      </c>
-      <c r="C114" s="14">
-        <v>44702</v>
+        <v>1271</v>
+      </c>
+      <c r="C114" s="10">
+        <v>44733</v>
       </c>
       <c r="D114" s="4"/>
       <c r="E114" s="4"/>
@@ -2663,10 +2642,10 @@
     </row>
     <row r="115" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B115" s="4">
-        <v>1257</v>
-      </c>
-      <c r="C115" s="14">
-        <v>44700</v>
+        <v>1270</v>
+      </c>
+      <c r="C115" s="10">
+        <v>44730</v>
       </c>
       <c r="D115" s="4"/>
       <c r="E115" s="4"/>
@@ -2676,10 +2655,10 @@
     </row>
     <row r="116" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B116" s="4">
-        <v>1256</v>
-      </c>
-      <c r="C116" s="14">
-        <v>44698</v>
+        <v>1269</v>
+      </c>
+      <c r="C116" s="10">
+        <v>44728</v>
       </c>
       <c r="D116" s="4"/>
       <c r="E116" s="4"/>
@@ -2689,10 +2668,10 @@
     </row>
     <row r="117" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B117" s="4">
-        <v>1255</v>
-      </c>
-      <c r="C117" s="14">
-        <v>44695</v>
+        <v>1268</v>
+      </c>
+      <c r="C117" s="10">
+        <v>44726</v>
       </c>
       <c r="D117" s="4"/>
       <c r="E117" s="4"/>
@@ -2702,10 +2681,10 @@
     </row>
     <row r="118" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B118" s="4">
-        <v>1254</v>
-      </c>
-      <c r="C118" s="14">
-        <v>44693</v>
+        <v>1267</v>
+      </c>
+      <c r="C118" s="10">
+        <v>44723</v>
       </c>
       <c r="D118" s="4"/>
       <c r="E118" s="4"/>
@@ -2715,10 +2694,10 @@
     </row>
     <row r="119" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B119" s="4">
-        <v>1253</v>
-      </c>
-      <c r="C119" s="14">
-        <v>44691</v>
+        <v>1266</v>
+      </c>
+      <c r="C119" s="10">
+        <v>44721</v>
       </c>
       <c r="D119" s="4"/>
       <c r="E119" s="4"/>
@@ -2728,10 +2707,10 @@
     </row>
     <row r="120" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B120" s="4">
-        <v>1252</v>
-      </c>
-      <c r="C120" s="14">
-        <v>44688</v>
+        <v>1265</v>
+      </c>
+      <c r="C120" s="10">
+        <v>44719</v>
       </c>
       <c r="D120" s="4"/>
       <c r="E120" s="4"/>
@@ -2741,10 +2720,10 @@
     </row>
     <row r="121" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B121" s="4">
-        <v>1251</v>
-      </c>
-      <c r="C121" s="14">
-        <v>44686</v>
+        <v>1264</v>
+      </c>
+      <c r="C121" s="10">
+        <v>44716</v>
       </c>
       <c r="D121" s="4"/>
       <c r="E121" s="4"/>
@@ -2754,10 +2733,10 @@
     </row>
     <row r="122" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B122" s="4">
-        <v>1250</v>
-      </c>
-      <c r="C122" s="14">
-        <v>44684</v>
+        <v>1263</v>
+      </c>
+      <c r="C122" s="10">
+        <v>44714</v>
       </c>
       <c r="D122" s="4"/>
       <c r="E122" s="4"/>
@@ -2767,10 +2746,10 @@
     </row>
     <row r="123" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B123" s="4">
-        <v>1249</v>
-      </c>
-      <c r="C123" s="14">
-        <v>44681</v>
+        <v>1262</v>
+      </c>
+      <c r="C123" s="10">
+        <v>44712</v>
       </c>
       <c r="D123" s="4"/>
       <c r="E123" s="4"/>
@@ -2780,10 +2759,10 @@
     </row>
     <row r="124" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B124" s="4">
-        <v>1248</v>
-      </c>
-      <c r="C124" s="14">
-        <v>44679</v>
+        <v>1261</v>
+      </c>
+      <c r="C124" s="10">
+        <v>44709</v>
       </c>
       <c r="D124" s="4"/>
       <c r="E124" s="4"/>
@@ -2793,10 +2772,10 @@
     </row>
     <row r="125" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B125" s="4">
-        <v>1247</v>
-      </c>
-      <c r="C125" s="14">
-        <v>44677</v>
+        <v>1260</v>
+      </c>
+      <c r="C125" s="10">
+        <v>44707</v>
       </c>
       <c r="D125" s="4"/>
       <c r="E125" s="4"/>
@@ -2806,10 +2785,10 @@
     </row>
     <row r="126" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B126" s="4">
-        <v>1246</v>
-      </c>
-      <c r="C126" s="14">
-        <v>44674</v>
+        <v>1259</v>
+      </c>
+      <c r="C126" s="10">
+        <v>44705</v>
       </c>
       <c r="D126" s="4"/>
       <c r="E126" s="4"/>
@@ -2819,10 +2798,10 @@
     </row>
     <row r="127" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B127" s="4">
-        <v>1245</v>
-      </c>
-      <c r="C127" s="14">
-        <v>44672</v>
+        <v>1258</v>
+      </c>
+      <c r="C127" s="10">
+        <v>44702</v>
       </c>
       <c r="D127" s="4"/>
       <c r="E127" s="4"/>
@@ -2832,10 +2811,10 @@
     </row>
     <row r="128" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B128" s="4">
-        <v>1244</v>
-      </c>
-      <c r="C128" s="14">
-        <v>44670</v>
+        <v>1257</v>
+      </c>
+      <c r="C128" s="10">
+        <v>44700</v>
       </c>
       <c r="D128" s="4"/>
       <c r="E128" s="4"/>
@@ -2845,10 +2824,10 @@
     </row>
     <row r="129" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B129" s="4">
-        <v>1243</v>
-      </c>
-      <c r="C129" s="14">
-        <v>44667</v>
+        <v>1256</v>
+      </c>
+      <c r="C129" s="10">
+        <v>44698</v>
       </c>
       <c r="D129" s="4"/>
       <c r="E129" s="4"/>
@@ -2858,10 +2837,10 @@
     </row>
     <row r="130" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B130" s="4">
-        <v>1242</v>
-      </c>
-      <c r="C130" s="14">
-        <v>44665</v>
+        <v>1255</v>
+      </c>
+      <c r="C130" s="10">
+        <v>44695</v>
       </c>
       <c r="D130" s="4"/>
       <c r="E130" s="4"/>
@@ -2871,10 +2850,10 @@
     </row>
     <row r="131" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B131" s="4">
-        <v>1241</v>
-      </c>
-      <c r="C131" s="14">
-        <v>44663</v>
+        <v>1254</v>
+      </c>
+      <c r="C131" s="10">
+        <v>44693</v>
       </c>
       <c r="D131" s="4"/>
       <c r="E131" s="4"/>
@@ -2884,10 +2863,10 @@
     </row>
     <row r="132" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B132" s="4">
-        <v>1240</v>
-      </c>
-      <c r="C132" s="14">
-        <v>44660</v>
+        <v>1253</v>
+      </c>
+      <c r="C132" s="10">
+        <v>44691</v>
       </c>
       <c r="D132" s="4"/>
       <c r="E132" s="4"/>
@@ -2897,10 +2876,10 @@
     </row>
     <row r="133" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B133" s="4">
-        <v>1239</v>
-      </c>
-      <c r="C133" s="14">
-        <v>44658</v>
+        <v>1252</v>
+      </c>
+      <c r="C133" s="10">
+        <v>44688</v>
       </c>
       <c r="D133" s="4"/>
       <c r="E133" s="4"/>
@@ -2910,10 +2889,10 @@
     </row>
     <row r="134" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B134" s="4">
-        <v>1238</v>
-      </c>
-      <c r="C134" s="14">
-        <v>44656</v>
+        <v>1251</v>
+      </c>
+      <c r="C134" s="10">
+        <v>44686</v>
       </c>
       <c r="D134" s="4"/>
       <c r="E134" s="4"/>
@@ -2923,10 +2902,10 @@
     </row>
     <row r="135" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B135" s="4">
-        <v>1237</v>
-      </c>
-      <c r="C135" s="14">
-        <v>44653</v>
+        <v>1250</v>
+      </c>
+      <c r="C135" s="10">
+        <v>44684</v>
       </c>
       <c r="D135" s="4"/>
       <c r="E135" s="4"/>
@@ -2936,10 +2915,10 @@
     </row>
     <row r="136" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B136" s="4">
-        <v>1236</v>
-      </c>
-      <c r="C136" s="14">
-        <v>44651</v>
+        <v>1249</v>
+      </c>
+      <c r="C136" s="10">
+        <v>44681</v>
       </c>
       <c r="D136" s="4"/>
       <c r="E136" s="4"/>
@@ -2949,10 +2928,10 @@
     </row>
     <row r="137" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B137" s="4">
-        <v>1235</v>
-      </c>
-      <c r="C137" s="14">
-        <v>44649</v>
+        <v>1248</v>
+      </c>
+      <c r="C137" s="10">
+        <v>44679</v>
       </c>
       <c r="D137" s="4"/>
       <c r="E137" s="4"/>
@@ -2962,10 +2941,10 @@
     </row>
     <row r="138" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B138" s="4">
-        <v>1234</v>
-      </c>
-      <c r="C138" s="14">
-        <v>44646</v>
+        <v>1247</v>
+      </c>
+      <c r="C138" s="10">
+        <v>44677</v>
       </c>
       <c r="D138" s="4"/>
       <c r="E138" s="4"/>
@@ -2975,10 +2954,10 @@
     </row>
     <row r="139" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B139" s="4">
-        <v>1233</v>
-      </c>
-      <c r="C139" s="14">
-        <v>44644</v>
+        <v>1246</v>
+      </c>
+      <c r="C139" s="10">
+        <v>44674</v>
       </c>
       <c r="D139" s="4"/>
       <c r="E139" s="4"/>
@@ -2988,10 +2967,10 @@
     </row>
     <row r="140" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B140" s="4">
-        <v>1232</v>
-      </c>
-      <c r="C140" s="14">
-        <v>44642</v>
+        <v>1245</v>
+      </c>
+      <c r="C140" s="10">
+        <v>44672</v>
       </c>
       <c r="D140" s="4"/>
       <c r="E140" s="4"/>
@@ -3001,10 +2980,10 @@
     </row>
     <row r="141" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B141" s="4">
-        <v>1231</v>
-      </c>
-      <c r="C141" s="14">
-        <v>44639</v>
+        <v>1244</v>
+      </c>
+      <c r="C141" s="10">
+        <v>44670</v>
       </c>
       <c r="D141" s="4"/>
       <c r="E141" s="4"/>
@@ -3014,10 +2993,10 @@
     </row>
     <row r="142" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B142" s="4">
-        <v>1230</v>
-      </c>
-      <c r="C142" s="14">
-        <v>44637</v>
+        <v>1243</v>
+      </c>
+      <c r="C142" s="10">
+        <v>44667</v>
       </c>
       <c r="D142" s="4"/>
       <c r="E142" s="4"/>
@@ -3027,10 +3006,10 @@
     </row>
     <row r="143" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B143" s="4">
-        <v>1229</v>
-      </c>
-      <c r="C143" s="14">
-        <v>44635</v>
+        <v>1242</v>
+      </c>
+      <c r="C143" s="10">
+        <v>44665</v>
       </c>
       <c r="D143" s="4"/>
       <c r="E143" s="4"/>
@@ -3040,10 +3019,10 @@
     </row>
     <row r="144" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B144" s="4">
-        <v>1228</v>
-      </c>
-      <c r="C144">
-        <v>44632</v>
+        <v>1241</v>
+      </c>
+      <c r="C144" s="10">
+        <v>44663</v>
       </c>
       <c r="D144" s="4"/>
       <c r="E144" s="4"/>
@@ -3053,10 +3032,10 @@
     </row>
     <row r="145" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B145" s="4">
-        <v>1227</v>
-      </c>
-      <c r="C145">
-        <v>44630</v>
+        <v>1240</v>
+      </c>
+      <c r="C145" s="10">
+        <v>44660</v>
       </c>
       <c r="D145" s="4"/>
       <c r="E145" s="4"/>
@@ -3066,10 +3045,10 @@
     </row>
     <row r="146" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B146" s="4">
-        <v>1226</v>
-      </c>
-      <c r="C146">
-        <v>44628</v>
+        <v>1239</v>
+      </c>
+      <c r="C146" s="10">
+        <v>44658</v>
       </c>
       <c r="D146" s="4"/>
       <c r="E146" s="4"/>
@@ -3079,10 +3058,10 @@
     </row>
     <row r="147" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B147" s="4">
-        <v>1225</v>
-      </c>
-      <c r="C147">
-        <v>44625</v>
+        <v>1238</v>
+      </c>
+      <c r="C147" s="10">
+        <v>44656</v>
       </c>
       <c r="D147" s="4"/>
       <c r="E147" s="4"/>
@@ -3092,10 +3071,10 @@
     </row>
     <row r="148" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B148" s="4">
-        <v>1224</v>
-      </c>
-      <c r="C148">
-        <v>44623</v>
+        <v>1237</v>
+      </c>
+      <c r="C148" s="10">
+        <v>44653</v>
       </c>
       <c r="D148" s="4"/>
       <c r="E148" s="4"/>
@@ -3105,10 +3084,10 @@
     </row>
     <row r="149" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B149" s="4">
-        <v>1223</v>
-      </c>
-      <c r="C149">
-        <v>44621</v>
+        <v>1236</v>
+      </c>
+      <c r="C149" s="10">
+        <v>44651</v>
       </c>
       <c r="D149" s="4"/>
       <c r="E149" s="4"/>
@@ -3118,10 +3097,10 @@
     </row>
     <row r="150" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B150" s="4">
-        <v>1222</v>
-      </c>
-      <c r="C150">
-        <v>44618</v>
+        <v>1235</v>
+      </c>
+      <c r="C150" s="10">
+        <v>44649</v>
       </c>
       <c r="D150" s="4"/>
       <c r="E150" s="4"/>
@@ -3131,10 +3110,10 @@
     </row>
     <row r="151" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B151" s="4">
-        <v>1221</v>
-      </c>
-      <c r="C151">
-        <v>44616</v>
+        <v>1234</v>
+      </c>
+      <c r="C151" s="10">
+        <v>44646</v>
       </c>
       <c r="D151" s="4"/>
       <c r="E151" s="4"/>
@@ -3144,10 +3123,10 @@
     </row>
     <row r="152" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B152" s="4">
-        <v>1220</v>
-      </c>
-      <c r="C152">
-        <v>44614</v>
+        <v>1233</v>
+      </c>
+      <c r="C152" s="10">
+        <v>44644</v>
       </c>
       <c r="D152" s="4"/>
       <c r="E152" s="4"/>
@@ -3157,10 +3136,10 @@
     </row>
     <row r="153" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B153" s="4">
-        <v>1219</v>
-      </c>
-      <c r="C153">
-        <v>44611</v>
+        <v>1232</v>
+      </c>
+      <c r="C153" s="10">
+        <v>44642</v>
       </c>
       <c r="D153" s="4"/>
       <c r="E153" s="4"/>
@@ -3170,10 +3149,10 @@
     </row>
     <row r="154" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B154" s="4">
-        <v>1218</v>
-      </c>
-      <c r="C154">
-        <v>44609</v>
+        <v>1231</v>
+      </c>
+      <c r="C154" s="10">
+        <v>44639</v>
       </c>
       <c r="D154" s="4"/>
       <c r="E154" s="4"/>
@@ -3183,10 +3162,10 @@
     </row>
     <row r="155" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B155" s="4">
-        <v>1217</v>
-      </c>
-      <c r="C155">
-        <v>44607</v>
+        <v>1230</v>
+      </c>
+      <c r="C155" s="10">
+        <v>44637</v>
       </c>
       <c r="D155" s="4"/>
       <c r="E155" s="4"/>
@@ -3196,10 +3175,10 @@
     </row>
     <row r="156" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B156" s="4">
-        <v>1216</v>
-      </c>
-      <c r="C156">
-        <v>44604</v>
+        <v>1229</v>
+      </c>
+      <c r="C156" s="10">
+        <v>44635</v>
       </c>
       <c r="D156" s="4"/>
       <c r="E156" s="4"/>
@@ -3209,10 +3188,10 @@
     </row>
     <row r="157" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B157" s="4">
-        <v>1215</v>
+        <v>1228</v>
       </c>
       <c r="C157">
-        <v>44602</v>
+        <v>44632</v>
       </c>
       <c r="D157" s="4"/>
       <c r="E157" s="4"/>
@@ -3222,10 +3201,10 @@
     </row>
     <row r="158" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B158" s="4">
-        <v>1214</v>
+        <v>1227</v>
       </c>
       <c r="C158">
-        <v>44600</v>
+        <v>44630</v>
       </c>
       <c r="D158" s="4"/>
       <c r="E158" s="4"/>
@@ -3235,10 +3214,10 @@
     </row>
     <row r="159" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B159" s="4">
-        <v>1213</v>
+        <v>1226</v>
       </c>
       <c r="C159">
-        <v>44597</v>
+        <v>44628</v>
       </c>
       <c r="D159" s="4"/>
       <c r="E159" s="4"/>
@@ -3248,10 +3227,10 @@
     </row>
     <row r="160" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B160" s="4">
-        <v>1212</v>
+        <v>1225</v>
       </c>
       <c r="C160">
-        <v>44595</v>
+        <v>44625</v>
       </c>
       <c r="D160" s="4"/>
       <c r="E160" s="4"/>
@@ -3261,10 +3240,10 @@
     </row>
     <row r="161" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B161" s="4">
-        <v>1211</v>
+        <v>1224</v>
       </c>
       <c r="C161">
-        <v>44593</v>
+        <v>44623</v>
       </c>
       <c r="D161" s="4"/>
       <c r="E161" s="4"/>
@@ -3272,6 +3251,175 @@
       <c r="G161" s="4"/>
       <c r="H161" s="4"/>
     </row>
+    <row r="162" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B162" s="4">
+        <v>1223</v>
+      </c>
+      <c r="C162">
+        <v>44621</v>
+      </c>
+      <c r="D162" s="4"/>
+      <c r="E162" s="4"/>
+      <c r="F162" s="4"/>
+      <c r="G162" s="4"/>
+      <c r="H162" s="4"/>
+    </row>
+    <row r="163" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B163" s="4">
+        <v>1222</v>
+      </c>
+      <c r="C163">
+        <v>44618</v>
+      </c>
+      <c r="D163" s="4"/>
+      <c r="E163" s="4"/>
+      <c r="F163" s="4"/>
+      <c r="G163" s="4"/>
+      <c r="H163" s="4"/>
+    </row>
+    <row r="164" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B164" s="4">
+        <v>1221</v>
+      </c>
+      <c r="C164">
+        <v>44616</v>
+      </c>
+      <c r="D164" s="4"/>
+      <c r="E164" s="4"/>
+      <c r="F164" s="4"/>
+      <c r="G164" s="4"/>
+      <c r="H164" s="4"/>
+    </row>
+    <row r="165" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B165" s="4">
+        <v>1220</v>
+      </c>
+      <c r="C165">
+        <v>44614</v>
+      </c>
+      <c r="D165" s="4"/>
+      <c r="E165" s="4"/>
+      <c r="F165" s="4"/>
+      <c r="G165" s="4"/>
+      <c r="H165" s="4"/>
+    </row>
+    <row r="166" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B166" s="4">
+        <v>1219</v>
+      </c>
+      <c r="C166">
+        <v>44611</v>
+      </c>
+      <c r="D166" s="4"/>
+      <c r="E166" s="4"/>
+      <c r="F166" s="4"/>
+      <c r="G166" s="4"/>
+      <c r="H166" s="4"/>
+    </row>
+    <row r="167" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B167" s="4">
+        <v>1218</v>
+      </c>
+      <c r="C167">
+        <v>44609</v>
+      </c>
+      <c r="D167" s="4"/>
+      <c r="E167" s="4"/>
+      <c r="F167" s="4"/>
+      <c r="G167" s="4"/>
+      <c r="H167" s="4"/>
+    </row>
+    <row r="168" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B168" s="4">
+        <v>1217</v>
+      </c>
+      <c r="C168">
+        <v>44607</v>
+      </c>
+      <c r="D168" s="4"/>
+      <c r="E168" s="4"/>
+      <c r="F168" s="4"/>
+      <c r="G168" s="4"/>
+      <c r="H168" s="4"/>
+    </row>
+    <row r="169" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B169" s="4">
+        <v>1216</v>
+      </c>
+      <c r="C169">
+        <v>44604</v>
+      </c>
+      <c r="D169" s="4"/>
+      <c r="E169" s="4"/>
+      <c r="F169" s="4"/>
+      <c r="G169" s="4"/>
+      <c r="H169" s="4"/>
+    </row>
+    <row r="170" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B170" s="4">
+        <v>1215</v>
+      </c>
+      <c r="C170">
+        <v>44602</v>
+      </c>
+      <c r="D170" s="4"/>
+      <c r="E170" s="4"/>
+      <c r="F170" s="4"/>
+      <c r="G170" s="4"/>
+      <c r="H170" s="4"/>
+    </row>
+    <row r="171" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B171" s="4">
+        <v>1214</v>
+      </c>
+      <c r="C171">
+        <v>44600</v>
+      </c>
+      <c r="D171" s="4"/>
+      <c r="E171" s="4"/>
+      <c r="F171" s="4"/>
+      <c r="G171" s="4"/>
+      <c r="H171" s="4"/>
+    </row>
+    <row r="172" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B172" s="4">
+        <v>1213</v>
+      </c>
+      <c r="C172">
+        <v>44597</v>
+      </c>
+      <c r="D172" s="4"/>
+      <c r="E172" s="4"/>
+      <c r="F172" s="4"/>
+      <c r="G172" s="4"/>
+      <c r="H172" s="4"/>
+    </row>
+    <row r="173" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B173" s="4">
+        <v>1212</v>
+      </c>
+      <c r="C173">
+        <v>44595</v>
+      </c>
+      <c r="D173" s="4"/>
+      <c r="E173" s="4"/>
+      <c r="F173" s="4"/>
+      <c r="G173" s="4"/>
+      <c r="H173" s="4"/>
+    </row>
+    <row r="174" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B174" s="4">
+        <v>1211</v>
+      </c>
+      <c r="C174">
+        <v>44593</v>
+      </c>
+      <c r="D174" s="4"/>
+      <c r="E174" s="4"/>
+      <c r="F174" s="4"/>
+      <c r="G174" s="4"/>
+      <c r="H174" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Update 29-03-2023 -->> Excel
</commit_message>
<xml_diff>
--- a/helps/Historial de Jugadas.xlsx
+++ b/helps/Historial de Jugadas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos\Randon\helps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3942C0C-457C-45E4-9923-7E2CF2DA7CC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBEFBDB-82AD-4ADB-B08A-2D3E59995DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" activeTab="1" xr2:uid="{A3392D85-3030-46DE-B96E-7922EDC7109E}"/>
   </bookViews>
@@ -210,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -239,6 +239,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1187,7 +1190,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15FEB743-8F41-4809-BA70-E7C1EBE37B84}">
-  <dimension ref="A1:H174"/>
+  <dimension ref="A1:H193"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
@@ -1217,7 +1220,7 @@
     <row r="3" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
         <v>1</v>
@@ -1238,32 +1241,32 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B5" s="4"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B6" s="4"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+    <row r="5" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B7" s="4"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B8" s="4"/>
@@ -1293,12 +1296,8 @@
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B11" s="4">
-        <v>1374</v>
-      </c>
-      <c r="C11" s="10">
-        <v>44973</v>
-      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="10"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -1307,10 +1306,10 @@
     </row>
     <row r="12" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B12" s="4">
-        <v>1373</v>
+        <v>1392</v>
       </c>
       <c r="C12" s="10">
-        <v>44971</v>
+        <v>45015</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
@@ -1320,10 +1319,10 @@
     </row>
     <row r="13" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B13" s="4">
-        <v>1372</v>
+        <v>1391</v>
       </c>
       <c r="C13" s="10">
-        <v>44968</v>
+        <v>45013</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -1333,10 +1332,10 @@
     </row>
     <row r="14" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B14" s="4">
-        <v>1371</v>
+        <v>1390</v>
       </c>
       <c r="C14" s="10">
-        <v>44966</v>
+        <v>45010</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
@@ -1346,10 +1345,10 @@
     </row>
     <row r="15" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B15" s="4">
-        <v>1370</v>
+        <v>1389</v>
       </c>
       <c r="C15" s="10">
-        <v>44964</v>
+        <v>45008</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -1359,10 +1358,10 @@
     </row>
     <row r="16" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B16" s="4">
-        <v>1369</v>
+        <v>1388</v>
       </c>
       <c r="C16" s="10">
-        <v>44961</v>
+        <v>45006</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
@@ -1372,10 +1371,10 @@
     </row>
     <row r="17" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B17" s="4">
-        <v>1368</v>
+        <v>1387</v>
       </c>
       <c r="C17" s="10">
-        <v>44959</v>
+        <v>45003</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -1385,10 +1384,10 @@
     </row>
     <row r="18" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B18" s="4">
-        <v>1367</v>
+        <v>1386</v>
       </c>
       <c r="C18" s="10">
-        <v>44957</v>
+        <v>45001</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
@@ -1398,10 +1397,10 @@
     </row>
     <row r="19" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B19" s="4">
-        <v>1366</v>
+        <v>1385</v>
       </c>
       <c r="C19" s="10">
-        <v>44954</v>
+        <v>44999</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
@@ -1411,10 +1410,10 @@
     </row>
     <row r="20" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B20" s="4">
-        <v>1365</v>
+        <v>1384</v>
       </c>
       <c r="C20" s="10">
-        <v>44952</v>
+        <v>44996</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
@@ -1424,10 +1423,10 @@
     </row>
     <row r="21" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B21" s="4">
-        <v>1364</v>
+        <v>1383</v>
       </c>
       <c r="C21" s="10">
-        <v>44950</v>
+        <v>44994</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
@@ -1437,10 +1436,10 @@
     </row>
     <row r="22" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B22" s="4">
-        <v>1363</v>
+        <v>1382</v>
       </c>
       <c r="C22" s="10">
-        <v>44947</v>
+        <v>44992</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
@@ -1450,10 +1449,10 @@
     </row>
     <row r="23" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B23" s="4">
-        <v>1362</v>
+        <v>1381</v>
       </c>
       <c r="C23" s="10">
-        <v>44945</v>
+        <v>44989</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
@@ -1463,10 +1462,10 @@
     </row>
     <row r="24" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B24" s="4">
-        <v>1361</v>
+        <v>1380</v>
       </c>
       <c r="C24" s="10">
-        <v>44943</v>
+        <v>44987</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
@@ -1476,10 +1475,10 @@
     </row>
     <row r="25" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B25" s="4">
-        <v>1360</v>
+        <v>1379</v>
       </c>
       <c r="C25" s="10">
-        <v>44940</v>
+        <v>44985</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
@@ -1489,10 +1488,10 @@
     </row>
     <row r="26" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B26" s="4">
-        <v>1359</v>
+        <v>1378</v>
       </c>
       <c r="C26" s="10">
-        <v>44938</v>
+        <v>44982</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
@@ -1502,10 +1501,10 @@
     </row>
     <row r="27" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B27" s="4">
-        <v>1358</v>
+        <v>1377</v>
       </c>
       <c r="C27" s="10">
-        <v>44936</v>
+        <v>44980</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
@@ -1515,10 +1514,10 @@
     </row>
     <row r="28" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B28" s="4">
-        <v>1357</v>
+        <v>1376</v>
       </c>
       <c r="C28" s="10">
-        <v>44933</v>
+        <v>44978</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
@@ -1528,10 +1527,10 @@
     </row>
     <row r="29" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B29" s="4">
-        <v>1356</v>
+        <v>1375</v>
       </c>
       <c r="C29" s="10">
-        <v>44931</v>
+        <v>44975</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -1541,10 +1540,10 @@
     </row>
     <row r="30" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B30" s="4">
-        <v>1355</v>
+        <v>1374</v>
       </c>
       <c r="C30" s="10">
-        <v>44929</v>
+        <v>44973</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
@@ -1554,10 +1553,10 @@
     </row>
     <row r="31" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B31" s="4">
-        <v>1354</v>
+        <v>1373</v>
       </c>
       <c r="C31" s="10">
-        <v>44926</v>
+        <v>44971</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -1567,10 +1566,10 @@
     </row>
     <row r="32" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B32" s="4">
-        <v>1353</v>
+        <v>1372</v>
       </c>
       <c r="C32" s="10">
-        <v>44924</v>
+        <v>44968</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -1580,10 +1579,10 @@
     </row>
     <row r="33" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B33" s="4">
-        <v>1352</v>
+        <v>1371</v>
       </c>
       <c r="C33" s="10">
-        <v>44922</v>
+        <v>44966</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
@@ -1593,10 +1592,10 @@
     </row>
     <row r="34" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B34" s="4">
-        <v>1351</v>
+        <v>1370</v>
       </c>
       <c r="C34" s="10">
-        <v>44919</v>
+        <v>44964</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
@@ -1606,10 +1605,10 @@
     </row>
     <row r="35" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B35" s="4">
-        <v>1350</v>
+        <v>1369</v>
       </c>
       <c r="C35" s="10">
-        <v>44917</v>
+        <v>44961</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -1619,10 +1618,10 @@
     </row>
     <row r="36" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B36" s="4">
-        <v>1349</v>
+        <v>1368</v>
       </c>
       <c r="C36" s="10">
-        <v>44915</v>
+        <v>44959</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -1632,10 +1631,10 @@
     </row>
     <row r="37" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B37" s="4">
-        <v>1348</v>
+        <v>1367</v>
       </c>
       <c r="C37" s="10">
-        <v>44912</v>
+        <v>44957</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -1645,10 +1644,10 @@
     </row>
     <row r="38" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B38" s="4">
-        <v>1347</v>
+        <v>1366</v>
       </c>
       <c r="C38" s="10">
-        <v>44910</v>
+        <v>44954</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
@@ -1658,10 +1657,10 @@
     </row>
     <row r="39" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B39" s="4">
-        <v>1346</v>
+        <v>1365</v>
       </c>
       <c r="C39" s="10">
-        <v>44908</v>
+        <v>44952</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
@@ -1671,10 +1670,10 @@
     </row>
     <row r="40" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B40" s="4">
-        <v>1345</v>
+        <v>1364</v>
       </c>
       <c r="C40" s="10">
-        <v>44905</v>
+        <v>44950</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
@@ -1684,10 +1683,10 @@
     </row>
     <row r="41" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B41" s="4">
-        <v>1344</v>
+        <v>1363</v>
       </c>
       <c r="C41" s="10">
-        <v>44903</v>
+        <v>44947</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
@@ -1697,10 +1696,10 @@
     </row>
     <row r="42" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B42" s="4">
-        <v>1343</v>
+        <v>1362</v>
       </c>
       <c r="C42" s="10">
-        <v>44901</v>
+        <v>44945</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
@@ -1710,10 +1709,10 @@
     </row>
     <row r="43" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B43" s="4">
-        <v>1342</v>
+        <v>1361</v>
       </c>
       <c r="C43" s="10">
-        <v>44898</v>
+        <v>44943</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
@@ -1723,10 +1722,10 @@
     </row>
     <row r="44" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B44" s="4">
-        <v>1341</v>
+        <v>1360</v>
       </c>
       <c r="C44" s="10">
-        <v>44896</v>
+        <v>44940</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -1736,10 +1735,10 @@
     </row>
     <row r="45" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B45" s="4">
-        <v>1340</v>
+        <v>1359</v>
       </c>
       <c r="C45" s="10">
-        <v>44894</v>
+        <v>44938</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
@@ -1749,10 +1748,10 @@
     </row>
     <row r="46" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B46" s="4">
-        <v>1339</v>
+        <v>1358</v>
       </c>
       <c r="C46" s="10">
-        <v>44891</v>
+        <v>44936</v>
       </c>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
@@ -1762,12 +1761,12 @@
     </row>
     <row r="47" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B47" s="4">
-        <v>1338</v>
+        <v>1357</v>
       </c>
       <c r="C47" s="10">
-        <v>44889</v>
-      </c>
-      <c r="D47" s="10"/>
+        <v>44933</v>
+      </c>
+      <c r="D47" s="4"/>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
@@ -1775,10 +1774,10 @@
     </row>
     <row r="48" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B48" s="4">
-        <v>1337</v>
+        <v>1356</v>
       </c>
       <c r="C48" s="10">
-        <v>44887</v>
+        <v>44931</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
@@ -1788,10 +1787,10 @@
     </row>
     <row r="49" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B49" s="4">
-        <v>1336</v>
+        <v>1355</v>
       </c>
       <c r="C49" s="10">
-        <v>44884</v>
+        <v>44929</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
@@ -1801,10 +1800,10 @@
     </row>
     <row r="50" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B50" s="4">
-        <v>1335</v>
+        <v>1354</v>
       </c>
       <c r="C50" s="10">
-        <v>44882</v>
+        <v>44926</v>
       </c>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
@@ -1814,10 +1813,10 @@
     </row>
     <row r="51" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B51" s="4">
-        <v>1334</v>
+        <v>1353</v>
       </c>
       <c r="C51" s="10">
-        <v>44880</v>
+        <v>44924</v>
       </c>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
@@ -1827,10 +1826,10 @@
     </row>
     <row r="52" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B52" s="4">
-        <v>1333</v>
+        <v>1352</v>
       </c>
       <c r="C52" s="10">
-        <v>44877</v>
+        <v>44922</v>
       </c>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
@@ -1840,10 +1839,10 @@
     </row>
     <row r="53" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B53" s="4">
-        <v>1332</v>
+        <v>1351</v>
       </c>
       <c r="C53" s="10">
-        <v>44875</v>
+        <v>44919</v>
       </c>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
@@ -1853,10 +1852,10 @@
     </row>
     <row r="54" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B54" s="4">
-        <v>1331</v>
+        <v>1350</v>
       </c>
       <c r="C54" s="10">
-        <v>44873</v>
+        <v>44917</v>
       </c>
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
@@ -1866,10 +1865,10 @@
     </row>
     <row r="55" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B55" s="4">
-        <v>1330</v>
+        <v>1349</v>
       </c>
       <c r="C55" s="10">
-        <v>44870</v>
+        <v>44915</v>
       </c>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
@@ -1879,10 +1878,10 @@
     </row>
     <row r="56" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B56" s="4">
-        <v>1329</v>
+        <v>1348</v>
       </c>
       <c r="C56" s="10">
-        <v>44868</v>
+        <v>44912</v>
       </c>
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
@@ -1892,10 +1891,10 @@
     </row>
     <row r="57" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B57" s="4">
-        <v>1328</v>
+        <v>1347</v>
       </c>
       <c r="C57" s="10">
-        <v>44866</v>
+        <v>44910</v>
       </c>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
@@ -1905,10 +1904,10 @@
     </row>
     <row r="58" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B58" s="4">
-        <v>1327</v>
+        <v>1346</v>
       </c>
       <c r="C58" s="10">
-        <v>44863</v>
+        <v>44908</v>
       </c>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
@@ -1918,10 +1917,10 @@
     </row>
     <row r="59" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B59" s="4">
-        <v>1326</v>
+        <v>1345</v>
       </c>
       <c r="C59" s="10">
-        <v>44861</v>
+        <v>44905</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
@@ -1931,10 +1930,10 @@
     </row>
     <row r="60" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B60" s="4">
-        <v>1325</v>
+        <v>1344</v>
       </c>
       <c r="C60" s="10">
-        <v>44859</v>
+        <v>44903</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
@@ -1944,10 +1943,10 @@
     </row>
     <row r="61" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B61" s="4">
-        <v>1324</v>
+        <v>1343</v>
       </c>
       <c r="C61" s="10">
-        <v>44856</v>
+        <v>44901</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
@@ -1957,10 +1956,10 @@
     </row>
     <row r="62" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B62" s="4">
-        <v>1323</v>
+        <v>1342</v>
       </c>
       <c r="C62" s="10">
-        <v>44854</v>
+        <v>44898</v>
       </c>
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
@@ -1970,10 +1969,10 @@
     </row>
     <row r="63" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B63" s="4">
-        <v>1322</v>
+        <v>1341</v>
       </c>
       <c r="C63" s="10">
-        <v>44852</v>
+        <v>44896</v>
       </c>
       <c r="D63" s="4"/>
       <c r="E63" s="4"/>
@@ -1983,10 +1982,10 @@
     </row>
     <row r="64" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B64" s="4">
-        <v>1321</v>
+        <v>1340</v>
       </c>
       <c r="C64" s="10">
-        <v>44849</v>
+        <v>44894</v>
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="4"/>
@@ -1996,10 +1995,10 @@
     </row>
     <row r="65" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B65" s="4">
-        <v>1320</v>
+        <v>1339</v>
       </c>
       <c r="C65" s="10">
-        <v>44847</v>
+        <v>44891</v>
       </c>
       <c r="D65" s="4"/>
       <c r="E65" s="4"/>
@@ -2009,12 +2008,12 @@
     </row>
     <row r="66" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B66" s="4">
-        <v>1319</v>
+        <v>1338</v>
       </c>
       <c r="C66" s="10">
-        <v>44845</v>
-      </c>
-      <c r="D66" s="4"/>
+        <v>44889</v>
+      </c>
+      <c r="D66" s="10"/>
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
       <c r="G66" s="4"/>
@@ -2022,10 +2021,10 @@
     </row>
     <row r="67" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B67" s="4">
-        <v>1318</v>
+        <v>1337</v>
       </c>
       <c r="C67" s="10">
-        <v>44842</v>
+        <v>44887</v>
       </c>
       <c r="D67" s="4"/>
       <c r="E67" s="4"/>
@@ -2035,10 +2034,10 @@
     </row>
     <row r="68" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B68" s="4">
-        <v>1317</v>
+        <v>1336</v>
       </c>
       <c r="C68" s="10">
-        <v>44840</v>
+        <v>44884</v>
       </c>
       <c r="D68" s="4"/>
       <c r="E68" s="4"/>
@@ -2048,10 +2047,10 @@
     </row>
     <row r="69" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B69" s="4">
-        <v>1316</v>
+        <v>1335</v>
       </c>
       <c r="C69" s="10">
-        <v>44838</v>
+        <v>44882</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69" s="4"/>
@@ -2061,10 +2060,10 @@
     </row>
     <row r="70" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B70" s="4">
-        <v>1315</v>
+        <v>1334</v>
       </c>
       <c r="C70" s="10">
-        <v>44835</v>
+        <v>44880</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="4"/>
@@ -2074,10 +2073,10 @@
     </row>
     <row r="71" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B71" s="4">
-        <v>1314</v>
+        <v>1333</v>
       </c>
       <c r="C71" s="10">
-        <v>44833</v>
+        <v>44877</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" s="4"/>
@@ -2087,10 +2086,10 @@
     </row>
     <row r="72" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B72" s="4">
-        <v>1313</v>
+        <v>1332</v>
       </c>
       <c r="C72" s="10">
-        <v>44831</v>
+        <v>44875</v>
       </c>
       <c r="D72" s="4"/>
       <c r="E72" s="4"/>
@@ -2100,10 +2099,10 @@
     </row>
     <row r="73" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B73" s="4">
-        <v>1312</v>
+        <v>1331</v>
       </c>
       <c r="C73" s="10">
-        <v>44828</v>
+        <v>44873</v>
       </c>
       <c r="D73" s="4"/>
       <c r="E73" s="4"/>
@@ -2113,10 +2112,10 @@
     </row>
     <row r="74" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B74" s="4">
-        <v>1311</v>
+        <v>1330</v>
       </c>
       <c r="C74" s="10">
-        <v>44826</v>
+        <v>44870</v>
       </c>
       <c r="D74" s="4"/>
       <c r="E74" s="4"/>
@@ -2126,10 +2125,10 @@
     </row>
     <row r="75" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B75" s="4">
-        <v>1310</v>
+        <v>1329</v>
       </c>
       <c r="C75" s="10">
-        <v>44824</v>
+        <v>44868</v>
       </c>
       <c r="D75" s="4"/>
       <c r="E75" s="4"/>
@@ -2139,10 +2138,10 @@
     </row>
     <row r="76" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B76" s="4">
-        <v>1309</v>
+        <v>1328</v>
       </c>
       <c r="C76" s="10">
-        <v>44821</v>
+        <v>44866</v>
       </c>
       <c r="D76" s="4"/>
       <c r="E76" s="4"/>
@@ -2152,10 +2151,10 @@
     </row>
     <row r="77" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B77" s="4">
-        <v>1308</v>
+        <v>1327</v>
       </c>
       <c r="C77" s="10">
-        <v>44819</v>
+        <v>44863</v>
       </c>
       <c r="D77" s="4"/>
       <c r="E77" s="4"/>
@@ -2165,10 +2164,10 @@
     </row>
     <row r="78" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B78" s="4">
-        <v>1307</v>
+        <v>1326</v>
       </c>
       <c r="C78" s="10">
-        <v>44817</v>
+        <v>44861</v>
       </c>
       <c r="D78" s="4"/>
       <c r="E78" s="4"/>
@@ -2178,10 +2177,10 @@
     </row>
     <row r="79" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B79" s="4">
-        <v>1306</v>
+        <v>1325</v>
       </c>
       <c r="C79" s="10">
-        <v>44814</v>
+        <v>44859</v>
       </c>
       <c r="D79" s="4"/>
       <c r="E79" s="4"/>
@@ -2191,10 +2190,10 @@
     </row>
     <row r="80" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B80" s="4">
-        <v>1305</v>
+        <v>1324</v>
       </c>
       <c r="C80" s="10">
-        <v>44812</v>
+        <v>44856</v>
       </c>
       <c r="D80" s="4"/>
       <c r="E80" s="4"/>
@@ -2204,10 +2203,10 @@
     </row>
     <row r="81" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B81" s="4">
-        <v>1304</v>
+        <v>1323</v>
       </c>
       <c r="C81" s="10">
-        <v>44810</v>
+        <v>44854</v>
       </c>
       <c r="D81" s="4"/>
       <c r="E81" s="4"/>
@@ -2217,10 +2216,10 @@
     </row>
     <row r="82" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B82" s="4">
-        <v>1303</v>
+        <v>1322</v>
       </c>
       <c r="C82" s="10">
-        <v>44807</v>
+        <v>44852</v>
       </c>
       <c r="D82" s="4"/>
       <c r="E82" s="4"/>
@@ -2230,10 +2229,10 @@
     </row>
     <row r="83" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B83" s="4">
-        <v>1302</v>
+        <v>1321</v>
       </c>
       <c r="C83" s="10">
-        <v>44805</v>
+        <v>44849</v>
       </c>
       <c r="D83" s="4"/>
       <c r="E83" s="4"/>
@@ -2243,10 +2242,10 @@
     </row>
     <row r="84" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B84" s="4">
-        <v>1301</v>
+        <v>1320</v>
       </c>
       <c r="C84" s="10">
-        <v>44803</v>
+        <v>44847</v>
       </c>
       <c r="D84" s="4"/>
       <c r="E84" s="4"/>
@@ -2256,10 +2255,10 @@
     </row>
     <row r="85" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B85" s="4">
-        <v>1300</v>
+        <v>1319</v>
       </c>
       <c r="C85" s="10">
-        <v>44800</v>
+        <v>44845</v>
       </c>
       <c r="D85" s="4"/>
       <c r="E85" s="4"/>
@@ -2269,10 +2268,10 @@
     </row>
     <row r="86" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B86" s="4">
-        <v>1299</v>
+        <v>1318</v>
       </c>
       <c r="C86" s="10">
-        <v>44798</v>
+        <v>44842</v>
       </c>
       <c r="D86" s="4"/>
       <c r="E86" s="4"/>
@@ -2282,10 +2281,10 @@
     </row>
     <row r="87" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B87" s="4">
-        <v>1298</v>
+        <v>1317</v>
       </c>
       <c r="C87" s="10">
-        <v>44796</v>
+        <v>44840</v>
       </c>
       <c r="D87" s="4"/>
       <c r="E87" s="4"/>
@@ -2295,10 +2294,10 @@
     </row>
     <row r="88" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B88" s="4">
-        <v>1297</v>
+        <v>1316</v>
       </c>
       <c r="C88" s="10">
-        <v>44793</v>
+        <v>44838</v>
       </c>
       <c r="D88" s="4"/>
       <c r="E88" s="4"/>
@@ -2308,10 +2307,10 @@
     </row>
     <row r="89" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B89" s="4">
-        <v>1296</v>
+        <v>1315</v>
       </c>
       <c r="C89" s="10">
-        <v>44791</v>
+        <v>44835</v>
       </c>
       <c r="D89" s="4"/>
       <c r="E89" s="4"/>
@@ -2321,10 +2320,10 @@
     </row>
     <row r="90" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B90" s="4">
-        <v>1295</v>
+        <v>1314</v>
       </c>
       <c r="C90" s="10">
-        <v>44789</v>
+        <v>44833</v>
       </c>
       <c r="D90" s="4"/>
       <c r="E90" s="4"/>
@@ -2334,10 +2333,10 @@
     </row>
     <row r="91" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B91" s="4">
-        <v>1294</v>
+        <v>1313</v>
       </c>
       <c r="C91" s="10">
-        <v>44786</v>
+        <v>44831</v>
       </c>
       <c r="D91" s="4"/>
       <c r="E91" s="4"/>
@@ -2347,10 +2346,10 @@
     </row>
     <row r="92" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B92" s="4">
-        <v>1293</v>
+        <v>1312</v>
       </c>
       <c r="C92" s="10">
-        <v>44784</v>
+        <v>44828</v>
       </c>
       <c r="D92" s="4"/>
       <c r="E92" s="4"/>
@@ -2360,10 +2359,10 @@
     </row>
     <row r="93" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B93" s="4">
-        <v>1292</v>
+        <v>1311</v>
       </c>
       <c r="C93" s="10">
-        <v>44782</v>
+        <v>44826</v>
       </c>
       <c r="D93" s="4"/>
       <c r="E93" s="4"/>
@@ -2373,10 +2372,10 @@
     </row>
     <row r="94" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B94" s="4">
-        <v>1291</v>
+        <v>1310</v>
       </c>
       <c r="C94" s="10">
-        <v>44779</v>
+        <v>44824</v>
       </c>
       <c r="D94" s="4"/>
       <c r="E94" s="4"/>
@@ -2386,10 +2385,10 @@
     </row>
     <row r="95" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B95" s="4">
-        <v>1290</v>
+        <v>1309</v>
       </c>
       <c r="C95" s="10">
-        <v>44777</v>
+        <v>44821</v>
       </c>
       <c r="D95" s="4"/>
       <c r="E95" s="4"/>
@@ -2399,10 +2398,10 @@
     </row>
     <row r="96" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B96" s="4">
-        <v>1289</v>
+        <v>1308</v>
       </c>
       <c r="C96" s="10">
-        <v>44775</v>
+        <v>44819</v>
       </c>
       <c r="D96" s="4"/>
       <c r="E96" s="4"/>
@@ -2412,10 +2411,10 @@
     </row>
     <row r="97" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B97" s="4">
-        <v>1288</v>
+        <v>1307</v>
       </c>
       <c r="C97" s="10">
-        <v>44772</v>
+        <v>44817</v>
       </c>
       <c r="D97" s="4"/>
       <c r="E97" s="4"/>
@@ -2425,10 +2424,10 @@
     </row>
     <row r="98" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B98" s="4">
-        <v>1287</v>
+        <v>1306</v>
       </c>
       <c r="C98" s="10">
-        <v>44770</v>
+        <v>44814</v>
       </c>
       <c r="D98" s="4"/>
       <c r="E98" s="4"/>
@@ -2438,10 +2437,10 @@
     </row>
     <row r="99" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B99" s="4">
-        <v>1286</v>
+        <v>1305</v>
       </c>
       <c r="C99" s="10">
-        <v>44768</v>
+        <v>44812</v>
       </c>
       <c r="D99" s="4"/>
       <c r="E99" s="4"/>
@@ -2451,10 +2450,10 @@
     </row>
     <row r="100" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B100" s="4">
-        <v>1285</v>
+        <v>1304</v>
       </c>
       <c r="C100" s="10">
-        <v>44765</v>
+        <v>44810</v>
       </c>
       <c r="D100" s="4"/>
       <c r="E100" s="4"/>
@@ -2464,10 +2463,10 @@
     </row>
     <row r="101" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B101" s="4">
-        <v>1284</v>
+        <v>1303</v>
       </c>
       <c r="C101" s="10">
-        <v>44763</v>
+        <v>44807</v>
       </c>
       <c r="D101" s="4"/>
       <c r="E101" s="4"/>
@@ -2477,10 +2476,10 @@
     </row>
     <row r="102" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B102" s="4">
-        <v>1283</v>
+        <v>1302</v>
       </c>
       <c r="C102" s="10">
-        <v>44761</v>
+        <v>44805</v>
       </c>
       <c r="D102" s="4"/>
       <c r="E102" s="4"/>
@@ -2490,10 +2489,10 @@
     </row>
     <row r="103" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B103" s="4">
-        <v>1282</v>
+        <v>1301</v>
       </c>
       <c r="C103" s="10">
-        <v>44758</v>
+        <v>44803</v>
       </c>
       <c r="D103" s="4"/>
       <c r="E103" s="4"/>
@@ -2503,10 +2502,10 @@
     </row>
     <row r="104" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B104" s="4">
-        <v>1281</v>
+        <v>1300</v>
       </c>
       <c r="C104" s="10">
-        <v>44756</v>
+        <v>44800</v>
       </c>
       <c r="D104" s="4"/>
       <c r="E104" s="4"/>
@@ -2516,10 +2515,10 @@
     </row>
     <row r="105" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B105" s="4">
-        <v>1280</v>
+        <v>1299</v>
       </c>
       <c r="C105" s="10">
-        <v>44754</v>
+        <v>44798</v>
       </c>
       <c r="D105" s="4"/>
       <c r="E105" s="4"/>
@@ -2529,10 +2528,10 @@
     </row>
     <row r="106" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B106" s="4">
-        <v>1279</v>
+        <v>1298</v>
       </c>
       <c r="C106" s="10">
-        <v>44751</v>
+        <v>44796</v>
       </c>
       <c r="D106" s="4"/>
       <c r="E106" s="4"/>
@@ -2542,10 +2541,10 @@
     </row>
     <row r="107" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B107" s="4">
-        <v>1278</v>
+        <v>1297</v>
       </c>
       <c r="C107" s="10">
-        <v>44749</v>
+        <v>44793</v>
       </c>
       <c r="D107" s="4"/>
       <c r="E107" s="4"/>
@@ -2555,10 +2554,10 @@
     </row>
     <row r="108" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B108" s="4">
-        <v>1277</v>
+        <v>1296</v>
       </c>
       <c r="C108" s="10">
-        <v>44747</v>
+        <v>44791</v>
       </c>
       <c r="D108" s="4"/>
       <c r="E108" s="4"/>
@@ -2568,10 +2567,10 @@
     </row>
     <row r="109" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B109" s="4">
-        <v>1276</v>
+        <v>1295</v>
       </c>
       <c r="C109" s="10">
-        <v>44744</v>
+        <v>44789</v>
       </c>
       <c r="D109" s="4"/>
       <c r="E109" s="4"/>
@@ -2581,10 +2580,10 @@
     </row>
     <row r="110" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B110" s="4">
-        <v>1275</v>
+        <v>1294</v>
       </c>
       <c r="C110" s="10">
-        <v>44742</v>
+        <v>44786</v>
       </c>
       <c r="D110" s="4"/>
       <c r="E110" s="4"/>
@@ -2594,10 +2593,10 @@
     </row>
     <row r="111" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B111" s="4">
-        <v>1274</v>
+        <v>1293</v>
       </c>
       <c r="C111" s="10">
-        <v>44740</v>
+        <v>44784</v>
       </c>
       <c r="D111" s="4"/>
       <c r="E111" s="4"/>
@@ -2607,10 +2606,10 @@
     </row>
     <row r="112" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B112" s="4">
-        <v>1273</v>
+        <v>1292</v>
       </c>
       <c r="C112" s="10">
-        <v>44737</v>
+        <v>44782</v>
       </c>
       <c r="D112" s="4"/>
       <c r="E112" s="4"/>
@@ -2620,10 +2619,10 @@
     </row>
     <row r="113" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B113" s="4">
-        <v>1272</v>
+        <v>1291</v>
       </c>
       <c r="C113" s="10">
-        <v>44735</v>
+        <v>44779</v>
       </c>
       <c r="D113" s="4"/>
       <c r="E113" s="4"/>
@@ -2633,10 +2632,10 @@
     </row>
     <row r="114" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B114" s="4">
-        <v>1271</v>
+        <v>1290</v>
       </c>
       <c r="C114" s="10">
-        <v>44733</v>
+        <v>44777</v>
       </c>
       <c r="D114" s="4"/>
       <c r="E114" s="4"/>
@@ -2646,10 +2645,10 @@
     </row>
     <row r="115" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B115" s="4">
-        <v>1270</v>
+        <v>1289</v>
       </c>
       <c r="C115" s="10">
-        <v>44730</v>
+        <v>44775</v>
       </c>
       <c r="D115" s="4"/>
       <c r="E115" s="4"/>
@@ -2659,10 +2658,10 @@
     </row>
     <row r="116" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B116" s="4">
-        <v>1269</v>
+        <v>1288</v>
       </c>
       <c r="C116" s="10">
-        <v>44728</v>
+        <v>44772</v>
       </c>
       <c r="D116" s="4"/>
       <c r="E116" s="4"/>
@@ -2672,10 +2671,10 @@
     </row>
     <row r="117" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B117" s="4">
-        <v>1268</v>
+        <v>1287</v>
       </c>
       <c r="C117" s="10">
-        <v>44726</v>
+        <v>44770</v>
       </c>
       <c r="D117" s="4"/>
       <c r="E117" s="4"/>
@@ -2685,10 +2684,10 @@
     </row>
     <row r="118" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B118" s="4">
-        <v>1267</v>
+        <v>1286</v>
       </c>
       <c r="C118" s="10">
-        <v>44723</v>
+        <v>44768</v>
       </c>
       <c r="D118" s="4"/>
       <c r="E118" s="4"/>
@@ -2698,10 +2697,10 @@
     </row>
     <row r="119" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B119" s="4">
-        <v>1266</v>
+        <v>1285</v>
       </c>
       <c r="C119" s="10">
-        <v>44721</v>
+        <v>44765</v>
       </c>
       <c r="D119" s="4"/>
       <c r="E119" s="4"/>
@@ -2711,10 +2710,10 @@
     </row>
     <row r="120" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B120" s="4">
-        <v>1265</v>
+        <v>1284</v>
       </c>
       <c r="C120" s="10">
-        <v>44719</v>
+        <v>44763</v>
       </c>
       <c r="D120" s="4"/>
       <c r="E120" s="4"/>
@@ -2724,10 +2723,10 @@
     </row>
     <row r="121" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B121" s="4">
-        <v>1264</v>
+        <v>1283</v>
       </c>
       <c r="C121" s="10">
-        <v>44716</v>
+        <v>44761</v>
       </c>
       <c r="D121" s="4"/>
       <c r="E121" s="4"/>
@@ -2737,10 +2736,10 @@
     </row>
     <row r="122" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B122" s="4">
-        <v>1263</v>
+        <v>1282</v>
       </c>
       <c r="C122" s="10">
-        <v>44714</v>
+        <v>44758</v>
       </c>
       <c r="D122" s="4"/>
       <c r="E122" s="4"/>
@@ -2750,10 +2749,10 @@
     </row>
     <row r="123" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B123" s="4">
-        <v>1262</v>
+        <v>1281</v>
       </c>
       <c r="C123" s="10">
-        <v>44712</v>
+        <v>44756</v>
       </c>
       <c r="D123" s="4"/>
       <c r="E123" s="4"/>
@@ -2763,10 +2762,10 @@
     </row>
     <row r="124" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B124" s="4">
-        <v>1261</v>
+        <v>1280</v>
       </c>
       <c r="C124" s="10">
-        <v>44709</v>
+        <v>44754</v>
       </c>
       <c r="D124" s="4"/>
       <c r="E124" s="4"/>
@@ -2776,10 +2775,10 @@
     </row>
     <row r="125" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B125" s="4">
-        <v>1260</v>
+        <v>1279</v>
       </c>
       <c r="C125" s="10">
-        <v>44707</v>
+        <v>44751</v>
       </c>
       <c r="D125" s="4"/>
       <c r="E125" s="4"/>
@@ -2789,10 +2788,10 @@
     </row>
     <row r="126" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B126" s="4">
-        <v>1259</v>
+        <v>1278</v>
       </c>
       <c r="C126" s="10">
-        <v>44705</v>
+        <v>44749</v>
       </c>
       <c r="D126" s="4"/>
       <c r="E126" s="4"/>
@@ -2802,10 +2801,10 @@
     </row>
     <row r="127" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B127" s="4">
-        <v>1258</v>
+        <v>1277</v>
       </c>
       <c r="C127" s="10">
-        <v>44702</v>
+        <v>44747</v>
       </c>
       <c r="D127" s="4"/>
       <c r="E127" s="4"/>
@@ -2815,10 +2814,10 @@
     </row>
     <row r="128" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B128" s="4">
-        <v>1257</v>
+        <v>1276</v>
       </c>
       <c r="C128" s="10">
-        <v>44700</v>
+        <v>44744</v>
       </c>
       <c r="D128" s="4"/>
       <c r="E128" s="4"/>
@@ -2828,10 +2827,10 @@
     </row>
     <row r="129" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B129" s="4">
-        <v>1256</v>
+        <v>1275</v>
       </c>
       <c r="C129" s="10">
-        <v>44698</v>
+        <v>44742</v>
       </c>
       <c r="D129" s="4"/>
       <c r="E129" s="4"/>
@@ -2841,10 +2840,10 @@
     </row>
     <row r="130" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B130" s="4">
-        <v>1255</v>
+        <v>1274</v>
       </c>
       <c r="C130" s="10">
-        <v>44695</v>
+        <v>44740</v>
       </c>
       <c r="D130" s="4"/>
       <c r="E130" s="4"/>
@@ -2854,10 +2853,10 @@
     </row>
     <row r="131" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B131" s="4">
-        <v>1254</v>
+        <v>1273</v>
       </c>
       <c r="C131" s="10">
-        <v>44693</v>
+        <v>44737</v>
       </c>
       <c r="D131" s="4"/>
       <c r="E131" s="4"/>
@@ -2867,10 +2866,10 @@
     </row>
     <row r="132" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B132" s="4">
-        <v>1253</v>
+        <v>1272</v>
       </c>
       <c r="C132" s="10">
-        <v>44691</v>
+        <v>44735</v>
       </c>
       <c r="D132" s="4"/>
       <c r="E132" s="4"/>
@@ -2880,10 +2879,10 @@
     </row>
     <row r="133" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B133" s="4">
-        <v>1252</v>
+        <v>1271</v>
       </c>
       <c r="C133" s="10">
-        <v>44688</v>
+        <v>44733</v>
       </c>
       <c r="D133" s="4"/>
       <c r="E133" s="4"/>
@@ -2893,10 +2892,10 @@
     </row>
     <row r="134" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B134" s="4">
-        <v>1251</v>
+        <v>1270</v>
       </c>
       <c r="C134" s="10">
-        <v>44686</v>
+        <v>44730</v>
       </c>
       <c r="D134" s="4"/>
       <c r="E134" s="4"/>
@@ -2906,10 +2905,10 @@
     </row>
     <row r="135" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B135" s="4">
-        <v>1250</v>
+        <v>1269</v>
       </c>
       <c r="C135" s="10">
-        <v>44684</v>
+        <v>44728</v>
       </c>
       <c r="D135" s="4"/>
       <c r="E135" s="4"/>
@@ -2919,10 +2918,10 @@
     </row>
     <row r="136" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B136" s="4">
-        <v>1249</v>
+        <v>1268</v>
       </c>
       <c r="C136" s="10">
-        <v>44681</v>
+        <v>44726</v>
       </c>
       <c r="D136" s="4"/>
       <c r="E136" s="4"/>
@@ -2932,10 +2931,10 @@
     </row>
     <row r="137" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B137" s="4">
-        <v>1248</v>
+        <v>1267</v>
       </c>
       <c r="C137" s="10">
-        <v>44679</v>
+        <v>44723</v>
       </c>
       <c r="D137" s="4"/>
       <c r="E137" s="4"/>
@@ -2945,10 +2944,10 @@
     </row>
     <row r="138" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B138" s="4">
-        <v>1247</v>
+        <v>1266</v>
       </c>
       <c r="C138" s="10">
-        <v>44677</v>
+        <v>44721</v>
       </c>
       <c r="D138" s="4"/>
       <c r="E138" s="4"/>
@@ -2958,10 +2957,10 @@
     </row>
     <row r="139" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B139" s="4">
-        <v>1246</v>
+        <v>1265</v>
       </c>
       <c r="C139" s="10">
-        <v>44674</v>
+        <v>44719</v>
       </c>
       <c r="D139" s="4"/>
       <c r="E139" s="4"/>
@@ -2971,10 +2970,10 @@
     </row>
     <row r="140" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B140" s="4">
-        <v>1245</v>
+        <v>1264</v>
       </c>
       <c r="C140" s="10">
-        <v>44672</v>
+        <v>44716</v>
       </c>
       <c r="D140" s="4"/>
       <c r="E140" s="4"/>
@@ -2984,10 +2983,10 @@
     </row>
     <row r="141" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B141" s="4">
-        <v>1244</v>
+        <v>1263</v>
       </c>
       <c r="C141" s="10">
-        <v>44670</v>
+        <v>44714</v>
       </c>
       <c r="D141" s="4"/>
       <c r="E141" s="4"/>
@@ -2997,10 +2996,10 @@
     </row>
     <row r="142" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B142" s="4">
-        <v>1243</v>
+        <v>1262</v>
       </c>
       <c r="C142" s="10">
-        <v>44667</v>
+        <v>44712</v>
       </c>
       <c r="D142" s="4"/>
       <c r="E142" s="4"/>
@@ -3010,10 +3009,10 @@
     </row>
     <row r="143" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B143" s="4">
-        <v>1242</v>
+        <v>1261</v>
       </c>
       <c r="C143" s="10">
-        <v>44665</v>
+        <v>44709</v>
       </c>
       <c r="D143" s="4"/>
       <c r="E143" s="4"/>
@@ -3023,10 +3022,10 @@
     </row>
     <row r="144" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B144" s="4">
-        <v>1241</v>
+        <v>1260</v>
       </c>
       <c r="C144" s="10">
-        <v>44663</v>
+        <v>44707</v>
       </c>
       <c r="D144" s="4"/>
       <c r="E144" s="4"/>
@@ -3036,10 +3035,10 @@
     </row>
     <row r="145" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B145" s="4">
-        <v>1240</v>
+        <v>1259</v>
       </c>
       <c r="C145" s="10">
-        <v>44660</v>
+        <v>44705</v>
       </c>
       <c r="D145" s="4"/>
       <c r="E145" s="4"/>
@@ -3049,10 +3048,10 @@
     </row>
     <row r="146" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B146" s="4">
-        <v>1239</v>
+        <v>1258</v>
       </c>
       <c r="C146" s="10">
-        <v>44658</v>
+        <v>44702</v>
       </c>
       <c r="D146" s="4"/>
       <c r="E146" s="4"/>
@@ -3062,10 +3061,10 @@
     </row>
     <row r="147" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B147" s="4">
-        <v>1238</v>
+        <v>1257</v>
       </c>
       <c r="C147" s="10">
-        <v>44656</v>
+        <v>44700</v>
       </c>
       <c r="D147" s="4"/>
       <c r="E147" s="4"/>
@@ -3075,10 +3074,10 @@
     </row>
     <row r="148" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B148" s="4">
-        <v>1237</v>
+        <v>1256</v>
       </c>
       <c r="C148" s="10">
-        <v>44653</v>
+        <v>44698</v>
       </c>
       <c r="D148" s="4"/>
       <c r="E148" s="4"/>
@@ -3088,10 +3087,10 @@
     </row>
     <row r="149" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B149" s="4">
-        <v>1236</v>
+        <v>1255</v>
       </c>
       <c r="C149" s="10">
-        <v>44651</v>
+        <v>44695</v>
       </c>
       <c r="D149" s="4"/>
       <c r="E149" s="4"/>
@@ -3101,10 +3100,10 @@
     </row>
     <row r="150" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B150" s="4">
-        <v>1235</v>
+        <v>1254</v>
       </c>
       <c r="C150" s="10">
-        <v>44649</v>
+        <v>44693</v>
       </c>
       <c r="D150" s="4"/>
       <c r="E150" s="4"/>
@@ -3114,10 +3113,10 @@
     </row>
     <row r="151" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B151" s="4">
-        <v>1234</v>
+        <v>1253</v>
       </c>
       <c r="C151" s="10">
-        <v>44646</v>
+        <v>44691</v>
       </c>
       <c r="D151" s="4"/>
       <c r="E151" s="4"/>
@@ -3127,10 +3126,10 @@
     </row>
     <row r="152" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B152" s="4">
-        <v>1233</v>
+        <v>1252</v>
       </c>
       <c r="C152" s="10">
-        <v>44644</v>
+        <v>44688</v>
       </c>
       <c r="D152" s="4"/>
       <c r="E152" s="4"/>
@@ -3140,10 +3139,10 @@
     </row>
     <row r="153" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B153" s="4">
-        <v>1232</v>
+        <v>1251</v>
       </c>
       <c r="C153" s="10">
-        <v>44642</v>
+        <v>44686</v>
       </c>
       <c r="D153" s="4"/>
       <c r="E153" s="4"/>
@@ -3153,10 +3152,10 @@
     </row>
     <row r="154" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B154" s="4">
-        <v>1231</v>
+        <v>1250</v>
       </c>
       <c r="C154" s="10">
-        <v>44639</v>
+        <v>44684</v>
       </c>
       <c r="D154" s="4"/>
       <c r="E154" s="4"/>
@@ -3166,10 +3165,10 @@
     </row>
     <row r="155" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B155" s="4">
-        <v>1230</v>
+        <v>1249</v>
       </c>
       <c r="C155" s="10">
-        <v>44637</v>
+        <v>44681</v>
       </c>
       <c r="D155" s="4"/>
       <c r="E155" s="4"/>
@@ -3179,10 +3178,10 @@
     </row>
     <row r="156" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B156" s="4">
-        <v>1229</v>
+        <v>1248</v>
       </c>
       <c r="C156" s="10">
-        <v>44635</v>
+        <v>44679</v>
       </c>
       <c r="D156" s="4"/>
       <c r="E156" s="4"/>
@@ -3192,10 +3191,10 @@
     </row>
     <row r="157" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B157" s="4">
-        <v>1228</v>
-      </c>
-      <c r="C157">
-        <v>44632</v>
+        <v>1247</v>
+      </c>
+      <c r="C157" s="10">
+        <v>44677</v>
       </c>
       <c r="D157" s="4"/>
       <c r="E157" s="4"/>
@@ -3205,10 +3204,10 @@
     </row>
     <row r="158" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B158" s="4">
-        <v>1227</v>
-      </c>
-      <c r="C158">
-        <v>44630</v>
+        <v>1246</v>
+      </c>
+      <c r="C158" s="10">
+        <v>44674</v>
       </c>
       <c r="D158" s="4"/>
       <c r="E158" s="4"/>
@@ -3218,10 +3217,10 @@
     </row>
     <row r="159" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B159" s="4">
-        <v>1226</v>
-      </c>
-      <c r="C159">
-        <v>44628</v>
+        <v>1245</v>
+      </c>
+      <c r="C159" s="10">
+        <v>44672</v>
       </c>
       <c r="D159" s="4"/>
       <c r="E159" s="4"/>
@@ -3231,10 +3230,10 @@
     </row>
     <row r="160" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B160" s="4">
-        <v>1225</v>
-      </c>
-      <c r="C160">
-        <v>44625</v>
+        <v>1244</v>
+      </c>
+      <c r="C160" s="10">
+        <v>44670</v>
       </c>
       <c r="D160" s="4"/>
       <c r="E160" s="4"/>
@@ -3244,10 +3243,10 @@
     </row>
     <row r="161" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B161" s="4">
-        <v>1224</v>
-      </c>
-      <c r="C161">
-        <v>44623</v>
+        <v>1243</v>
+      </c>
+      <c r="C161" s="10">
+        <v>44667</v>
       </c>
       <c r="D161" s="4"/>
       <c r="E161" s="4"/>
@@ -3257,10 +3256,10 @@
     </row>
     <row r="162" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B162" s="4">
-        <v>1223</v>
-      </c>
-      <c r="C162">
-        <v>44621</v>
+        <v>1242</v>
+      </c>
+      <c r="C162" s="10">
+        <v>44665</v>
       </c>
       <c r="D162" s="4"/>
       <c r="E162" s="4"/>
@@ -3270,10 +3269,10 @@
     </row>
     <row r="163" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B163" s="4">
-        <v>1222</v>
-      </c>
-      <c r="C163">
-        <v>44618</v>
+        <v>1241</v>
+      </c>
+      <c r="C163" s="10">
+        <v>44663</v>
       </c>
       <c r="D163" s="4"/>
       <c r="E163" s="4"/>
@@ -3283,10 +3282,10 @@
     </row>
     <row r="164" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B164" s="4">
-        <v>1221</v>
-      </c>
-      <c r="C164">
-        <v>44616</v>
+        <v>1240</v>
+      </c>
+      <c r="C164" s="10">
+        <v>44660</v>
       </c>
       <c r="D164" s="4"/>
       <c r="E164" s="4"/>
@@ -3296,10 +3295,10 @@
     </row>
     <row r="165" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B165" s="4">
-        <v>1220</v>
-      </c>
-      <c r="C165">
-        <v>44614</v>
+        <v>1239</v>
+      </c>
+      <c r="C165" s="10">
+        <v>44658</v>
       </c>
       <c r="D165" s="4"/>
       <c r="E165" s="4"/>
@@ -3309,10 +3308,10 @@
     </row>
     <row r="166" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B166" s="4">
-        <v>1219</v>
-      </c>
-      <c r="C166">
-        <v>44611</v>
+        <v>1238</v>
+      </c>
+      <c r="C166" s="10">
+        <v>44656</v>
       </c>
       <c r="D166" s="4"/>
       <c r="E166" s="4"/>
@@ -3322,10 +3321,10 @@
     </row>
     <row r="167" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B167" s="4">
-        <v>1218</v>
-      </c>
-      <c r="C167">
-        <v>44609</v>
+        <v>1237</v>
+      </c>
+      <c r="C167" s="10">
+        <v>44653</v>
       </c>
       <c r="D167" s="4"/>
       <c r="E167" s="4"/>
@@ -3335,10 +3334,10 @@
     </row>
     <row r="168" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B168" s="4">
-        <v>1217</v>
-      </c>
-      <c r="C168">
-        <v>44607</v>
+        <v>1236</v>
+      </c>
+      <c r="C168" s="10">
+        <v>44651</v>
       </c>
       <c r="D168" s="4"/>
       <c r="E168" s="4"/>
@@ -3348,10 +3347,10 @@
     </row>
     <row r="169" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B169" s="4">
-        <v>1216</v>
-      </c>
-      <c r="C169">
-        <v>44604</v>
+        <v>1235</v>
+      </c>
+      <c r="C169" s="10">
+        <v>44649</v>
       </c>
       <c r="D169" s="4"/>
       <c r="E169" s="4"/>
@@ -3361,10 +3360,10 @@
     </row>
     <row r="170" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B170" s="4">
-        <v>1215</v>
-      </c>
-      <c r="C170">
-        <v>44602</v>
+        <v>1234</v>
+      </c>
+      <c r="C170" s="10">
+        <v>44646</v>
       </c>
       <c r="D170" s="4"/>
       <c r="E170" s="4"/>
@@ -3374,10 +3373,10 @@
     </row>
     <row r="171" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B171" s="4">
-        <v>1214</v>
-      </c>
-      <c r="C171">
-        <v>44600</v>
+        <v>1233</v>
+      </c>
+      <c r="C171" s="10">
+        <v>44644</v>
       </c>
       <c r="D171" s="4"/>
       <c r="E171" s="4"/>
@@ -3387,10 +3386,10 @@
     </row>
     <row r="172" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B172" s="4">
-        <v>1213</v>
-      </c>
-      <c r="C172">
-        <v>44597</v>
+        <v>1232</v>
+      </c>
+      <c r="C172" s="10">
+        <v>44642</v>
       </c>
       <c r="D172" s="4"/>
       <c r="E172" s="4"/>
@@ -3400,10 +3399,10 @@
     </row>
     <row r="173" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B173" s="4">
-        <v>1212</v>
-      </c>
-      <c r="C173">
-        <v>44595</v>
+        <v>1231</v>
+      </c>
+      <c r="C173" s="10">
+        <v>44639</v>
       </c>
       <c r="D173" s="4"/>
       <c r="E173" s="4"/>
@@ -3413,10 +3412,10 @@
     </row>
     <row r="174" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B174" s="4">
-        <v>1211</v>
-      </c>
-      <c r="C174">
-        <v>44593</v>
+        <v>1230</v>
+      </c>
+      <c r="C174" s="10">
+        <v>44637</v>
       </c>
       <c r="D174" s="4"/>
       <c r="E174" s="4"/>
@@ -3424,6 +3423,253 @@
       <c r="G174" s="4"/>
       <c r="H174" s="4"/>
     </row>
+    <row r="175" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B175" s="4">
+        <v>1229</v>
+      </c>
+      <c r="C175" s="10">
+        <v>44635</v>
+      </c>
+      <c r="D175" s="4"/>
+      <c r="E175" s="4"/>
+      <c r="F175" s="4"/>
+      <c r="G175" s="4"/>
+      <c r="H175" s="4"/>
+    </row>
+    <row r="176" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B176" s="4">
+        <v>1228</v>
+      </c>
+      <c r="C176">
+        <v>44632</v>
+      </c>
+      <c r="D176" s="4"/>
+      <c r="E176" s="4"/>
+      <c r="F176" s="4"/>
+      <c r="G176" s="4"/>
+      <c r="H176" s="4"/>
+    </row>
+    <row r="177" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B177" s="4">
+        <v>1227</v>
+      </c>
+      <c r="C177">
+        <v>44630</v>
+      </c>
+      <c r="D177" s="4"/>
+      <c r="E177" s="4"/>
+      <c r="F177" s="4"/>
+      <c r="G177" s="4"/>
+      <c r="H177" s="4"/>
+    </row>
+    <row r="178" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B178" s="4">
+        <v>1226</v>
+      </c>
+      <c r="C178">
+        <v>44628</v>
+      </c>
+      <c r="D178" s="4"/>
+      <c r="E178" s="4"/>
+      <c r="F178" s="4"/>
+      <c r="G178" s="4"/>
+      <c r="H178" s="4"/>
+    </row>
+    <row r="179" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B179" s="4">
+        <v>1225</v>
+      </c>
+      <c r="C179">
+        <v>44625</v>
+      </c>
+      <c r="D179" s="4"/>
+      <c r="E179" s="4"/>
+      <c r="F179" s="4"/>
+      <c r="G179" s="4"/>
+      <c r="H179" s="4"/>
+    </row>
+    <row r="180" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B180" s="4">
+        <v>1224</v>
+      </c>
+      <c r="C180">
+        <v>44623</v>
+      </c>
+      <c r="D180" s="4"/>
+      <c r="E180" s="4"/>
+      <c r="F180" s="4"/>
+      <c r="G180" s="4"/>
+      <c r="H180" s="4"/>
+    </row>
+    <row r="181" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B181" s="4">
+        <v>1223</v>
+      </c>
+      <c r="C181">
+        <v>44621</v>
+      </c>
+      <c r="D181" s="4"/>
+      <c r="E181" s="4"/>
+      <c r="F181" s="4"/>
+      <c r="G181" s="4"/>
+      <c r="H181" s="4"/>
+    </row>
+    <row r="182" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B182" s="4">
+        <v>1222</v>
+      </c>
+      <c r="C182">
+        <v>44618</v>
+      </c>
+      <c r="D182" s="4"/>
+      <c r="E182" s="4"/>
+      <c r="F182" s="4"/>
+      <c r="G182" s="4"/>
+      <c r="H182" s="4"/>
+    </row>
+    <row r="183" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B183" s="4">
+        <v>1221</v>
+      </c>
+      <c r="C183">
+        <v>44616</v>
+      </c>
+      <c r="D183" s="4"/>
+      <c r="E183" s="4"/>
+      <c r="F183" s="4"/>
+      <c r="G183" s="4"/>
+      <c r="H183" s="4"/>
+    </row>
+    <row r="184" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B184" s="4">
+        <v>1220</v>
+      </c>
+      <c r="C184">
+        <v>44614</v>
+      </c>
+      <c r="D184" s="4"/>
+      <c r="E184" s="4"/>
+      <c r="F184" s="4"/>
+      <c r="G184" s="4"/>
+      <c r="H184" s="4"/>
+    </row>
+    <row r="185" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B185" s="4">
+        <v>1219</v>
+      </c>
+      <c r="C185">
+        <v>44611</v>
+      </c>
+      <c r="D185" s="4"/>
+      <c r="E185" s="4"/>
+      <c r="F185" s="4"/>
+      <c r="G185" s="4"/>
+      <c r="H185" s="4"/>
+    </row>
+    <row r="186" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B186" s="4">
+        <v>1218</v>
+      </c>
+      <c r="C186">
+        <v>44609</v>
+      </c>
+      <c r="D186" s="4"/>
+      <c r="E186" s="4"/>
+      <c r="F186" s="4"/>
+      <c r="G186" s="4"/>
+      <c r="H186" s="4"/>
+    </row>
+    <row r="187" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B187" s="4">
+        <v>1217</v>
+      </c>
+      <c r="C187">
+        <v>44607</v>
+      </c>
+      <c r="D187" s="4"/>
+      <c r="E187" s="4"/>
+      <c r="F187" s="4"/>
+      <c r="G187" s="4"/>
+      <c r="H187" s="4"/>
+    </row>
+    <row r="188" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B188" s="4">
+        <v>1216</v>
+      </c>
+      <c r="C188">
+        <v>44604</v>
+      </c>
+      <c r="D188" s="4"/>
+      <c r="E188" s="4"/>
+      <c r="F188" s="4"/>
+      <c r="G188" s="4"/>
+      <c r="H188" s="4"/>
+    </row>
+    <row r="189" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B189" s="4">
+        <v>1215</v>
+      </c>
+      <c r="C189">
+        <v>44602</v>
+      </c>
+      <c r="D189" s="4"/>
+      <c r="E189" s="4"/>
+      <c r="F189" s="4"/>
+      <c r="G189" s="4"/>
+      <c r="H189" s="4"/>
+    </row>
+    <row r="190" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B190" s="4">
+        <v>1214</v>
+      </c>
+      <c r="C190">
+        <v>44600</v>
+      </c>
+      <c r="D190" s="4"/>
+      <c r="E190" s="4"/>
+      <c r="F190" s="4"/>
+      <c r="G190" s="4"/>
+      <c r="H190" s="4"/>
+    </row>
+    <row r="191" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B191" s="4">
+        <v>1213</v>
+      </c>
+      <c r="C191">
+        <v>44597</v>
+      </c>
+      <c r="D191" s="4"/>
+      <c r="E191" s="4"/>
+      <c r="F191" s="4"/>
+      <c r="G191" s="4"/>
+      <c r="H191" s="4"/>
+    </row>
+    <row r="192" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B192" s="4">
+        <v>1212</v>
+      </c>
+      <c r="C192">
+        <v>44595</v>
+      </c>
+      <c r="D192" s="4"/>
+      <c r="E192" s="4"/>
+      <c r="F192" s="4"/>
+      <c r="G192" s="4"/>
+      <c r="H192" s="4"/>
+    </row>
+    <row r="193" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B193" s="4">
+        <v>1211</v>
+      </c>
+      <c r="C193">
+        <v>44593</v>
+      </c>
+      <c r="D193" s="4"/>
+      <c r="E193" s="4"/>
+      <c r="F193" s="4"/>
+      <c r="G193" s="4"/>
+      <c r="H193" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Update 31-03-2023 -->> Excel
</commit_message>
<xml_diff>
--- a/helps/Historial de Jugadas.xlsx
+++ b/helps/Historial de Jugadas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos\Randon\helps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBEFBDB-82AD-4ADB-B08A-2D3E59995DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D89F627-E1D4-4F58-9159-FAEB4496462E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" activeTab="1" xr2:uid="{A3392D85-3030-46DE-B96E-7922EDC7109E}"/>
   </bookViews>
@@ -210,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -239,9 +239,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1193,7 +1190,7 @@
   <dimension ref="A1:H193"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.15625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -1242,30 +1239,30 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
@@ -1296,8 +1293,12 @@
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B11" s="4"/>
-      <c r="C11" s="10"/>
+      <c r="B11" s="4">
+        <v>1393</v>
+      </c>
+      <c r="C11" s="10">
+        <v>45017</v>
+      </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>

</xml_diff>